<commit_message>
modified parser and .csv files to address UTF-8 encoding in first few bytes
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16170" windowHeight="7965"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -777,9 +777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D140" sqref="D133:D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12983,8 +12983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O152"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20146,8 +20146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
yard_in / out formatting in CSV and some other stuff
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
     <sheet name="Red Line" sheetId="2" r:id="rId2"/>
-    <sheet name="greenline.csv" sheetId="3" r:id="rId3"/>
-    <sheet name="redline.csv" sheetId="4" r:id="rId4"/>
+    <sheet name="GreenLineFinal" sheetId="3" r:id="rId3"/>
+    <sheet name="RedLineFinal" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="107">
   <si>
     <t>Line</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>Beacon</t>
+  </si>
+  <si>
+    <t>YARD_IN</t>
+  </si>
+  <si>
+    <t>YARD_OUT</t>
   </si>
 </sst>
 </file>
@@ -778,8 +784,8 @@
   <dimension ref="A1:O154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D140" sqref="D133:D140"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O154" sqref="A3:O154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7946,7 +7952,7 @@
         <v>29</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="C153" s="2">
         <v>151</v>
@@ -7993,7 +7999,7 @@
         <v>29</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="C154" s="2">
         <v>152</v>
@@ -8047,7 +8053,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="O79" sqref="A3:O79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12983,8 +12989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41:G42"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20048,7 +20054,7 @@
         <v>29</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="C151" s="2">
         <v>151</v>
@@ -20095,7 +20101,7 @@
         <v>29</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="C152" s="2">
         <v>152</v>
@@ -20147,7 +20153,7 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection sqref="A1:O77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added setMaintenance() for CTC and more parsing
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -354,235 +354,235 @@
     <t>Coordinates</t>
   </si>
   <si>
-    <t>(217.163268,120.999802);(217.489804,120.999639);(217.816340,120.999825);(218.142876,121.000138);(218.469412,121.000353);(218.795948,121.000245);(219.122483,120.999665);(219.449018,120.998979);(219.775553,120.999149);(220.102082,121.001049);(220.428607,121.003620);(220.755130,121.003358);(221.081566,120.996619);(221.407945,120.986844);(221.734313,120.986911);(222.059724,121.009338);(222.384220,121.045126);(222.708896,121.053197);(223.015293,120.969982);(223.270264,120.777195);(223.479417,120.527395);(223.683912,120.273266);(223.926550,120.062199);(224.223953,119.953943);(224.547575,119.947778);(224.872058,119.982967);(225.197010,120.012211);(225.523227,120.018472);(225.849508,120.007638);(226.175627,119.991245);(226.501932,119.981470);(226.828104,119.989404);(227.153004,120.019611);(227.477617,120.053072);(227.800713,120.041076);(228.095504,119.925496);(228.335895,119.710877);(228.540845,119.457030);(228.751842,119.208833);(229.008274,119.017491);(229.314903,118.933133);(229.639076,118.942329);(229.961419,118.992986);(230.283297,119.047287);(230.607595,119.070342);(230.922266,119.013056);(231.193664,118.846480);(231.414349,118.607901);(231.618001,118.352770);(231.844958,118.121105);</t>
+    <t>217.163268_120.999802;217.489804_120.999639;217.816340_120.999825;218.142876_121.000138;218.469412_121.000353;218.795948_121.000245;219.122483_120.999665;219.449018_120.998979;219.775553_120.999149;220.102082_121.001049;220.428607_121.003620;220.755130_121.003358;221.081566_120.996619;221.407945_120.986844;221.734313_120.986911;222.059724_121.009338;222.384220_121.045126;222.708896_121.053197;223.015293_120.969982;223.270264_120.777195;223.479417_120.527395;223.683912_120.273266;223.926550_120.062199;224.223953_119.953943;224.547575_119.947778;224.872058_119.982967;225.197010_120.012211;225.523227_120.018472;225.849508_120.007638;226.175627_119.991245;226.501932_119.981470;226.828104_119.989404;227.153004_120.019611;227.477617_120.053072;227.800713_120.041076;228.095504_119.925496;228.335895_119.710877;228.540845_119.457030;228.751842_119.208833;229.008274_119.017491;229.314903_118.933133;229.639076_118.942329;229.961419_118.992986;230.283297_119.047287;230.607595_119.070342;230.922266_119.013056;231.193664_118.846480;231.414349_118.607901;231.618001_118.352770;231.844958_118.121105;</t>
   </si>
   <si>
-    <t>(232.443039,117.929303);(232.767068,117.960037);(233.088704,118.016048);(233.411424,118.063319);(233.735008,118.061550);(234.035173,117.958989);(234.282139,117.753626);(234.488760,117.501359);(234.696423,117.250059);(234.946296,117.049122);(235.248923,116.954891);(235.573361,116.956295);(235.898284,116.987775);(236.223969,117.003153);(236.550363,116.997350);(236.876612,116.997725);(237.201667,117.023956);(237.526368,117.055648);(237.847216,117.032134);(238.129907,116.893381);(238.352910,116.659259);(238.548588,116.397998);(238.766522,116.158182);(239.044031,116.012511);(239.363225,115.991522);(239.688265,116.017890);(240.001476,115.972245);(240.262786,115.796949);(240.466822,115.543716);(240.662061,115.282489);(240.901963,115.071978);(241.202336,114.985709);(241.526778,115.002849);(241.850203,115.009469);(242.142151,114.900605);(242.371200,114.675222);(242.563935,114.411883);(242.774818,114.165496);(243.047133,114.011783);(243.365172,113.986781);(243.690164,114.014001);(244.004148,113.971724);(244.267724,113.799991);(244.473972,113.548688);(244.669572,113.287635);(244.906944,113.072885);(245.204879,112.976070);(245.529250,112.984428);(245.854140,112.999625);(246.163312,112.927922);</t>
+    <t>232.443039_117.929303;232.767068_117.960037;233.088704_118.016048;233.411424_118.063319;233.735008_118.061550;234.035173_117.958989;234.282139_117.753626;234.488760_117.501359;234.696423_117.250059;234.946296_117.049122;235.248923_116.954891;235.573361_116.956295;235.898284_116.987775;236.223969_117.003153;236.550363_116.997350;236.876612_116.997725;237.201667_117.023956;237.526368_117.055648;237.847216_117.032134;238.129907_116.893381;238.352910_116.659259;238.548588_116.397998;238.766522_116.158182;239.044031_116.012511;239.363225_115.991522;239.688265_116.017890;240.001476_115.972245;240.262786_115.796949;240.466822_115.543716;240.662061_115.282489;240.901963_115.071978;241.202336_114.985709;241.526778_115.002849;241.850203_115.009469;242.142151_114.900605;242.371200_114.675222;242.563935_114.411883;242.774818_114.165496;243.047133_114.011783;243.365172_113.986781;243.690164_114.014001;244.004148_113.971724;244.267724_113.799991;244.473972_113.548688;244.669572_113.287635;244.906944_113.072885;245.204879_112.976070;245.529250_112.984428;245.854140_112.999625;246.163312_112.927922;</t>
   </si>
   <si>
-    <t>(246.640537,112.500456);(246.831860,112.235969);(247.025213,111.973036);(247.235802,111.723974);(247.464102,111.490808);(247.703088,111.268377);(247.944988,111.049045);(248.183526,110.826103);(248.416887,110.597731);(248.646411,110.365485);(248.873714,110.131054);(249.100380,109.896005);(249.327842,109.661728);(249.557365,109.429478);(249.790135,109.200493);(250.027112,108.975875);(250.267106,108.754457);(250.505532,108.531383);(250.736033,108.300280);(250.951276,108.055174);(251.144752,107.792698);(251.315475,107.514721);(251.467393,107.225876);(251.605508,106.930076);(251.734994,106.630335);(251.860998,106.329092);(251.988597,106.028531);(252.121537,105.730309);(252.260582,105.434879);(252.404696,105.141879);(252.552714,104.850827);(252.703466,104.561175);(252.855781,104.272341);(253.008501,103.983719);(253.160639,103.694791);(253.311505,103.405198);(253.460548,103.114663);(253.607213,102.822924);(253.750941,102.529728);(253.891160,102.234840);(254.027285,101.938044);(254.158720,101.639145);(254.284854,101.337975);(254.405067,101.034397);(254.518729,100.728310);(254.625203,100.419655);(254.723856,100.108417);(254.814062,99.794632);(254.895211,99.478389);(254.966724,99.159834);</t>
+    <t>246.640537_112.500456;246.831860_112.235969;247.025213_111.973036;247.235802_111.723974;247.464102_111.490808;247.703088_111.268377;247.944988_111.049045;248.183526_110.826103;248.416887_110.597731;248.646411_110.365485;248.873714_110.131054;249.100380_109.896005;249.327842_109.661728;249.557365_109.429478;249.790135_109.200493;250.027112_108.975875;250.267106_108.754457;250.505532_108.531383;250.736033_108.300280;250.951276_108.055174;251.144752_107.792698;251.315475_107.514721;251.467393_107.225876;251.605508_106.930076;251.734994_106.630335;251.860998_106.329092;251.988597_106.028531;252.121537_105.730309;252.260582_105.434879;252.404696_105.141879;252.552714_104.850827;252.703466_104.561175;252.855781_104.272341;253.008501_103.983719;253.160639_103.694791;253.311505_103.405198;253.460548_103.114663;253.607213_102.822924;253.750941_102.529728;253.891160_102.234840;254.027285_101.938044;254.158720_101.639145;254.284854_101.337975;254.405067_101.034397;254.518729_100.728310;254.625203_100.419655;254.723856_100.108417;254.814062_99.794632;254.895211_99.478389;254.966724_99.159834;</t>
   </si>
   <si>
-    <t>(254.903319,98.875801);(254.711809,98.625985);(254.524217,98.373216);(254.341015,98.117251);(254.162763,97.857820);(253.990132,97.594622);(253.823933,97.327325);(253.665154,97.055568);(253.515008,96.778962);(253.375006,96.497109);(253.247030,96.209628);(253.133443,95.916209);(253.037200,95.616716);(252.961951,95.311360);(252.912055,95.000974);(252.892383,94.687375);(252.907723,94.373700);(252.961703,94.064460);(253.055520,93.764937);(253.187224,93.479945);(253.352125,93.212592);(253.544114,92.963739);(253.757042,92.732321);(253.985538,92.516082);(254.225258,92.312229);(254.472796,92.117853);(254.725458,91.930133);(254.981047,91.746389);(255.237669,91.564079);(255.493564,91.380758);(255.746970,91.194033);(255.995985,91.001530);(256.238438,90.800884);(256.471765,90.589773);(256.692898,90.366020);(256.898219,90.127794);(257.084231,89.874276);(257.250440,89.607250);(257.399955,89.330404);(257.537036,89.047108);(257.666118,88.760026);(257.791639,88.471349);(257.918016,88.183049);(258.049307,87.896979);(258.187013,87.613936);(258.329590,87.333297);(258.474651,87.053927);(258.619808,86.774605);(258.762672,86.494112);(258.900857,86.211301);</t>
+    <t>254.903319_98.875801;254.711809_98.625985;254.524217_98.373216;254.341015_98.117251;254.162763_97.857820;253.990132_97.594622;253.823933_97.327325;253.665154_97.055568;253.515008_96.778962;253.375006_96.497109;253.247030_96.209628;253.133443_95.916209;253.037200_95.616716;252.961951_95.311360;252.912055_95.000974;252.892383_94.687375;252.907723_94.373700;252.961703_94.064460;253.055520_93.764937;253.187224_93.479945;253.352125_93.212592;253.544114_92.963739;253.757042_92.732321;253.985538_92.516082;254.225258_92.312229;254.472796_92.117853;254.725458_91.930133;254.981047_91.746389;255.237669_91.564079;255.493564_91.380758;255.746970_91.194033;255.995985_91.001530;256.238438_90.800884;256.471765_90.589773;256.692898_90.366020;256.898219_90.127794;257.084231_89.874276;257.250440_89.607250;257.399955_89.330404;257.537036_89.047108;257.666118_88.760026;257.791639_88.471349;257.918016_88.183049;258.049307_87.896979;258.187013_87.613936;258.329590_87.333297;258.474651_87.053927;258.619808_86.774605;258.762672_86.494112;258.900857_86.211301;</t>
   </si>
   <si>
-    <t>(259.157334,85.636435);(259.279916,85.346495);(259.404976,85.057633);(259.537519,84.772182);(259.682588,84.492987);(259.845098,84.223725);(260.029151,83.968882);(260.234468,83.730722);(260.455235,83.506526);(260.684389,83.290750);(260.915813,83.077365);(261.144630,82.861217);(261.369241,82.640691);(261.590869,82.417152);(261.811240,82.192367);(262.032066,81.968031);(262.254236,81.745028);(262.477343,81.522959);(262.700453,81.300892);(262.922630,81.077894);(263.143309,80.853415);(263.363233,80.628194);(263.584239,80.404040);(263.808327,80.182985);(264.037299,79.967020);(264.270112,79.755160);(264.501337,79.541606);(264.723852,79.319170);(264.930946,79.082524);(265.120465,78.831466);(265.303024,78.575058);(265.499712,78.330100);(265.734842,78.126185);(266.019317,78.014115);(266.330051,78.003451);(266.643588,78.028081);(266.949383,77.993627);(267.210996,77.840383);(267.415500,77.603680);(267.601508,77.349884);(267.816455,77.124606);(268.090766,76.999709);(268.400716,76.991582);(268.713937,77.017422);(269.014920,76.968821);(269.265658,76.796692);(269.462174,76.552359);(269.648774,76.299191);(269.873986,76.087188);(270.158442,75.988196);</t>
+    <t>259.157334_85.636435;259.279916_85.346495;259.404976_85.057633;259.537519_84.772182;259.682588_84.492987;259.845098_84.223725;260.029151_83.968882;260.234468_83.730722;260.455235_83.506526;260.684389_83.290750;260.915813_83.077365;261.144630_82.861217;261.369241_82.640691;261.590869_82.417152;261.811240_82.192367;262.032066_81.968031;262.254236_81.745028;262.477343_81.522959;262.700453_81.300892;262.922630_81.077894;263.143309_80.853415;263.363233_80.628194;263.584239_80.404040;263.808327_80.182985;264.037299_79.967020;264.270112_79.755160;264.501337_79.541606;264.723852_79.319170;264.930946_79.082524;265.120465_78.831466;265.303024_78.575058;265.499712_78.330100;265.734842_78.126185;266.019317_78.014115;266.330051_78.003451;266.643588_78.028081;266.949383_77.993627;267.210996_77.840383;267.415500_77.603680;267.601508_77.349884;267.816455_77.124606;268.090766_76.999709;268.400716_76.991582;268.713937_77.017422;269.014920_76.968821;269.265658_76.796692;269.462174_76.552359;269.648774_76.299191;269.873986_76.087188;270.158442_75.988196;</t>
   </si>
   <si>
-    <t>(270.783493,76.015892);(271.076651,75.941381);(271.314039,75.746825);(271.504634,75.497060);(271.695569,75.247595);(271.933832,75.054364);(272.227562,74.980631);(272.540617,74.998911);(272.852958,75.007530);(273.140649,74.913691);(273.373258,74.709611);(273.566362,74.461507);(273.762070,74.215724);(274.001463,74.020996);(274.293310,73.929999);(274.605494,73.934732);(274.916099,73.983965);(275.225744,74.040308);(275.537913,74.072980);(275.846289,74.040299);(276.120590,73.904163);(276.343336,73.685525);(276.538895,73.439023);(276.744622,73.201965);(276.995406,73.022813);(277.292885,72.946896);(277.606037,72.954566);(277.918890,72.988832);(278.232527,73.011945);(278.547137,73.013918);(278.861782,73.004973);(279.176457,72.997442);(279.491226,72.996064);(279.806005,72.998225);(280.120784,73.000444);(280.435570,73.001088);(280.750358,73.000605);(281.065146,72.999961);(281.379934,72.999709);(281.694722,72.999805);(282.009511,72.999986);(282.324299,73.000076);(282.639087,73.000062);(282.953876,73.000011);(283.268664,72.999978);(283.583452,72.999976);(283.898241,72.999993);(284.213029,73.000014);(284.527817,73.000026);(284.842606,73.000014);</t>
+    <t>270.783493_76.015892;271.076651_75.941381;271.314039_75.746825;271.504634_75.497060;271.695569_75.247595;271.933832_75.054364;272.227562_74.980631;272.540617_74.998911;272.852958_75.007530;273.140649_74.913691;273.373258_74.709611;273.566362_74.461507;273.762070_74.215724;274.001463_74.020996;274.293310_73.929999;274.605494_73.934732;274.916099_73.983965;275.225744_74.040308;275.537913_74.072980;275.846289_74.040299;276.120590_73.904163;276.343336_73.685525;276.538895_73.439023;276.744622_73.201965;276.995406_73.022813;277.292885_72.946896;277.606037_72.954566;277.918890_72.988832;278.232527_73.011945;278.547137_73.013918;278.861782_73.004973;279.176457_72.997442;279.491226_72.996064;279.806005_72.998225;280.120784_73.000444;280.435570_73.001088;280.750358_73.000605;281.065146_72.999961;281.379934_72.999709;281.694722_72.999805;282.009511_72.999986;282.324299_73.000076;282.639087_73.000062;282.953876_73.000011;283.268664_72.999978;283.583452_72.999976;283.898241_72.999993;284.213029_73.000014;284.527817_73.000026;284.842606_73.000014;</t>
   </si>
   <si>
-    <t>(285.131662,73.000000);(285.394986,72.999999);(285.658310,73.000000);(285.921634,73.000000);(286.184958,73.000000);(286.448282,73.000000);(286.711606,73.000000);(286.974930,73.000000);(287.238254,72.999999);(287.501578,72.999998);(287.764902,72.999999);(288.028226,73.000001);(288.291550,73.000004);(288.554874,73.000006);(288.818198,73.000004);(289.081522,72.999996);(289.344846,72.999984);(289.608171,72.999978);(289.871495,72.999989);(290.134819,73.000024);(290.398143,73.000067);(290.661467,73.000080);(290.924791,73.000021);(291.188115,72.999876);(291.451439,72.999726);(291.714763,72.999720);(291.978086,73.000012);(292.241410,73.000591);(292.504733,73.001089);(292.768057,73.000931);(293.031376,72.999585);(293.294690,72.997338);(293.558007,72.995788);(293.821318,72.997129);(294.084556,73.003155);(294.347737,73.011728);(294.610979,73.015827);(294.874010,73.007586);(295.136060,72.983362);(295.397618,72.953238);(295.659952,72.941354);(295.916432,72.982117);(296.144732,73.101669);(296.333547,73.282569);(296.498461,73.487599);(296.661474,73.694259);(296.844431,73.881770);(297.065568,74.015418);(297.318505,74.071399);(297.580478,74.065830);(297.840942,74.028845);(298.100006,73.981733);(298.360037,73.941216);(298.622036,73.926548);(298.879133,73.965446);(299.110009,74.080756);(299.302338,74.257685);(299.469553,74.460777);(299.632866,74.667251);(299.813206,74.857713);(300.029599,75.000032);(300.279534,75.066894);(300.541297,75.068713);(300.802154,75.035288);(301.061287,74.988626);(301.320965,74.945582);(301.582737,74.924966);(301.841518,74.954009);(302.076649,75.059544);(302.272357,75.231896);(302.439808,75.434669);(302.601260,75.642622);(302.778608,75.835971);(302.992491,75.981657);(303.241681,76.049028);</t>
+    <t>285.131662_73.000000;285.394986_72.999999;285.658310_73.000000;285.921634_73.000000;286.184958_73.000000;286.448282_73.000000;286.711606_73.000000;286.974930_73.000000;287.238254_72.999999;287.501578_72.999998;287.764902_72.999999;288.028226_73.000001;288.291550_73.000004;288.554874_73.000006;288.818198_73.000004;289.081522_72.999996;289.344846_72.999984;289.608171_72.999978;289.871495_72.999989;290.134819_73.000024;290.398143_73.000067;290.661467_73.000080;290.924791_73.000021;291.188115_72.999876;291.451439_72.999726;291.714763_72.999720;291.978086_73.000012;292.241410_73.000591;292.504733_73.001089;292.768057_73.000931;293.031376_72.999585;293.294690_72.997338;293.558007_72.995788;293.821318_72.997129;294.084556_73.003155;294.347737_73.011728;294.610979_73.015827;294.874010_73.007586;295.136060_72.983362;295.397618_72.953238;295.659952_72.941354;295.916432_72.982117;296.144732_73.101669;296.333547_73.282569;296.498461_73.487599;296.661474_73.694259;296.844431_73.881770;297.065568_74.015418;297.318505_74.071399;297.580478_74.065830;297.840942_74.028845;298.100006_73.981733;298.360037_73.941216;298.622036_73.926548;298.879133_73.965446;299.110009_74.080756;299.302338_74.257685;299.469553_74.460777;299.632866_74.667251;299.813206_74.857713;300.029599_75.000032;300.279534_75.066894;300.541297_75.068713;300.802154_75.035288;301.061287_74.988626;301.320965_74.945582;301.582737_74.924966;301.841518_74.954009;302.076649_75.059544;302.272357_75.231896;302.439808_75.434669;302.601260_75.642622;302.778608_75.835971;302.992491_75.981657;303.241681_76.049028;</t>
   </si>
   <si>
-    <t>(303.765601,76.024987);(304.027699,76.001309);(304.290697,75.995178);(304.553916,76.001579);(304.817125,76.004610);(305.079790,75.990720);(305.341624,75.963193);(305.603903,75.944562);(305.863461,75.968661);(306.100267,76.069406);(306.297433,76.239850);(306.465535,76.442037);(306.626822,76.650128);(306.803166,76.844486);(307.015339,76.993194);(307.263171,77.066026);(307.524707,77.070788);(307.785643,77.038288);(308.044800,76.991775);(308.304431,76.948390);(308.566156,76.926236);(308.825699,76.951045);(309.063979,77.049941);(309.264253,77.216644);(309.435077,77.416467);(309.597538,77.623662);(309.772412,77.819638);(309.980210,77.975610);(310.224422,78.059475);(310.485336,78.072831);(310.746648,78.044673);(311.005881,77.998761);(311.265053,77.952477);(311.526298,77.924073);(311.786745,77.939786);(312.027641,78.030685);(312.228623,78.195301);(312.396547,78.397427);(312.555052,78.607656);(312.727540,78.805507);(312.936989,78.957205);(313.184626,79.025157);(313.446591,79.022426);(313.708886,79.000171);(313.970153,79.006596);(314.217210,79.082256);(314.431869,79.229324);(314.612020,79.419793);(314.767808,79.631660);(314.910054,79.853172);(315.047698,80.077652);(315.188565,80.300073);(315.340667,80.514734);(315.513493,80.712365);(315.717217,80.875757);(315.954976,80.978562);(316.213427,81.009841);(316.476095,80.997122);(316.738765,80.983223);(316.997589,81.011573);(317.235206,81.113363);(317.437939,81.277997);(317.611668,81.475092);(317.769818,81.685521);(317.924942,81.898282);(318.087651,82.105130);(318.262440,82.301864);(318.447388,82.489179);(318.638936,82.669823);(318.833317,82.847458);(319.026817,83.026041);(319.217184,83.207950);(319.404470,83.393042);(319.589674,83.580225);(319.773803,83.768468);</t>
+    <t>303.765601_76.024987;304.027699_76.001309;304.290697_75.995178;304.553916_76.001579;304.817125_76.004610;305.079790_75.990720;305.341624_75.963193;305.603903_75.944562;305.863461_75.968661;306.100267_76.069406;306.297433_76.239850;306.465535_76.442037;306.626822_76.650128;306.803166_76.844486;307.015339_76.993194;307.263171_77.066026;307.524707_77.070788;307.785643_77.038288;308.044800_76.991775;308.304431_76.948390;308.566156_76.926236;308.825699_76.951045;309.063979_77.049941;309.264253_77.216644;309.435077_77.416467;309.597538_77.623662;309.772412_77.819638;309.980210_77.975610;310.224422_78.059475;310.485336_78.072831;310.746648_78.044673;311.005881_77.998761;311.265053_77.952477;311.526298_77.924073;311.786745_77.939786;312.027641_78.030685;312.228623_78.195301;312.396547_78.397427;312.555052_78.607656;312.727540_78.805507;312.936989_78.957205;313.184626_79.025157;313.446591_79.022426;313.708886_79.000171;313.970153_79.006596;314.217210_79.082256;314.431869_79.229324;314.612020_79.419793;314.767808_79.631660;314.910054_79.853172;315.047698_80.077652;315.188565_80.300073;315.340667_80.514734;315.513493_80.712365;315.717217_80.875757;315.954976_80.978562;316.213427_81.009841;316.476095_80.997122;316.738765_80.983223;316.997589_81.011573;317.235206_81.113363;317.437939_81.277997;317.611668_81.475092;317.769818_81.685521;317.924942_81.898282;318.087651_82.105130;318.262440_82.301864;318.447388_82.489179;318.638936_82.669823;318.833317_82.847458;319.026817_83.026041;319.217184_83.207950;319.404470_83.393042;319.589674_83.580225;319.773803_83.768468;</t>
   </si>
   <si>
-    <t>(320.142620,84.144407);(320.328277,84.331143);(320.514585,84.517231);(320.701257,84.702954);(320.888007,84.888600);(321.074572,85.074430);(321.260858,85.260541);(321.446958,85.446837);(321.633012,85.633178);(321.819163,85.819425);(322.005543,86.005440);(322.192181,86.191198);(322.378903,86.376870);(322.565440,86.562729);(322.751516,86.749049);(322.936851,86.936104);(323.121326,87.124009);(323.305385,87.312323);(323.489939,87.500148);(323.675953,87.686524);(323.864353,87.870479);(324.055836,88.051217);(324.249572,88.229555);(324.442827,88.408407);(324.632173,88.591341);(324.813816,88.781827);(324.983385,88.982992);(325.137448,89.196218);(325.275943,89.419961);(325.401297,89.651404);(325.516428,89.888159);(325.624382,90.128310);(325.728205,90.370296);(325.830904,90.612767);(325.935455,90.854436);(326.044545,91.094073);(326.159070,91.331166);(326.277897,91.566143);(326.399388,91.799763);(326.521905,92.032849);(326.643798,92.266259);(326.763385,92.500853);(326.878933,92.737450);(326.988656,92.976787);(327.091202,93.219277);(327.186288,93.464792);(327.274315,93.712932);(327.355759,93.963314);(327.431124,94.215599);(327.500926,94.469483);(327.565694,94.724702);(327.625959,94.981024);(327.682251,95.238252);(327.735097,95.496212);(327.785019,95.754756);(327.832531,96.013754);(327.878145,96.273096);(327.922365,96.532680);(327.965691,96.792415);(328.008620,97.052216);(328.051649,97.312000);(328.095274,97.571685);(328.139994,97.831183);(328.186310,98.090399);(328.234729,98.349230);(328.285764,98.607555);(328.339932,98.865240);(328.397758,99.122126);(328.459769,99.378030);(328.526497,99.632742);(328.598472,99.886017);(328.676218,100.137576);(328.760250,100.387100);(328.851059,100.634233);(328.949109,100.878577);</t>
+    <t>320.142620_84.144407;320.328277_84.331143;320.514585_84.517231;320.701257_84.702954;320.888007_84.888600;321.074572_85.074430;321.260858_85.260541;321.446958_85.446837;321.633012_85.633178;321.819163_85.819425;322.005543_86.005440;322.192181_86.191198;322.378903_86.376870;322.565440_86.562729;322.751516_86.749049;322.936851_86.936104;323.121326_87.124009;323.305385_87.312323;323.489939_87.500148;323.675953_87.686524;323.864353_87.870479;324.055836_88.051217;324.249572_88.229555;324.442827_88.408407;324.632173_88.591341;324.813816_88.781827;324.983385_88.982992;325.137448_89.196218;325.275943_89.419961;325.401297_89.651404;325.516428_89.888159;325.624382_90.128310;325.728205_90.370296;325.830904_90.612767;325.935455_90.854436;326.044545_91.094073;326.159070_91.331166;326.277897_91.566143;326.399388_91.799763;326.521905_92.032849;326.643798_92.266259;326.763385_92.500853;326.878933_92.737450;326.988656_92.976787;327.091202_93.219277;327.186288_93.464792;327.274315_93.712932;327.355759_93.963314;327.431124_94.215599;327.500926_94.469483;327.565694_94.724702;327.625959_94.981024;327.682251_95.238252;327.735097_95.496212;327.785019_95.754756;327.832531_96.013754;327.878145_96.273096;327.922365_96.532680;327.965691_96.792415;328.008620_97.052216;328.051649_97.312000;328.095274_97.571685;328.139994_97.831183;328.186310_98.090399;328.234729_98.349230;328.285764_98.607555;328.339932_98.865240;328.397758_99.122126;328.459769_99.378030;328.526497_99.632742;328.598472_99.886017;328.676218_100.137576;328.760250_100.387100;328.851059_100.634233;328.949109_100.878577;</t>
   </si>
   <si>
-    <t>(328.882559,101.083504);(328.655585,101.260647);(328.445001,101.457028);(328.251449,101.670280);(328.074575,101.897637);(327.913137,102.136281);(327.765234,102.383609);(327.628555,102.637366);(327.500586,102.895664);(327.378742,103.156932);(327.260442,103.419839);(327.143137,103.683195);(327.024318,103.945866);(326.902102,104.206967);(326.776236,104.466332);(326.647572,104.724325);(326.517053,104.981387);(326.385620,105.237985);(326.254231,105.494605);(326.123879,105.751752);(325.995581,106.009926);(325.869741,106.269308);(325.745546,106.529485);(325.621538,106.789752);(325.496265,107.049410);(325.368396,107.307794);(325.236803,107.564295);(325.100605,107.818374);(324.958840,108.069376);(324.807690,108.314721);(324.638961,108.547917);(324.441824,108.756440);(324.206330,108.916681);(323.935468,108.998304);(323.649205,109.005723);(323.361654,108.986432);(323.076042,108.998458);(322.810388,109.092163);(322.584846,109.266435);(322.394294,109.481794);(322.220204,109.711514);(322.044879,109.940243);(321.855010,110.156701);(321.649449,110.358597);(321.437147,110.553630);(321.228594,110.752531);(321.033922,110.964677);(320.856951,111.191934);(320.688086,111.425580);(320.509417,111.651350);(320.300874,111.847206);(320.048700,111.972380);(319.767159,112.003589);(319.480093,111.980813);(319.193603,111.974489);(318.927140,112.055629);(318.710284,112.236791);(318.534160,112.464313);(318.362870,112.695935);(318.160068,112.895904);(317.904842,113.004353);(317.620384,113.010932);(317.333614,112.983427);(317.051739,113.005235);(316.805854,113.134126);(316.612782,113.344977);(316.444489,113.578935);(316.263717,113.802129);(316.035387,113.964424);(315.761363,114.018479);(315.474643,113.997186);(315.188192,113.983231);(314.920177,114.056723);(314.701853,114.235102);(314.526130,114.462839);</t>
+    <t>328.882559_101.083504;328.655585_101.260647;328.445001_101.457028;328.251449_101.670280;328.074575_101.897637;327.913137_102.136281;327.765234_102.383609;327.628555_102.637366;327.500586_102.895664;327.378742_103.156932;327.260442_103.419839;327.143137_103.683195;327.024318_103.945866;326.902102_104.206967;326.776236_104.466332;326.647572_104.724325;326.517053_104.981387;326.385620_105.237985;326.254231_105.494605;326.123879_105.751752;325.995581_106.009926;325.869741_106.269308;325.745546_106.529485;325.621538_106.789752;325.496265_107.049410;325.368396_107.307794;325.236803_107.564295;325.100605_107.818374;324.958840_108.069376;324.807690_108.314721;324.638961_108.547917;324.441824_108.756440;324.206330_108.916681;323.935468_108.998304;323.649205_109.005723;323.361654_108.986432;323.076042_108.998458;322.810388_109.092163;322.584846_109.266435;322.394294_109.481794;322.220204_109.711514;322.044879_109.940243;321.855010_110.156701;321.649449_110.358597;321.437147_110.553630;321.228594_110.752531;321.033922_110.964677;320.856951_111.191934;320.688086_111.425580;320.509417_111.651350;320.300874_111.847206;320.048700_111.972380;319.767159_112.003589;319.480093_111.980813;319.193603_111.974489;318.927140_112.055629;318.710284_112.236791;318.534160_112.464313;318.362870_112.695935;318.160068_112.895904;317.904842_113.004353;317.620384_113.010932;317.333614_112.983427;317.051739_113.005235;316.805854_113.134126;316.612782_113.344977;316.444489_113.578935;316.263717_113.802129;316.035387_113.964424;315.761363_114.018479;315.474643_113.997186;315.188192_113.983231;314.920177_114.056723;314.701853_114.235102;314.526130_114.462839;</t>
   </si>
   <si>
-    <t>(314.526130,114.462839);(314.356246,114.695508);(314.154804,114.896771);(313.900105,115.005768);(313.615661,115.012087);(313.328911,114.984426);(313.047166,115.006678);(312.801495,115.136131);(312.608405,115.347025);(312.439848,115.580795);(312.258809,115.803782);(312.030447,115.966254);(311.756476,116.021634);(311.469657,116.002004);(311.183009,115.987361);(310.912026,116.054534);(310.686231,116.223700);(310.502794,116.445041);(310.330206,116.675873);(310.135999,116.886501);(309.894250,117.029702);(309.615329,117.077782);(309.328950,117.057733);(309.044974,117.008766);(308.761383,116.957205);(308.475428,116.926318);(308.191108,116.947918);(307.931575,117.056577);(307.716860,117.244057);(307.534021,117.466502);(307.354552,117.691929);(307.149873,117.891915);(306.899919,118.020845);(306.618371,118.059052);(306.331330,118.040500);(306.045001,118.007162);(305.757780,117.985041);(305.469665,117.981372);(305.181573,117.990792);(304.893656,118.005574);(304.605628,118.017306);(304.317463,118.017792);(304.029941,118.000304);(303.743575,117.967635);(303.456830,117.941231);(303.172060,117.960050);(302.912213,118.066478);(302.698276,118.254611);(302.516734,118.478118);(302.337995,118.704091);(302.132399,118.902728);(301.880517,119.027057);(301.598068,119.060150);(301.311126,119.038915);(301.024855,119.005151);(300.737578,118.983958);(300.449448,118.981415);(300.161378,118.991638);(299.873471,119.006633);(299.585430,119.017878);(299.297274,119.017264);(299.009842,118.998372);(298.723521,118.965188);(298.436698,118.940509);(298.152654,118.964351);(297.895639,119.077401);(297.684852,119.269633);(297.504463,119.494164);(297.324822,119.719352);(297.116261,119.914384);(296.861372,120.032210);(296.577944,120.059858);(296.291068,120.036558);(296.004771,120.003086);(295.717404,119.983213);</t>
+    <t>314.526130_114.462839;314.356246_114.695508;314.154804_114.896771;313.900105_115.005768;313.615661_115.012087;313.328911_114.984426;313.047166_115.006678;312.801495_115.136131;312.608405_115.347025;312.439848_115.580795;312.258809_115.803782;312.030447_115.966254;311.756476_116.021634;311.469657_116.002004;311.183009_115.987361;310.912026_116.054534;310.686231_116.223700;310.502794_116.445041;310.330206_116.675873;310.135999_116.886501;309.894250_117.029702;309.615329_117.077782;309.328950_117.057733;309.044974_117.008766;308.761383_116.957205;308.475428_116.926318;308.191108_116.947918;307.931575_117.056577;307.716860_117.244057;307.534021_117.466502;307.354552_117.691929;307.149873_117.891915;306.899919_118.020845;306.618371_118.059052;306.331330_118.040500;306.045001_118.007162;305.757780_117.985041;305.469665_117.981372;305.181573_117.990792;304.893656_118.005574;304.605628_118.017306;304.317463_118.017792;304.029941_118.000304;303.743575_117.967635;303.456830_117.941231;303.172060_117.960050;302.912213_118.066478;302.698276_118.254611;302.516734_118.478118;302.337995_118.704091;302.132399_118.902728;301.880517_119.027057;301.598068_119.060150;301.311126_119.038915;301.024855_119.005151;300.737578_118.983958;300.449448_118.981415;300.161378_118.991638;299.873471_119.006633;299.585430_119.017878;299.297274_119.017264;299.009842_118.998372;298.723521_118.965188;298.436698_118.940509;298.152654_118.964351;297.895639_119.077401;297.684852_119.269633;297.504463_119.494164;297.324822_119.719352;297.116261_119.914384;296.861372_120.032210;296.577944_120.059858;296.291068_120.036558;296.004771_120.003086;295.717404_119.983213;</t>
   </si>
   <si>
-    <t>(295.717404,119.983213);(295.429257,119.981797);(295.141204,119.992628);(294.853299,120.007649);(294.565242,120.018328);(294.277099,120.016610);(293.989758,119.996354);(293.703475,119.962751);(293.416583,119.939960);(293.133419,119.969096);(292.879413,120.088820);(292.671805,120.285004);(292.492537,120.510511);(292.311867,120.734787);(292.100084,120.925715);(291.842079,121.036374);(291.557744,121.058242);(291.270910,121.033163);(290.984448,121.001402);(290.696863,120.985279);(290.408671,120.986549);(290.120520,120.995567);(289.832327,121.002633);(289.544045,121.004186);(289.255753,121.002353);(288.967463,121.000009);(288.679166,120.998914);(288.390866,120.999074);(288.102567,120.999727);(287.814267,121.000206);(287.525967,121.000296);(287.237667,121.000157);(286.949366,120.999993);(286.661066,120.999925);(286.372766,120.999942);(286.084466,120.999985);(285.796165,121.000006);(285.507865,121.000000);(285.219565,120.999994);(284.931265,121.000013);(284.642964,121.000056);(284.354664,121.000076);(284.066364,121.000013);(283.778064,120.999853);(283.489763,120.999707);(283.201463,120.999779);(282.913163,121.000239);(282.624864,121.000897);(282.336564,121.001105);(282.048267,121.000091);(281.759977,120.997783);(281.471685,120.995849);(281.183401,120.997141);(280.895202,121.003940);(280.607054,121.013076);(280.318857,121.015047);(280.031212,120.999989);(279.744716,120.968662);(279.457943,120.942279);(279.173078,120.960311);(278.912945,121.065903);(278.698811,121.253722);(278.517330,121.477269);(278.338775,121.703389);(278.133345,121.902187);(277.881497,122.026455);(277.599022,122.059284);(277.312057,122.038093);(277.025682,122.005297);(276.738283,121.986159);(276.450114,121.985311);(276.161961,121.994021);(275.873794,122.002286);(275.585527,122.005219);(275.297236,122.003768);</t>
+    <t>295.717404_119.983213;295.429257_119.981797;295.141204_119.992628;294.853299_120.007649;294.565242_120.018328;294.277099_120.016610;293.989758_119.996354;293.703475_119.962751;293.416583_119.939960;293.133419_119.969096;292.879413_120.088820;292.671805_120.285004;292.492537_120.510511;292.311867_120.734787;292.100084_120.925715;291.842079_121.036374;291.557744_121.058242;291.270910_121.033163;290.984448_121.001402;290.696863_120.985279;290.408671_120.986549;290.120520_120.995567;289.832327_121.002633;289.544045_121.004186;289.255753_121.002353;288.967463_121.000009;288.679166_120.998914;288.390866_120.999074;288.102567_120.999727;287.814267_121.000206;287.525967_121.000296;287.237667_121.000157;286.949366_120.999993;286.661066_120.999925;286.372766_120.999942;286.084466_120.999985;285.796165_121.000006;285.507865_121.000000;285.219565_120.999994;284.931265_121.000013;284.642964_121.000056;284.354664_121.000076;284.066364_121.000013;283.778064_120.999853;283.489763_120.999707;283.201463_120.999779;282.913163_121.000239;282.624864_121.000897;282.336564_121.001105;282.048267_121.000091;281.759977_120.997783;281.471685_120.995849;281.183401_120.997141;280.895202_121.003940;280.607054_121.013076;280.318857_121.015047;280.031212_120.999989;279.744716_120.968662;279.457943_120.942279;279.173078_120.960311;278.912945_121.065903;278.698811_121.253722;278.517330_121.477269;278.338775_121.703389;278.133345_121.902187;277.881497_122.026455;277.599022_122.059284;277.312057_122.038093;277.025682_122.005297;276.738283_121.986159;276.450114_121.985311;276.161961_121.994021;275.873794_122.002286;275.585527_122.005219;275.297236_122.003768;</t>
   </si>
   <si>
-    <t>(273.848958,122.000000);(273.546875,122.000000);(273.244792,122.000000);(272.942708,122.000000);(272.640625,122.000000);(272.338542,122.000000);(272.036458,122.000000);(271.734375,122.000000);(271.432292,122.000000);(271.130208,122.000000);(270.828125,122.000000);(270.526042,122.000000);(270.223958,122.000000);(269.921875,122.000000);(269.619792,122.000000);(269.317708,122.000000);(269.015625,122.000000);(268.713542,122.000000);(268.411458,122.000000);(268.109375,122.000000);(267.807292,122.000000);(267.505208,122.000000);(267.203125,122.000000);(266.901042,122.000000);(266.598958,122.000000);(266.296875,122.000000);(265.994792,122.000000);(265.692708,122.000000);(265.390625,122.000000);(265.088542,122.000000);(264.786458,122.000000);(264.484375,122.000000);(264.182292,122.000000);(263.880208,122.000000);(263.578125,122.000000);(263.276042,122.000000);(262.973958,122.000000);(262.671875,122.000000);(262.369792,122.000000);(262.067708,122.000000);(261.765625,122.000000);(261.463542,122.000000);(261.161458,122.000000);(260.859375,122.000000);(260.557292,122.000000);(260.255208,122.000000);(259.953125,122.000000);(259.651042,122.000000);(259.348958,122.000000);(259.046875,122.000000);(258.744792,122.000000);(258.442708,122.000000);(258.140625,122.000000);(257.838542,122.000000);(257.536458,122.000000);(257.234375,122.000000);(256.932292,122.000000);(256.630208,122.000000);(256.328125,122.000000);(256.026042,122.000000);(255.723958,122.000000);(255.421875,122.000000);(255.119792,122.000000);(254.817708,122.000000);(254.515625,122.000000);(254.213542,122.000000);(253.911458,122.000000);(253.609375,122.000000);(253.307292,122.000000);(253.005208,122.000000);</t>
+    <t>273.848958_122.000000;273.546875_122.000000;273.244792_122.000000;272.942708_122.000000;272.640625_122.000000;272.338542_122.000000;272.036458_122.000000;271.734375_122.000000;271.432292_122.000000;271.130208_122.000000;270.828125_122.000000;270.526042_122.000000;270.223958_122.000000;269.921875_122.000000;269.619792_122.000000;269.317708_122.000000;269.015625_122.000000;268.713542_122.000000;268.411458_122.000000;268.109375_122.000000;267.807292_122.000000;267.505208_122.000000;267.203125_122.000000;266.901042_122.000000;266.598958_122.000000;266.296875_122.000000;265.994792_122.000000;265.692708_122.000000;265.390625_122.000000;265.088542_122.000000;264.786458_122.000000;264.484375_122.000000;264.182292_122.000000;263.880208_122.000000;263.578125_122.000000;263.276042_122.000000;262.973958_122.000000;262.671875_122.000000;262.369792_122.000000;262.067708_122.000000;261.765625_122.000000;261.463542_122.000000;261.161458_122.000000;260.859375_122.000000;260.557292_122.000000;260.255208_122.000000;259.953125_122.000000;259.651042_122.000000;259.348958_122.000000;259.046875_122.000000;258.744792_122.000000;258.442708_122.000000;258.140625_122.000000;257.838542_122.000000;257.536458_122.000000;257.234375_122.000000;256.932292_122.000000;256.630208_122.000000;256.328125_122.000000;256.026042_122.000000;255.723958_122.000000;255.421875_122.000000;255.119792_122.000000;254.817708_122.000000;254.515625_122.000000;254.213542_122.000000;253.911458_122.000000;253.609375_122.000000;253.307292_122.000000;253.005208_122.000000;</t>
   </si>
   <si>
-    <t>(253.005208,122.000000);(252.703125,122.000000);(252.401042,122.000000);(252.098958,122.000000);(251.796875,122.000000);(251.494792,122.000000);(251.192708,122.000000);(250.890625,122.000000);(250.588542,122.000000);(250.286458,122.000000);(249.984375,122.000000);(249.682292,122.000000);(249.380208,122.000000);(249.078125,122.000000);(248.776042,122.000000);(248.473958,122.000000);(248.171875,122.000000);(247.869792,122.000000);(247.567708,122.000000);(247.265625,122.000000);(246.963542,122.000000);(246.661458,122.000000);(246.359375,122.000000);(246.057292,122.000000);(245.755208,122.000000);(245.453125,122.000000);(245.151042,122.000000);(244.848958,122.000000);(244.546875,122.000000);(244.244792,122.000000);(243.942708,122.000000);(243.640625,122.000000);(243.338542,122.000000);(243.036458,122.000000);(242.734375,122.000000);(242.432292,122.000000);(242.130208,122.000000);(241.828125,122.000000);(241.526042,122.000000);(241.223958,122.000000);(240.921875,122.000000);(240.619792,122.000000);(240.317708,122.000000);(240.015625,122.000000);(239.713542,122.000000);(239.411458,122.000000);(239.109375,122.000000);(238.807292,122.000000);(238.505208,122.000000);(238.203125,122.000000);(237.901042,122.000000);(237.598958,122.000000);(237.296875,122.000000);(236.994792,122.000000);(236.692708,122.000000);(236.390625,122.000000);(236.088542,122.000000);(235.786458,122.000000);(235.484375,122.000000);(235.182292,122.000000);</t>
+    <t>253.005208_122.000000;252.703125_122.000000;252.401042_122.000000;252.098958_122.000000;251.796875_122.000000;251.494792_122.000000;251.192708_122.000000;250.890625_122.000000;250.588542_122.000000;250.286458_122.000000;249.984375_122.000000;249.682292_122.000000;249.380208_122.000000;249.078125_122.000000;248.776042_122.000000;248.473958_122.000000;248.171875_122.000000;247.869792_122.000000;247.567708_122.000000;247.265625_122.000000;246.963542_122.000000;246.661458_122.000000;246.359375_122.000000;246.057292_122.000000;245.755208_122.000000;245.453125_122.000000;245.151042_122.000000;244.848958_122.000000;244.546875_122.000000;244.244792_122.000000;243.942708_122.000000;243.640625_122.000000;243.338542_122.000000;243.036458_122.000000;242.734375_122.000000;242.432292_122.000000;242.130208_122.000000;241.828125_122.000000;241.526042_122.000000;241.223958_122.000000;240.921875_122.000000;240.619792_122.000000;240.317708_122.000000;240.015625_122.000000;239.713542_122.000000;239.411458_122.000000;239.109375_122.000000;238.807292_122.000000;238.505208_122.000000;238.203125_122.000000;237.901042_122.000000;237.598958_122.000000;237.296875_122.000000;236.994792_122.000000;236.692708_122.000000;236.390625_122.000000;236.088542_122.000000;235.786458_122.000000;235.484375_122.000000;235.182292_122.000000;</t>
   </si>
   <si>
-    <t>(235.182292,122.000000);(234.880208,122.000000);(234.578125,122.000000);(234.276042,122.000000);(233.973958,122.000000);(233.671875,122.000000);(233.369792,122.000000);(233.067708,122.000000);(232.765625,122.000000);(232.463542,122.000000);(232.161458,122.000000);(231.859375,122.000000);(231.557292,122.000000);(231.255208,122.000000);(230.953125,122.000000);(230.651042,122.000000);(230.348958,122.000000);(230.046875,122.000000);(229.744792,122.000000);(229.442708,122.000000);(229.140625,122.000000);(228.838542,122.000000);(228.536458,122.000000);(228.234375,122.000000);(227.932292,122.000000);(227.630208,122.000000);(227.328125,122.000000);(227.026042,122.000000);(226.723958,122.000000);(226.421875,122.000000);(226.119792,122.000000);(225.817708,122.000000);(225.515625,122.000000);(225.213542,122.000000);(224.911458,122.000000);(224.609375,122.000000);(224.307292,122.000000);(224.005208,122.000000);(223.703125,122.000000);(223.401042,122.000000);(223.098958,122.000000);(222.796875,122.000000);(222.494792,122.000000);(222.192708,122.000000);(221.890625,122.000000);(221.588542,122.000000);(221.286458,122.000000);(220.984375,122.000000);(220.682292,122.000000);(220.380208,122.000000);(220.078125,122.000000);(219.776042,122.000000);(219.473958,122.000000);(219.171875,122.000000);(218.869792,122.000000);(218.567708,122.000000);(218.265625,122.000000);(217.963542,122.000000);(217.661458,122.000000);(217.359375,122.000000);</t>
+    <t>235.182292_122.000000;234.880208_122.000000;234.578125_122.000000;234.276042_122.000000;233.973958_122.000000;233.671875_122.000000;233.369792_122.000000;233.067708_122.000000;232.765625_122.000000;232.463542_122.000000;232.161458_122.000000;231.859375_122.000000;231.557292_122.000000;231.255208_122.000000;230.953125_122.000000;230.651042_122.000000;230.348958_122.000000;230.046875_122.000000;229.744792_122.000000;229.442708_122.000000;229.140625_122.000000;228.838542_122.000000;228.536458_122.000000;228.234375_122.000000;227.932292_122.000000;227.630208_122.000000;227.328125_122.000000;227.026042_122.000000;226.723958_122.000000;226.421875_122.000000;226.119792_122.000000;225.817708_122.000000;225.515625_122.000000;225.213542_122.000000;224.911458_122.000000;224.609375_122.000000;224.307292_122.000000;224.005208_122.000000;223.703125_122.000000;223.401042_122.000000;223.098958_122.000000;222.796875_122.000000;222.494792_122.000000;222.192708_122.000000;221.890625_122.000000;221.588542_122.000000;221.286458_122.000000;220.984375_122.000000;220.682292_122.000000;220.380208_122.000000;220.078125_122.000000;219.776042_122.000000;219.473958_122.000000;219.171875_122.000000;218.869792_122.000000;218.567708_122.000000;218.265625_122.000000;217.963542_122.000000;217.661458_122.000000;217.359375_122.000000;</t>
   </si>
   <si>
-    <t>(215.988038,122.000000);(215.964115,122.000000);(215.940191,122.000000);(215.916268,122.000000);(215.892344,122.000000);(215.868421,122.000000);(215.844498,122.000000);(215.820574,122.000000);(215.796651,122.000000);(215.772727,122.000000);(215.748804,122.000000);(215.724880,122.000000);(215.700957,122.000000);(215.677033,122.000000);(215.653110,122.000000);(215.629187,122.000000);(215.605263,122.000000);(215.581340,122.000000);(215.557416,122.000000);(215.533493,122.000000);(215.509569,122.000000);(215.485646,122.000000);(215.461722,122.000000);(215.437799,122.000000);(215.413876,122.000000);(215.389952,122.000000);(215.366029,122.000000);(215.342105,122.000000);(215.318182,122.000000);(215.294258,122.000000);(215.270335,122.000000);(215.246411,122.000000);(215.222488,122.000000);(215.198565,122.000000);(215.174641,122.000000);(215.150718,122.000000);(215.126794,122.000000);(215.102871,122.000000);(215.078947,122.000000);(215.055024,122.000000);(215.031100,122.000000);(215.007177,122.000000);(214.983254,122.000000);(214.959330,122.000000);(214.935407,122.000000);(214.911483,122.000000);(214.887560,122.000000);(214.863636,122.000000);(214.839713,122.000000);(214.815789,122.000000);</t>
+    <t>215.988038_122.000000;215.964115_122.000000;215.940191_122.000000;215.916268_122.000000;215.892344_122.000000;215.868421_122.000000;215.844498_122.000000;215.820574_122.000000;215.796651_122.000000;215.772727_122.000000;215.748804_122.000000;215.724880_122.000000;215.700957_122.000000;215.677033_122.000000;215.653110_122.000000;215.629187_122.000000;215.605263_122.000000;215.581340_122.000000;215.557416_122.000000;215.533493_122.000000;215.509569_122.000000;215.485646_122.000000;215.461722_122.000000;215.437799_122.000000;215.413876_122.000000;215.389952_122.000000;215.366029_122.000000;215.342105_122.000000;215.318182_122.000000;215.294258_122.000000;215.270335_122.000000;215.246411_122.000000;215.222488_122.000000;215.198565_122.000000;215.174641_122.000000;215.150718_122.000000;215.126794_122.000000;215.102871_122.000000;215.078947_122.000000;215.055024_122.000000;215.031100_122.000000;215.007177_122.000000;214.983254_122.000000;214.959330_122.000000;214.935407_122.000000;214.911483_122.000000;214.887560_122.000000;214.863636_122.000000;214.839713_122.000000;214.815789_122.000000;</t>
   </si>
   <si>
-    <t>(214.815789,122.000000);(214.791866,122.000000);(214.767943,122.000000);(214.744019,122.000000);(214.720096,122.000000);(214.696172,122.000000);(214.672249,122.000000);(214.648325,122.000000);(214.624402,122.000000);(214.600478,122.000000);(214.576555,122.000000);(214.552632,122.000000);(214.528708,122.000000);(214.504785,122.000000);(214.480861,122.000000);(214.456938,122.000000);(214.433014,122.000000);(214.409091,122.000000);(214.385167,122.000000);(214.361244,122.000000);(214.337321,122.000000);(214.313397,122.000000);(214.289474,122.000000);(214.265550,122.000000);(214.241627,122.000000);(214.217703,122.000000);(214.193780,122.000000);(214.169856,122.000000);(214.145933,122.000000);(214.122010,122.000000);(214.098086,122.000000);(214.074163,122.000000);(214.050239,122.000000);(214.026316,122.000000);(214.002392,122.000000);(213.978469,122.000000);(213.954545,122.000000);(213.930622,122.000000);(213.906699,122.000000);(213.882775,122.000000);(213.858852,122.000000);(213.834928,122.000000);(213.811005,122.000000);(213.787081,122.000000);(213.763158,122.000000);(213.739234,122.000000);(213.715311,122.000000);(213.691388,122.000000);(213.667464,122.000000);(213.643541,122.000000);(213.619617,122.000000);(213.595694,122.000000);(213.571770,122.000000);(213.547847,122.000000);(213.523923,122.000000);(213.500000,122.000000);(213.476077,122.000000);(213.452153,122.000000);(213.428230,122.000000);(213.404306,122.000000);(213.380383,122.000000);(213.356459,122.000000);(213.332536,122.000000);(213.308612,122.000000);(213.284689,122.000000);(213.260766,122.000000);(213.236842,122.000000);(213.212919,122.000000);(213.188995,122.000000);(213.165072,122.000000);(213.141148,122.000000);(213.117225,122.000000);(213.093301,122.000000);(213.069378,122.000000);(213.045455,122.000000);(213.021531,122.000000);(212.997608,122.000000);(212.973684,122.000000);(212.949761,122.000000);(212.925837,122.000000);(212.901914,122.000000);(212.877990,122.000000);(212.854067,122.000000);(212.830144,122.000000);(212.806220,122.000000);(212.782297,122.000000);(212.758373,122.000000);(212.734450,122.000000);(212.710526,122.000000);(212.686603,122.000000);(212.662679,122.000000);(212.638756,122.000000);(212.614833,122.000000);(212.590909,122.000000);(212.566986,122.000000);(212.543062,122.000000);(212.519139,122.000000);(212.495215,122.000000);(212.471292,122.000000);(212.447368,122.000000);(212.423445,122.000000);(212.399522,122.000000);(212.375598,122.000000);(212.351675,122.000000);(212.327751,122.000000);(212.303828,122.000000);(212.279904,122.000000);(212.255981,122.000000);(212.232057,122.000000);(212.208134,122.000000);(212.184211,122.000000);(212.160287,122.000000);(212.136364,122.000000);(212.112440,122.000000);(212.088517,122.000000);(212.064593,122.000000);(212.040670,122.000000);(212.016746,122.000000);(211.992823,122.000000);(211.968900,122.000000);(211.944976,122.000000);(211.921053,122.000000);(211.897129,122.000000);(211.873206,122.000000);(211.849282,122.000000);(211.825359,122.000000);(211.801435,122.000000);(211.777512,122.000000);(211.753589,122.000000);(211.729665,122.000000);(211.705742,122.000000);(211.681818,122.000000);(211.657895,122.000000);(211.633971,122.000000);(211.610048,122.000000);(211.586124,122.000000);(211.562201,122.000000);(211.538278,122.000000);(211.514354,122.000000);(211.490431,122.000000);(211.466507,122.000000);(211.442584,122.000000);(211.418660,122.000000);(211.394737,122.000000);(211.370813,122.000000);(211.346890,122.000000);(211.322967,122.000000);(211.299043,122.000000);(211.275120,122.000000);(211.251196,122.000000);(211.227273,122.000000);(211.203349,122.000000);(211.179426,122.000000);(211.155502,122.000000);(211.131579,122.000000);(211.107656,122.000000);(211.083732,122.000000);(211.059809,122.000000);(211.035885,122.000000);(211.011962,122.000000);(210.988038,122.000000);(210.964115,122.000000);(210.940191,122.000000);(210.916268,122.000000);(210.892344,122.000000);(210.868421,122.000000);(210.844498,122.000000);(210.820574,122.000000);(210.796651,122.000000);(210.772727,122.000000);(210.748804,122.000000);(210.724880,122.000000);(210.700957,122.000000);(210.677033,122.000000);(210.653110,122.000000);(210.629187,122.000000);(210.605263,122.000000);(210.581340,122.000000);(210.557416,122.000000);(210.533493,122.000000);(210.509569,122.000000);(210.485646,122.000000);(210.461722,122.000000);(210.437799,122.000000);(210.413876,122.000000);(210.389952,122.000000);(210.366029,122.000000);(210.342105,122.000000);(210.318182,122.000000);(210.294258,122.000000);(210.270335,122.000000);(210.246411,122.000000);(210.222488,122.000000);(210.198565,122.000000);(210.174641,122.000000);(210.150718,122.000000);(210.126794,122.000000);(210.102871,122.000000);(210.078947,122.000000);(210.055024,122.000000);</t>
+    <t>214.815789_122.000000;214.791866_122.000000;214.767943_122.000000;214.744019_122.000000;214.720096_122.000000;214.696172_122.000000;214.672249_122.000000;214.648325_122.000000;214.624402_122.000000;214.600478_122.000000;214.576555_122.000000;214.552632_122.000000;214.528708_122.000000;214.504785_122.000000;214.480861_122.000000;214.456938_122.000000;214.433014_122.000000;214.409091_122.000000;214.385167_122.000000;214.361244_122.000000;214.337321_122.000000;214.313397_122.000000;214.289474_122.000000;214.265550_122.000000;214.241627_122.000000;214.217703_122.000000;214.193780_122.000000;214.169856_122.000000;214.145933_122.000000;214.122010_122.000000;214.098086_122.000000;214.074163_122.000000;214.050239_122.000000;214.026316_122.000000;214.002392_122.000000;213.978469_122.000000;213.954545_122.000000;213.930622_122.000000;213.906699_122.000000;213.882775_122.000000;213.858852_122.000000;213.834928_122.000000;213.811005_122.000000;213.787081_122.000000;213.763158_122.000000;213.739234_122.000000;213.715311_122.000000;213.691388_122.000000;213.667464_122.000000;213.643541_122.000000;213.619617_122.000000;213.595694_122.000000;213.571770_122.000000;213.547847_122.000000;213.523923_122.000000;213.500000_122.000000;213.476077_122.000000;213.452153_122.000000;213.428230_122.000000;213.404306_122.000000;213.380383_122.000000;213.356459_122.000000;213.332536_122.000000;213.308612_122.000000;213.284689_122.000000;213.260766_122.000000;213.236842_122.000000;213.212919_122.000000;213.188995_122.000000;213.165072_122.000000;213.141148_122.000000;213.117225_122.000000;213.093301_122.000000;213.069378_122.000000;213.045455_122.000000;213.021531_122.000000;212.997608_122.000000;212.973684_122.000000;212.949761_122.000000;212.925837_122.000000;212.901914_122.000000;212.877990_122.000000;212.854067_122.000000;212.830144_122.000000;212.806220_122.000000;212.782297_122.000000;212.758373_122.000000;212.734450_122.000000;212.710526_122.000000;212.686603_122.000000;212.662679_122.000000;212.638756_122.000000;212.614833_122.000000;212.590909_122.000000;212.566986_122.000000;212.543062_122.000000;212.519139_122.000000;212.495215_122.000000;212.471292_122.000000;212.447368_122.000000;212.423445_122.000000;212.399522_122.000000;212.375598_122.000000;212.351675_122.000000;212.327751_122.000000;212.303828_122.000000;212.279904_122.000000;212.255981_122.000000;212.232057_122.000000;212.208134_122.000000;212.184211_122.000000;212.160287_122.000000;212.136364_122.000000;212.112440_122.000000;212.088517_122.000000;212.064593_122.000000;212.040670_122.000000;212.016746_122.000000;211.992823_122.000000;211.968900_122.000000;211.944976_122.000000;211.921053_122.000000;211.897129_122.000000;211.873206_122.000000;211.849282_122.000000;211.825359_122.000000;211.801435_122.000000;211.777512_122.000000;211.753589_122.000000;211.729665_122.000000;211.705742_122.000000;211.681818_122.000000;211.657895_122.000000;211.633971_122.000000;211.610048_122.000000;211.586124_122.000000;211.562201_122.000000;211.538278_122.000000;211.514354_122.000000;211.490431_122.000000;211.466507_122.000000;211.442584_122.000000;211.418660_122.000000;211.394737_122.000000;211.370813_122.000000;211.346890_122.000000;211.322967_122.000000;211.299043_122.000000;211.275120_122.000000;211.251196_122.000000;211.227273_122.000000;211.203349_122.000000;211.179426_122.000000;211.155502_122.000000;211.131579_122.000000;211.107656_122.000000;211.083732_122.000000;211.059809_122.000000;211.035885_122.000000;211.011962_122.000000;210.988038_122.000000;210.964115_122.000000;210.940191_122.000000;210.916268_122.000000;210.892344_122.000000;210.868421_122.000000;210.844498_122.000000;210.820574_122.000000;210.796651_122.000000;210.772727_122.000000;210.748804_122.000000;210.724880_122.000000;210.700957_122.000000;210.677033_122.000000;210.653110_122.000000;210.629187_122.000000;210.605263_122.000000;210.581340_122.000000;210.557416_122.000000;210.533493_122.000000;210.509569_122.000000;210.485646_122.000000;210.461722_122.000000;210.437799_122.000000;210.413876_122.000000;210.389952_122.000000;210.366029_122.000000;210.342105_122.000000;210.318182_122.000000;210.294258_122.000000;210.270335_122.000000;210.246411_122.000000;210.222488_122.000000;210.198565_122.000000;210.174641_122.000000;210.150718_122.000000;210.126794_122.000000;210.102871_122.000000;210.078947_122.000000;210.055024_122.000000;</t>
   </si>
   <si>
-    <t>(210.055024,122.000000);(210.031100,122.000000);(210.007177,122.000000);(209.983254,122.000000);(209.959330,122.000000);(209.935407,122.000000);(209.911483,122.000000);(209.887560,122.000000);(209.863636,122.000000);(209.839713,122.000000);(209.815789,122.000000);(209.791866,122.000000);(209.767943,122.000000);(209.744019,122.000000);(209.720096,122.000000);(209.696172,122.000000);(209.672249,122.000000);(209.648325,122.000000);(209.624402,122.000000);(209.600478,122.000000);(209.576555,122.000000);(209.552632,122.000000);(209.528708,122.000000);(209.504785,122.000000);(209.480861,122.000000);(209.456938,122.000000);(209.433014,122.000000);(209.409091,122.000000);(209.385167,122.000000);(209.361244,122.000000);(209.337321,122.000000);(209.313397,122.000000);(209.289474,122.000000);(209.265550,122.000000);(209.241627,122.000000);(209.217703,122.000000);(209.193780,122.000000);(209.169856,122.000000);(209.145933,122.000000);(209.122010,122.000000);(209.098086,122.000000);(209.074163,122.000000);(209.050239,122.000000);(209.026316,122.000000);(209.002392,122.000000);(208.978469,122.000000);(208.954545,122.000000);(208.930622,122.000000);(208.906699,122.000000);(208.882775,122.000000);(208.858852,122.000000);(208.834928,122.000000);(208.811005,122.000000);(208.787081,122.000000);(208.763158,122.000000);(208.739234,122.000000);(208.715311,122.000000);(208.691388,122.000000);(208.667464,122.000000);(208.643541,122.000000);(208.619617,122.000000);(208.595694,122.000000);(208.571770,122.000000);(208.547847,122.000000);(208.523923,122.000000);(208.500000,122.000000);(208.476077,122.000000);(208.452153,122.000000);(208.428230,122.000000);(208.404306,122.000000);(208.380383,122.000000);(208.356459,122.000000);(208.332536,122.000000);(208.308612,122.000000);(208.284689,122.000000);(208.260766,122.000000);(208.236842,122.000000);(208.212919,122.000000);(208.188995,122.000000);(208.165072,122.000000);(208.141148,122.000000);(208.117225,122.000000);(208.093301,122.000000);(208.069378,122.000000);(208.045455,122.000000);(208.021531,122.000000);(207.997608,122.000000);(207.973684,122.000000);(207.949761,122.000000);(207.925837,122.000000);(207.901914,122.000000);(207.877990,122.000000);(207.854067,122.000000);(207.830144,122.000000);(207.806220,122.000000);(207.782297,122.000000);(207.758373,122.000000);(207.734450,122.000000);(207.710526,122.000000);(207.686603,122.000000);(207.662679,122.000000);(207.638756,122.000000);(207.614833,122.000000);(207.590909,122.000000);(207.566986,122.000000);(207.543062,122.000000);(207.519139,122.000000);(207.495215,122.000000);(207.471292,122.000000);(207.447368,122.000000);(207.423445,122.000000);(207.399522,122.000000);(207.375598,122.000000);(207.351675,122.000000);(207.327751,122.000000);(207.303828,122.000000);(207.279904,122.000000);(207.255981,122.000000);(207.232057,122.000000);(207.208134,122.000000);(207.184211,122.000000);(207.160287,122.000000);(207.136364,122.000000);(207.112440,122.000000);(207.088517,122.000000);(207.064593,122.000000);(207.040670,122.000000);(207.016746,122.000000);(206.992823,122.000000);(206.968900,122.000000);(206.944976,122.000000);(206.921053,122.000000);(206.897129,122.000000);(206.873206,122.000000);(206.849282,122.000000);(206.825359,122.000000);(206.801435,122.000000);(206.777512,122.000000);(206.753589,122.000000);(206.729665,122.000000);(206.705742,122.000000);(206.681818,122.000000);(206.657895,122.000000);(206.633971,122.000000);(206.610048,122.000000);(206.586124,122.000000);(206.562201,122.000000);(206.538278,122.000000);(206.514354,122.000000);(206.490431,122.000000);(206.466507,122.000000);(206.442584,122.000000);(206.418660,122.000000);(206.394737,122.000000);(206.370813,122.000000);(206.346890,122.000000);(206.322967,122.000000);(206.299043,122.000000);(206.275120,122.000000);(206.251196,122.000000);(206.227273,122.000000);(206.203349,122.000000);(206.179426,122.000000);(206.155502,122.000000);(206.131579,122.000000);(206.107656,122.000000);(206.083732,122.000000);(206.059809,122.000000);(206.035885,122.000000);(206.011962,122.000000);(205.988038,122.000000);(205.964115,122.000000);(205.940191,122.000000);(205.916268,122.000000);(205.892344,122.000000);(205.868421,122.000000);(205.844498,122.000000);(205.820574,122.000000);(205.796651,122.000000);(205.772727,122.000000);(205.748804,122.000000);(205.724880,122.000000);(205.700957,122.000000);(205.677033,122.000000);(205.653110,122.000000);(205.629187,122.000000);(205.605263,122.000000);(205.581340,122.000000);(205.557416,122.000000);(205.533493,122.000000);(205.509569,122.000000);(205.485646,122.000000);(205.461722,122.000000);(205.437799,122.000000);(205.413876,122.000000);(205.389952,122.000000);(205.366029,122.000000);(205.342105,122.000000);(205.318182,122.000000);(205.294258,122.000000);(205.270335,122.000000);(205.246411,122.000000);(205.222488,122.000000);(205.198565,122.000000);(205.174641,122.000000);(205.150718,122.000000);(205.126794,122.000000);(205.102871,122.000000);(205.078947,122.000000);(205.055024,122.000000);(205.031100,122.000000);(205.007177,122.000000);(204.983254,122.000000);(204.959330,122.000000);(204.935407,122.000000);(204.911483,122.000000);(204.887560,122.000000);(204.863636,122.000000);(204.839713,122.000000);(204.815789,122.000000);(204.791866,122.000000);(204.767943,122.000000);(204.744019,122.000000);(204.720096,122.000000);(204.696172,122.000000);(204.672249,122.000000);(204.648325,122.000000);(204.624402,122.000000);(204.600478,122.000000);(204.576555,122.000000);(204.552632,122.000000);(204.528708,122.000000);(204.504785,122.000000);(204.480861,122.000000);(204.456938,122.000000);(204.433014,122.000000);(204.409091,122.000000);(204.385167,122.000000);(204.361244,122.000000);(204.337321,122.000000);(204.313397,122.000000);(204.289474,122.000000);(204.265550,122.000000);(204.241627,122.000000);(204.217703,122.000000);(204.193780,122.000000);(204.169856,122.000000);(204.145933,122.000000);(204.122010,122.000000);(204.098086,122.000000);(204.074163,122.000000);(204.050239,122.000000);(204.026316,122.000000);(204.002392,122.000000);(203.978469,122.000000);(203.954545,122.000000);(203.930622,122.000000);(203.906699,122.000000);(203.882775,122.000000);(203.858852,122.000000);(203.834928,122.000000);(203.811005,122.000000);(203.787081,122.000000);(203.763158,122.000000);(203.739234,122.000000);(203.715311,122.000000);(203.691388,122.000000);(203.667464,122.000000);(203.643541,122.000000);(203.619617,122.000000);(203.595694,122.000000);(203.571770,122.000000);(203.547847,122.000000);(203.523923,122.000000);(203.500000,122.000000);(203.476077,122.000000);(203.452153,122.000000);(203.428230,122.000000);(203.404306,122.000000);(203.380383,122.000000);(203.356459,122.000000);(203.332536,122.000000);(203.308612,122.000000);(203.284689,122.000000);(203.260766,122.000000);(203.236842,122.000000);(203.212919,122.000000);(203.188995,122.000000);(203.165072,122.000000);(203.141148,122.000000);(203.117225,122.000000);(203.093301,122.000000);(203.069378,122.000000);(203.045455,122.000000);(203.021531,122.000000);(202.997608,122.000000);(202.973684,122.000000);(202.949761,122.000000);(202.925837,122.000000);(202.901914,122.000000);(202.877990,122.000000);(202.854067,122.000000);(202.830144,122.000000);(202.806220,122.000000);(202.782297,122.000000);(202.758373,122.000000);(202.734450,122.000000);(202.710526,122.000000);(202.686603,122.000000);(202.662679,122.000000);(202.638756,122.000000);(202.614833,122.000000);(202.590909,122.000000);(202.566986,122.000000);(202.543062,122.000000);(202.519139,122.000000);(202.495215,122.000000);(202.471292,122.000000);(202.447368,122.000000);(202.423445,122.000000);(202.399522,122.000000);(202.375598,122.000000);(202.351675,122.000000);(202.327751,122.000000);(202.303828,122.000000);(202.279904,122.000000);(202.255981,122.000000);(202.232057,122.000000);(202.208134,122.000000);(202.184211,122.000000);(202.160287,122.000000);(202.136364,122.000000);(202.112440,122.000000);(202.088517,122.000000);(202.064593,122.000000);(202.040670,122.000000);(202.016746,122.000000);(201.992823,122.000000);(201.968900,122.000000);(201.944976,122.000000);(201.921053,122.000000);(201.897129,122.000000);(201.873206,122.000000);(201.849282,122.000000);(201.825359,122.000000);(201.801435,122.000000);(201.777512,122.000000);(201.753589,122.000000);(201.729665,122.000000);(201.705742,122.000000);(201.681818,122.000000);(201.657895,122.000000);(201.633971,122.000000);(201.610048,122.000000);(201.586124,122.000000);(201.562201,122.000000);(201.538278,122.000000);(201.514354,122.000000);(201.490431,122.000000);(201.466507,122.000000);(201.442584,122.000000);(201.418660,122.000000);(201.394737,122.000000);(201.370813,122.000000);(201.346890,122.000000);(201.322967,122.000000);(201.299043,122.000000);(201.275120,122.000000);(201.251196,122.000000);(201.227273,122.000000);(201.203349,122.000000);(201.179426,122.000000);(201.155502,122.000000);(201.131579,122.000000);(201.107656,122.000000);(201.083732,122.000000);(201.059809,122.000000);(201.035885,122.000000);(201.011962,122.000000);(200.988038,122.000000);(200.964115,122.000000);(200.940191,122.000000);(200.916268,122.000000);(200.892344,122.000000);(200.868421,122.000000);(200.844498,122.000000);(200.820574,122.000000);(200.796651,122.000000);(200.772727,122.000000);(200.748804,122.000000);(200.724880,122.000000);(200.700957,122.000000);(200.677033,122.000000);(200.653110,122.000000);(200.629187,122.000000);(200.605263,122.000000);(200.581340,122.000000);(200.557416,122.000000);(200.533493,122.000000);(200.509569,122.000000);</t>
+    <t>210.055024_122.000000;210.031100_122.000000;210.007177_122.000000;209.983254_122.000000;209.959330_122.000000;209.935407_122.000000;209.911483_122.000000;209.887560_122.000000;209.863636_122.000000;209.839713_122.000000;209.815789_122.000000;209.791866_122.000000;209.767943_122.000000;209.744019_122.000000;209.720096_122.000000;209.696172_122.000000;209.672249_122.000000;209.648325_122.000000;209.624402_122.000000;209.600478_122.000000;209.576555_122.000000;209.552632_122.000000;209.528708_122.000000;209.504785_122.000000;209.480861_122.000000;209.456938_122.000000;209.433014_122.000000;209.409091_122.000000;209.385167_122.000000;209.361244_122.000000;209.337321_122.000000;209.313397_122.000000;209.289474_122.000000;209.265550_122.000000;209.241627_122.000000;209.217703_122.000000;209.193780_122.000000;209.169856_122.000000;209.145933_122.000000;209.122010_122.000000;209.098086_122.000000;209.074163_122.000000;209.050239_122.000000;209.026316_122.000000;209.002392_122.000000;208.978469_122.000000;208.954545_122.000000;208.930622_122.000000;208.906699_122.000000;208.882775_122.000000;208.858852_122.000000;208.834928_122.000000;208.811005_122.000000;208.787081_122.000000;208.763158_122.000000;208.739234_122.000000;208.715311_122.000000;208.691388_122.000000;208.667464_122.000000;208.643541_122.000000;208.619617_122.000000;208.595694_122.000000;208.571770_122.000000;208.547847_122.000000;208.523923_122.000000;208.500000_122.000000;208.476077_122.000000;208.452153_122.000000;208.428230_122.000000;208.404306_122.000000;208.380383_122.000000;208.356459_122.000000;208.332536_122.000000;208.308612_122.000000;208.284689_122.000000;208.260766_122.000000;208.236842_122.000000;208.212919_122.000000;208.188995_122.000000;208.165072_122.000000;208.141148_122.000000;208.117225_122.000000;208.093301_122.000000;208.069378_122.000000;208.045455_122.000000;208.021531_122.000000;207.997608_122.000000;207.973684_122.000000;207.949761_122.000000;207.925837_122.000000;207.901914_122.000000;207.877990_122.000000;207.854067_122.000000;207.830144_122.000000;207.806220_122.000000;207.782297_122.000000;207.758373_122.000000;207.734450_122.000000;207.710526_122.000000;207.686603_122.000000;207.662679_122.000000;207.638756_122.000000;207.614833_122.000000;207.590909_122.000000;207.566986_122.000000;207.543062_122.000000;207.519139_122.000000;207.495215_122.000000;207.471292_122.000000;207.447368_122.000000;207.423445_122.000000;207.399522_122.000000;207.375598_122.000000;207.351675_122.000000;207.327751_122.000000;207.303828_122.000000;207.279904_122.000000;207.255981_122.000000;207.232057_122.000000;207.208134_122.000000;207.184211_122.000000;207.160287_122.000000;207.136364_122.000000;207.112440_122.000000;207.088517_122.000000;207.064593_122.000000;207.040670_122.000000;207.016746_122.000000;206.992823_122.000000;206.968900_122.000000;206.944976_122.000000;206.921053_122.000000;206.897129_122.000000;206.873206_122.000000;206.849282_122.000000;206.825359_122.000000;206.801435_122.000000;206.777512_122.000000;206.753589_122.000000;206.729665_122.000000;206.705742_122.000000;206.681818_122.000000;206.657895_122.000000;206.633971_122.000000;206.610048_122.000000;206.586124_122.000000;206.562201_122.000000;206.538278_122.000000;206.514354_122.000000;206.490431_122.000000;206.466507_122.000000;206.442584_122.000000;206.418660_122.000000;206.394737_122.000000;206.370813_122.000000;206.346890_122.000000;206.322967_122.000000;206.299043_122.000000;206.275120_122.000000;206.251196_122.000000;206.227273_122.000000;206.203349_122.000000;206.179426_122.000000;206.155502_122.000000;206.131579_122.000000;206.107656_122.000000;206.083732_122.000000;206.059809_122.000000;206.035885_122.000000;206.011962_122.000000;205.988038_122.000000;205.964115_122.000000;205.940191_122.000000;205.916268_122.000000;205.892344_122.000000;205.868421_122.000000;205.844498_122.000000;205.820574_122.000000;205.796651_122.000000;205.772727_122.000000;205.748804_122.000000;205.724880_122.000000;205.700957_122.000000;205.677033_122.000000;205.653110_122.000000;205.629187_122.000000;205.605263_122.000000;205.581340_122.000000;205.557416_122.000000;205.533493_122.000000;205.509569_122.000000;205.485646_122.000000;205.461722_122.000000;205.437799_122.000000;205.413876_122.000000;205.389952_122.000000;205.366029_122.000000;205.342105_122.000000;205.318182_122.000000;205.294258_122.000000;205.270335_122.000000;205.246411_122.000000;205.222488_122.000000;205.198565_122.000000;205.174641_122.000000;205.150718_122.000000;205.126794_122.000000;205.102871_122.000000;205.078947_122.000000;205.055024_122.000000;205.031100_122.000000;205.007177_122.000000;204.983254_122.000000;204.959330_122.000000;204.935407_122.000000;204.911483_122.000000;204.887560_122.000000;204.863636_122.000000;204.839713_122.000000;204.815789_122.000000;204.791866_122.000000;204.767943_122.000000;204.744019_122.000000;204.720096_122.000000;204.696172_122.000000;204.672249_122.000000;204.648325_122.000000;204.624402_122.000000;204.600478_122.000000;204.576555_122.000000;204.552632_122.000000;204.528708_122.000000;204.504785_122.000000;204.480861_122.000000;204.456938_122.000000;204.433014_122.000000;204.409091_122.000000;204.385167_122.000000;204.361244_122.000000;204.337321_122.000000;204.313397_122.000000;204.289474_122.000000;204.265550_122.000000;204.241627_122.000000;204.217703_122.000000;204.193780_122.000000;204.169856_122.000000;204.145933_122.000000;204.122010_122.000000;204.098086_122.000000;204.074163_122.000000;204.050239_122.000000;204.026316_122.000000;204.002392_122.000000;203.978469_122.000000;203.954545_122.000000;203.930622_122.000000;203.906699_122.000000;203.882775_122.000000;203.858852_122.000000;203.834928_122.000000;203.811005_122.000000;203.787081_122.000000;203.763158_122.000000;203.739234_122.000000;203.715311_122.000000;203.691388_122.000000;203.667464_122.000000;203.643541_122.000000;203.619617_122.000000;203.595694_122.000000;203.571770_122.000000;203.547847_122.000000;203.523923_122.000000;203.500000_122.000000;203.476077_122.000000;203.452153_122.000000;203.428230_122.000000;203.404306_122.000000;203.380383_122.000000;203.356459_122.000000;203.332536_122.000000;203.308612_122.000000;203.284689_122.000000;203.260766_122.000000;203.236842_122.000000;203.212919_122.000000;203.188995_122.000000;203.165072_122.000000;203.141148_122.000000;203.117225_122.000000;203.093301_122.000000;203.069378_122.000000;203.045455_122.000000;203.021531_122.000000;202.997608_122.000000;202.973684_122.000000;202.949761_122.000000;202.925837_122.000000;202.901914_122.000000;202.877990_122.000000;202.854067_122.000000;202.830144_122.000000;202.806220_122.000000;202.782297_122.000000;202.758373_122.000000;202.734450_122.000000;202.710526_122.000000;202.686603_122.000000;202.662679_122.000000;202.638756_122.000000;202.614833_122.000000;202.590909_122.000000;202.566986_122.000000;202.543062_122.000000;202.519139_122.000000;202.495215_122.000000;202.471292_122.000000;202.447368_122.000000;202.423445_122.000000;202.399522_122.000000;202.375598_122.000000;202.351675_122.000000;202.327751_122.000000;202.303828_122.000000;202.279904_122.000000;202.255981_122.000000;202.232057_122.000000;202.208134_122.000000;202.184211_122.000000;202.160287_122.000000;202.136364_122.000000;202.112440_122.000000;202.088517_122.000000;202.064593_122.000000;202.040670_122.000000;202.016746_122.000000;201.992823_122.000000;201.968900_122.000000;201.944976_122.000000;201.921053_122.000000;201.897129_122.000000;201.873206_122.000000;201.849282_122.000000;201.825359_122.000000;201.801435_122.000000;201.777512_122.000000;201.753589_122.000000;201.729665_122.000000;201.705742_122.000000;201.681818_122.000000;201.657895_122.000000;201.633971_122.000000;201.610048_122.000000;201.586124_122.000000;201.562201_122.000000;201.538278_122.000000;201.514354_122.000000;201.490431_122.000000;201.466507_122.000000;201.442584_122.000000;201.418660_122.000000;201.394737_122.000000;201.370813_122.000000;201.346890_122.000000;201.322967_122.000000;201.299043_122.000000;201.275120_122.000000;201.251196_122.000000;201.227273_122.000000;201.203349_122.000000;201.179426_122.000000;201.155502_122.000000;201.131579_122.000000;201.107656_122.000000;201.083732_122.000000;201.059809_122.000000;201.035885_122.000000;201.011962_122.000000;200.988038_122.000000;200.964115_122.000000;200.940191_122.000000;200.916268_122.000000;200.892344_122.000000;200.868421_122.000000;200.844498_122.000000;200.820574_122.000000;200.796651_122.000000;200.772727_122.000000;200.748804_122.000000;200.724880_122.000000;200.700957_122.000000;200.677033_122.000000;200.653110_122.000000;200.629187_122.000000;200.605263_122.000000;200.581340_122.000000;200.557416_122.000000;200.533493_122.000000;200.509569_122.000000;</t>
   </si>
   <si>
-    <t>(200.509569,122.000000);(200.485646,122.000000);(200.461722,122.000000);(200.437799,122.000000);(200.413876,122.000000);(200.389952,122.000000);(200.366029,122.000000);(200.342105,122.000000);(200.318182,122.000000);(200.294258,122.000000);(200.270335,122.000000);(200.246411,122.000000);(200.222488,122.000000);(200.198565,122.000000);(200.174641,122.000000);(200.150718,122.000000);(200.126794,122.000000);(200.102871,122.000000);(200.078947,122.000000);(200.055024,122.000000);(200.031100,122.000000);(200.007177,122.000000);(199.983254,122.000000);(199.959330,122.000000);(199.935407,122.000000);(199.911483,122.000000);(199.887560,122.000000);(199.863636,122.000000);(199.839713,122.000000);(199.815789,122.000000);(199.791866,122.000000);(199.767943,122.000000);(199.744019,122.000000);(199.720096,122.000000);(199.696172,122.000000);(199.672249,122.000000);(199.648325,122.000000);(199.624402,122.000000);(199.600478,122.000000);(199.576555,122.000000);(199.552632,122.000000);(199.528708,122.000000);(199.504785,122.000000);(199.480861,122.000000);(199.456938,122.000000);(199.433014,122.000000);(199.409091,122.000000);(199.385167,122.000000);(199.361244,122.000000);(199.337321,122.000000);(199.313397,122.000000);(199.289474,122.000000);(199.265550,122.000000);(199.241627,122.000000);(199.217703,122.000000);(199.193780,122.000000);(199.169856,122.000000);(199.145933,122.000000);(199.122010,122.000000);(199.098086,122.000000);(199.074163,122.000000);(199.050239,122.000000);(199.026316,122.000000);(199.002392,122.000000);(198.978469,122.000000);(198.954545,122.000000);(198.930622,122.000000);(198.906699,122.000000);(198.882775,122.000000);(198.858852,122.000000);(198.834928,122.000000);(198.811005,122.000000);(198.787081,122.000000);(198.763158,122.000000);(198.739234,122.000000);(198.715311,122.000000);(198.691388,122.000000);(198.667464,122.000000);(198.643541,122.000000);(198.619617,122.000000);(198.595694,122.000000);(198.571770,122.000000);(198.547847,122.000000);(198.523923,122.000000);(198.500000,122.000000);(198.476077,122.000000);(198.452153,122.000000);(198.428230,122.000000);(198.404306,122.000000);(198.380383,122.000000);(198.356459,122.000000);(198.332536,122.000000);(198.308612,122.000000);(198.284689,122.000000);(198.260766,122.000000);(198.236842,122.000000);(198.212919,122.000000);(198.188995,122.000000);(198.165072,122.000000);(198.141148,122.000000);(198.117225,122.000000);(198.093301,122.000000);(198.069378,122.000000);(198.045455,122.000000);(198.021531,122.000000);(197.997608,122.000000);(197.973684,122.000000);(197.949761,122.000000);(197.925837,122.000000);(197.901914,122.000000);(197.877990,122.000000);(197.854067,122.000000);(197.830144,122.000000);(197.806220,122.000000);(197.782297,122.000000);(197.758373,122.000000);(197.734450,122.000000);(197.710526,122.000000);(197.686603,122.000000);(197.662679,122.000000);(197.638756,122.000000);(197.614833,122.000000);(197.590909,122.000000);(197.566986,122.000000);(197.543062,122.000000);(197.519139,122.000000);(197.495215,122.000000);(197.471292,122.000000);(197.447368,122.000000);(197.423445,122.000000);(197.399522,122.000000);(197.375598,122.000000);(197.351675,122.000000);(197.327751,122.000000);(197.303828,122.000000);(197.279904,122.000000);(197.255981,122.000000);(197.232057,122.000000);(197.208134,122.000000);(197.184211,122.000000);(197.160287,122.000000);(197.136364,122.000000);(197.112440,122.000000);(197.088517,122.000000);(197.064593,122.000000);(197.040670,122.000000);(197.016746,122.000000);(196.992823,122.000000);(196.968900,122.000000);(196.944976,122.000000);(196.921053,122.000000);(196.897129,122.000000);(196.873206,122.000000);(196.849282,122.000000);(196.825359,122.000000);(196.801435,122.000000);(196.777512,122.000000);(196.753589,122.000000);(196.729665,122.000000);(196.705742,122.000000);(196.681818,122.000000);(196.657895,122.000000);(196.633971,122.000000);(196.610048,122.000000);(196.586124,122.000000);(196.562201,122.000000);(196.538278,122.000000);(196.514354,122.000000);(196.490431,122.000000);(196.466507,122.000000);(196.442584,122.000000);(196.418660,122.000000);(196.394737,122.000000);(196.370813,122.000000);(196.346890,122.000000);(196.322967,122.000000);(196.299043,122.000000);(196.275120,122.000000);(196.251196,122.000000);(196.227273,122.000000);(196.203349,122.000000);(196.179426,122.000000);(196.155502,122.000000);(196.131579,122.000000);(196.107656,122.000000);(196.083732,122.000000);(196.059809,122.000000);(196.035885,122.000000);(196.011962,122.000000);(195.988038,122.000000);(195.964115,122.000000);(195.940191,122.000000);(195.916268,122.000000);(195.892344,122.000000);(195.868421,122.000000);(195.844498,122.000000);(195.820574,122.000000);(195.796651,122.000000);(195.772727,122.000000);(195.748804,122.000000);(195.724880,122.000000);(195.700957,122.000000);(195.677033,122.000000);(195.653110,122.000000);(195.629187,122.000000);(195.605263,122.000000);(195.581340,122.000000);(195.557416,122.000000);(195.533493,122.000000);(195.509569,122.000000);(195.485646,122.000000);(195.461722,122.000000);(195.437799,122.000000);(195.413876,122.000000);(195.389952,122.000000);(195.366029,122.000000);(195.342105,122.000000);(195.318182,122.000000);(195.294258,122.000000);(195.270335,122.000000);(195.246411,122.000000);(195.222488,122.000000);(195.198565,122.000000);(195.174641,122.000000);(195.150718,122.000000);(195.126794,122.000000);(195.102871,122.000000);(195.078947,122.000000);(195.055024,122.000000);(195.031100,122.000000);(195.007177,122.000000);(194.983254,122.000000);(194.959330,122.000000);(194.935407,122.000000);(194.911483,122.000000);(194.887560,122.000000);(194.863636,122.000000);(194.839713,122.000000);(194.815789,122.000000);(194.791866,122.000000);(194.767943,122.000000);(194.744019,122.000000);(194.720096,122.000000);(194.696172,122.000000);(194.672249,122.000000);(194.648325,122.000000);(194.624402,122.000000);(194.600478,122.000000);(194.576555,122.000000);(194.552632,122.000000);(194.528708,122.000000);(194.504785,122.000000);(194.480861,122.000000);(194.456938,122.000000);(194.433014,122.000000);(194.409091,122.000000);(194.385167,122.000000);(194.361244,122.000000);(194.337321,122.000000);(194.313397,122.000000);(194.289474,122.000000);(194.265550,122.000000);(194.241627,122.000000);(194.217703,122.000000);(194.193780,122.000000);(194.169856,122.000000);(194.145933,122.000000);(194.122010,122.000000);(194.098086,122.000000);(194.074163,122.000000);(194.050239,122.000000);(194.026316,122.000000);(194.002392,122.000000);(193.978469,122.000000);(193.954545,122.000000);(193.930622,122.000000);(193.906699,122.000000);(193.882775,122.000000);(193.858852,122.000000);(193.834928,122.000000);(193.811005,122.000000);(193.787081,122.000000);(193.763158,122.000000);(193.739234,122.000000);(193.715311,122.000000);(193.691388,122.000000);(193.667464,122.000000);(193.643541,122.000000);(193.619617,122.000000);(193.595694,122.000000);(193.571770,122.000000);(193.547847,122.000000);(193.523923,122.000000);(193.500000,122.000000);(193.476077,122.000000);(193.452153,122.000000);(193.428230,122.000000);(193.404306,122.000000);(193.380383,122.000000);(193.356459,122.000000);(193.332536,122.000000);(193.308612,122.000000);(193.284689,122.000000);(193.260766,122.000000);(193.236842,122.000000);(193.212919,122.000000);(193.188995,122.000000);(193.165072,122.000000);(193.141148,122.000000);(193.117225,122.000000);(193.093301,122.000000);(193.069378,122.000000);(193.045455,122.000000);(193.021531,122.000000);(192.997608,122.000000);(192.973684,122.000000);(192.949761,122.000000);(192.925837,122.000000);(192.901914,122.000000);(192.877990,122.000000);(192.854067,122.000000);(192.830144,122.000000);(192.806220,122.000000);(192.782297,122.000000);(192.758373,122.000000);(192.734450,122.000000);(192.710526,122.000000);(192.686603,122.000000);(192.662679,122.000000);(192.638756,122.000000);(192.614833,122.000000);(192.590909,122.000000);(192.566986,122.000000);(192.543062,122.000000);(192.519139,122.000000);(192.495215,122.000000);(192.471292,122.000000);(192.447368,122.000000);(192.423445,122.000000);(192.399522,122.000000);(192.375598,122.000000);(192.351675,122.000000);(192.327751,122.000000);(192.303828,122.000000);(192.279904,122.000000);(192.255981,122.000000);(192.232057,122.000000);(192.208134,122.000000);(192.184211,122.000000);(192.160287,122.000000);(192.136364,122.000000);(192.112440,122.000000);(192.088517,122.000000);(192.064593,122.000000);(192.040670,122.000000);(192.016746,122.000000);(191.992823,122.000000);(191.968900,122.000000);(191.944976,122.000000);(191.921053,122.000000);(191.897129,122.000000);(191.873206,122.000000);(191.849282,122.000000);(191.825359,122.000000);(191.801435,122.000000);(191.777512,122.000000);(191.753589,122.000000);(191.729665,122.000000);(191.705742,122.000000);(191.681818,122.000000);(191.657895,122.000000);(191.633971,122.000000);(191.610048,122.000000);(191.586124,122.000000);(191.562201,122.000000);(191.538278,122.000000);(191.514354,122.000000);(191.490431,122.000000);(191.466507,122.000000);(191.442584,122.000000);(191.418660,122.000000);(191.394737,122.000000);(191.370813,122.000000);(191.346890,122.000000);(191.322967,122.000000);(191.299043,122.000000);(191.275120,122.000000);(191.251196,122.000000);(191.227273,122.000000);(191.203349,122.000000);(191.179426,122.000000);(191.155502,122.000000);(191.131579,122.000000);(191.107656,122.000000);(191.083732,122.000000);(191.059809,122.000000);(191.035885,122.000000);(191.011962,122.000000);(190.988038,122.000000);(190.964115,122.000000);</t>
+    <t>200.509569_122.000000;200.485646_122.000000;200.461722_122.000000;200.437799_122.000000;200.413876_122.000000;200.389952_122.000000;200.366029_122.000000;200.342105_122.000000;200.318182_122.000000;200.294258_122.000000;200.270335_122.000000;200.246411_122.000000;200.222488_122.000000;200.198565_122.000000;200.174641_122.000000;200.150718_122.000000;200.126794_122.000000;200.102871_122.000000;200.078947_122.000000;200.055024_122.000000;200.031100_122.000000;200.007177_122.000000;199.983254_122.000000;199.959330_122.000000;199.935407_122.000000;199.911483_122.000000;199.887560_122.000000;199.863636_122.000000;199.839713_122.000000;199.815789_122.000000;199.791866_122.000000;199.767943_122.000000;199.744019_122.000000;199.720096_122.000000;199.696172_122.000000;199.672249_122.000000;199.648325_122.000000;199.624402_122.000000;199.600478_122.000000;199.576555_122.000000;199.552632_122.000000;199.528708_122.000000;199.504785_122.000000;199.480861_122.000000;199.456938_122.000000;199.433014_122.000000;199.409091_122.000000;199.385167_122.000000;199.361244_122.000000;199.337321_122.000000;199.313397_122.000000;199.289474_122.000000;199.265550_122.000000;199.241627_122.000000;199.217703_122.000000;199.193780_122.000000;199.169856_122.000000;199.145933_122.000000;199.122010_122.000000;199.098086_122.000000;199.074163_122.000000;199.050239_122.000000;199.026316_122.000000;199.002392_122.000000;198.978469_122.000000;198.954545_122.000000;198.930622_122.000000;198.906699_122.000000;198.882775_122.000000;198.858852_122.000000;198.834928_122.000000;198.811005_122.000000;198.787081_122.000000;198.763158_122.000000;198.739234_122.000000;198.715311_122.000000;198.691388_122.000000;198.667464_122.000000;198.643541_122.000000;198.619617_122.000000;198.595694_122.000000;198.571770_122.000000;198.547847_122.000000;198.523923_122.000000;198.500000_122.000000;198.476077_122.000000;198.452153_122.000000;198.428230_122.000000;198.404306_122.000000;198.380383_122.000000;198.356459_122.000000;198.332536_122.000000;198.308612_122.000000;198.284689_122.000000;198.260766_122.000000;198.236842_122.000000;198.212919_122.000000;198.188995_122.000000;198.165072_122.000000;198.141148_122.000000;198.117225_122.000000;198.093301_122.000000;198.069378_122.000000;198.045455_122.000000;198.021531_122.000000;197.997608_122.000000;197.973684_122.000000;197.949761_122.000000;197.925837_122.000000;197.901914_122.000000;197.877990_122.000000;197.854067_122.000000;197.830144_122.000000;197.806220_122.000000;197.782297_122.000000;197.758373_122.000000;197.734450_122.000000;197.710526_122.000000;197.686603_122.000000;197.662679_122.000000;197.638756_122.000000;197.614833_122.000000;197.590909_122.000000;197.566986_122.000000;197.543062_122.000000;197.519139_122.000000;197.495215_122.000000;197.471292_122.000000;197.447368_122.000000;197.423445_122.000000;197.399522_122.000000;197.375598_122.000000;197.351675_122.000000;197.327751_122.000000;197.303828_122.000000;197.279904_122.000000;197.255981_122.000000;197.232057_122.000000;197.208134_122.000000;197.184211_122.000000;197.160287_122.000000;197.136364_122.000000;197.112440_122.000000;197.088517_122.000000;197.064593_122.000000;197.040670_122.000000;197.016746_122.000000;196.992823_122.000000;196.968900_122.000000;196.944976_122.000000;196.921053_122.000000;196.897129_122.000000;196.873206_122.000000;196.849282_122.000000;196.825359_122.000000;196.801435_122.000000;196.777512_122.000000;196.753589_122.000000;196.729665_122.000000;196.705742_122.000000;196.681818_122.000000;196.657895_122.000000;196.633971_122.000000;196.610048_122.000000;196.586124_122.000000;196.562201_122.000000;196.538278_122.000000;196.514354_122.000000;196.490431_122.000000;196.466507_122.000000;196.442584_122.000000;196.418660_122.000000;196.394737_122.000000;196.370813_122.000000;196.346890_122.000000;196.322967_122.000000;196.299043_122.000000;196.275120_122.000000;196.251196_122.000000;196.227273_122.000000;196.203349_122.000000;196.179426_122.000000;196.155502_122.000000;196.131579_122.000000;196.107656_122.000000;196.083732_122.000000;196.059809_122.000000;196.035885_122.000000;196.011962_122.000000;195.988038_122.000000;195.964115_122.000000;195.940191_122.000000;195.916268_122.000000;195.892344_122.000000;195.868421_122.000000;195.844498_122.000000;195.820574_122.000000;195.796651_122.000000;195.772727_122.000000;195.748804_122.000000;195.724880_122.000000;195.700957_122.000000;195.677033_122.000000;195.653110_122.000000;195.629187_122.000000;195.605263_122.000000;195.581340_122.000000;195.557416_122.000000;195.533493_122.000000;195.509569_122.000000;195.485646_122.000000;195.461722_122.000000;195.437799_122.000000;195.413876_122.000000;195.389952_122.000000;195.366029_122.000000;195.342105_122.000000;195.318182_122.000000;195.294258_122.000000;195.270335_122.000000;195.246411_122.000000;195.222488_122.000000;195.198565_122.000000;195.174641_122.000000;195.150718_122.000000;195.126794_122.000000;195.102871_122.000000;195.078947_122.000000;195.055024_122.000000;195.031100_122.000000;195.007177_122.000000;194.983254_122.000000;194.959330_122.000000;194.935407_122.000000;194.911483_122.000000;194.887560_122.000000;194.863636_122.000000;194.839713_122.000000;194.815789_122.000000;194.791866_122.000000;194.767943_122.000000;194.744019_122.000000;194.720096_122.000000;194.696172_122.000000;194.672249_122.000000;194.648325_122.000000;194.624402_122.000000;194.600478_122.000000;194.576555_122.000000;194.552632_122.000000;194.528708_122.000000;194.504785_122.000000;194.480861_122.000000;194.456938_122.000000;194.433014_122.000000;194.409091_122.000000;194.385167_122.000000;194.361244_122.000000;194.337321_122.000000;194.313397_122.000000;194.289474_122.000000;194.265550_122.000000;194.241627_122.000000;194.217703_122.000000;194.193780_122.000000;194.169856_122.000000;194.145933_122.000000;194.122010_122.000000;194.098086_122.000000;194.074163_122.000000;194.050239_122.000000;194.026316_122.000000;194.002392_122.000000;193.978469_122.000000;193.954545_122.000000;193.930622_122.000000;193.906699_122.000000;193.882775_122.000000;193.858852_122.000000;193.834928_122.000000;193.811005_122.000000;193.787081_122.000000;193.763158_122.000000;193.739234_122.000000;193.715311_122.000000;193.691388_122.000000;193.667464_122.000000;193.643541_122.000000;193.619617_122.000000;193.595694_122.000000;193.571770_122.000000;193.547847_122.000000;193.523923_122.000000;193.500000_122.000000;193.476077_122.000000;193.452153_122.000000;193.428230_122.000000;193.404306_122.000000;193.380383_122.000000;193.356459_122.000000;193.332536_122.000000;193.308612_122.000000;193.284689_122.000000;193.260766_122.000000;193.236842_122.000000;193.212919_122.000000;193.188995_122.000000;193.165072_122.000000;193.141148_122.000000;193.117225_122.000000;193.093301_122.000000;193.069378_122.000000;193.045455_122.000000;193.021531_122.000000;192.997608_122.000000;192.973684_122.000000;192.949761_122.000000;192.925837_122.000000;192.901914_122.000000;192.877990_122.000000;192.854067_122.000000;192.830144_122.000000;192.806220_122.000000;192.782297_122.000000;192.758373_122.000000;192.734450_122.000000;192.710526_122.000000;192.686603_122.000000;192.662679_122.000000;192.638756_122.000000;192.614833_122.000000;192.590909_122.000000;192.566986_122.000000;192.543062_122.000000;192.519139_122.000000;192.495215_122.000000;192.471292_122.000000;192.447368_122.000000;192.423445_122.000000;192.399522_122.000000;192.375598_122.000000;192.351675_122.000000;192.327751_122.000000;192.303828_122.000000;192.279904_122.000000;192.255981_122.000000;192.232057_122.000000;192.208134_122.000000;192.184211_122.000000;192.160287_122.000000;192.136364_122.000000;192.112440_122.000000;192.088517_122.000000;192.064593_122.000000;192.040670_122.000000;192.016746_122.000000;191.992823_122.000000;191.968900_122.000000;191.944976_122.000000;191.921053_122.000000;191.897129_122.000000;191.873206_122.000000;191.849282_122.000000;191.825359_122.000000;191.801435_122.000000;191.777512_122.000000;191.753589_122.000000;191.729665_122.000000;191.705742_122.000000;191.681818_122.000000;191.657895_122.000000;191.633971_122.000000;191.610048_122.000000;191.586124_122.000000;191.562201_122.000000;191.538278_122.000000;191.514354_122.000000;191.490431_122.000000;191.466507_122.000000;191.442584_122.000000;191.418660_122.000000;191.394737_122.000000;191.370813_122.000000;191.346890_122.000000;191.322967_122.000000;191.299043_122.000000;191.275120_122.000000;191.251196_122.000000;191.227273_122.000000;191.203349_122.000000;191.179426_122.000000;191.155502_122.000000;191.131579_122.000000;191.107656_122.000000;191.083732_122.000000;191.059809_122.000000;191.035885_122.000000;191.011962_122.000000;190.988038_122.000000;190.964115_122.000000;</t>
   </si>
   <si>
-    <t>(190.964115,122.000000);(190.940191,122.000000);(190.916268,122.000000);(190.892344,122.000000);(190.868421,122.000000);(190.844498,122.000000);(190.820574,122.000000);(190.796651,122.000000);(190.772727,122.000000);(190.748804,122.000000);(190.724880,122.000000);(190.700957,122.000000);(190.677033,122.000000);(190.653110,122.000000);(190.629187,122.000000);(190.605263,122.000000);(190.581340,122.000000);(190.557416,122.000000);(190.533493,122.000000);(190.509569,122.000000);(190.485646,122.000000);(190.461722,122.000000);(190.437799,122.000000);(190.413876,122.000000);(190.389952,122.000000);(190.366029,122.000000);(190.342105,122.000000);(190.318182,122.000000);(190.294258,122.000000);(190.270335,122.000000);(190.246411,122.000000);(190.222488,122.000000);(190.198565,122.000000);(190.174641,122.000000);(190.150718,122.000000);(190.126794,122.000000);(190.102871,122.000000);(190.078947,122.000000);(190.055024,122.000000);(190.031100,122.000000);(190.007177,122.000000);(189.983254,122.000000);(189.959330,122.000000);(189.935407,122.000000);(189.911483,122.000000);(189.887560,122.000000);(189.863636,122.000000);(189.839713,122.000000);(189.815789,122.000000);(189.791866,122.000000);(189.767943,122.000000);(189.744019,122.000000);(189.720096,122.000000);(189.696172,122.000000);(189.672249,122.000000);(189.648325,122.000000);(189.624402,122.000000);(189.600478,122.000000);(189.576555,122.000000);(189.552632,122.000000);(189.528708,122.000000);(189.504785,122.000000);(189.480861,122.000000);(189.456938,122.000000);(189.433014,122.000000);(189.409091,122.000000);(189.385167,122.000000);(189.361244,122.000000);(189.337321,122.000000);(189.313397,122.000000);(189.289474,122.000000);(189.265550,122.000000);(189.241627,122.000000);(189.217703,122.000000);(189.193780,122.000000);(189.169856,122.000000);(189.145933,122.000000);(189.122010,122.000000);(189.098086,122.000000);(189.074163,122.000000);(189.050239,122.000000);(189.026316,122.000000);(189.002392,122.000000);(188.978469,122.000000);(188.954545,122.000000);(188.930622,122.000000);(188.906699,122.000000);(188.882775,122.000000);(188.858852,122.000000);(188.834928,122.000000);(188.811005,122.000000);(188.787081,122.000000);(188.763158,122.000000);(188.739234,122.000000);(188.715311,122.000000);(188.691388,122.000000);(188.667464,122.000000);(188.643541,122.000000);(188.619617,122.000000);(188.595694,122.000000);(188.571770,122.000000);(188.547847,122.000000);(188.523923,122.000000);(188.500000,122.000000);(188.476077,122.000000);(188.452153,122.000000);(188.428230,122.000000);(188.404306,122.000000);(188.380383,122.000000);(188.356459,122.000000);(188.332536,122.000000);(188.308612,122.000000);(188.284689,122.000000);(188.260766,122.000000);(188.236842,122.000000);(188.212919,122.000000);(188.188995,122.000000);(188.165072,122.000000);(188.141148,122.000000);(188.117225,122.000000);(188.093301,122.000000);(188.069378,122.000000);(188.045455,122.000000);(188.021531,122.000000);(187.997608,122.000000);(187.973684,122.000000);(187.949761,122.000000);(187.925837,122.000000);(187.901914,122.000000);(187.877990,122.000000);(187.854067,122.000000);(187.830144,122.000000);(187.806220,122.000000);(187.782297,122.000000);(187.758373,122.000000);(187.734450,122.000000);(187.710526,122.000000);(187.686603,122.000000);(187.662679,122.000000);(187.638756,122.000000);(187.614833,122.000000);(187.590909,122.000000);(187.566986,122.000000);(187.543062,122.000000);(187.519139,122.000000);(187.495215,122.000000);(187.471292,122.000000);(187.447368,122.000000);(187.423445,122.000000);(187.399522,122.000000);(187.375598,122.000000);(187.351675,122.000000);(187.327751,122.000000);(187.303828,122.000000);(187.279904,122.000000);(187.255981,122.000000);(187.232057,122.000000);(187.208134,122.000000);(187.184211,122.000000);(187.160287,122.000000);(187.136364,122.000000);(187.112440,122.000000);(187.088517,122.000000);(187.064593,122.000000);(187.040670,122.000000);(187.016746,122.000000);(186.992823,122.000000);(186.968900,122.000000);(186.944976,122.000000);(186.921053,122.000000);(186.897129,122.000000);(186.873206,122.000000);(186.849282,122.000000);(186.825359,122.000000);(186.801435,122.000000);(186.777512,122.000000);(186.753589,122.000000);(186.729665,122.000000);(186.705742,122.000000);(186.681818,122.000000);(186.657895,122.000000);(186.633971,122.000000);(186.610048,122.000000);(186.586124,122.000000);(186.562201,122.000000);(186.538278,122.000000);(186.514354,122.000000);(186.490431,122.000000);(186.466507,122.000000);(186.442584,122.000000);(186.418660,122.000000);(186.394737,122.000000);(186.370813,122.000000);(186.346890,122.000000);(186.322967,122.000000);(186.299043,122.000000);(186.275120,122.000000);(186.251196,122.000000);(186.227273,122.000000);(186.203349,122.000000);</t>
+    <t>190.964115_122.000000;190.940191_122.000000;190.916268_122.000000;190.892344_122.000000;190.868421_122.000000;190.844498_122.000000;190.820574_122.000000;190.796651_122.000000;190.772727_122.000000;190.748804_122.000000;190.724880_122.000000;190.700957_122.000000;190.677033_122.000000;190.653110_122.000000;190.629187_122.000000;190.605263_122.000000;190.581340_122.000000;190.557416_122.000000;190.533493_122.000000;190.509569_122.000000;190.485646_122.000000;190.461722_122.000000;190.437799_122.000000;190.413876_122.000000;190.389952_122.000000;190.366029_122.000000;190.342105_122.000000;190.318182_122.000000;190.294258_122.000000;190.270335_122.000000;190.246411_122.000000;190.222488_122.000000;190.198565_122.000000;190.174641_122.000000;190.150718_122.000000;190.126794_122.000000;190.102871_122.000000;190.078947_122.000000;190.055024_122.000000;190.031100_122.000000;190.007177_122.000000;189.983254_122.000000;189.959330_122.000000;189.935407_122.000000;189.911483_122.000000;189.887560_122.000000;189.863636_122.000000;189.839713_122.000000;189.815789_122.000000;189.791866_122.000000;189.767943_122.000000;189.744019_122.000000;189.720096_122.000000;189.696172_122.000000;189.672249_122.000000;189.648325_122.000000;189.624402_122.000000;189.600478_122.000000;189.576555_122.000000;189.552632_122.000000;189.528708_122.000000;189.504785_122.000000;189.480861_122.000000;189.456938_122.000000;189.433014_122.000000;189.409091_122.000000;189.385167_122.000000;189.361244_122.000000;189.337321_122.000000;189.313397_122.000000;189.289474_122.000000;189.265550_122.000000;189.241627_122.000000;189.217703_122.000000;189.193780_122.000000;189.169856_122.000000;189.145933_122.000000;189.122010_122.000000;189.098086_122.000000;189.074163_122.000000;189.050239_122.000000;189.026316_122.000000;189.002392_122.000000;188.978469_122.000000;188.954545_122.000000;188.930622_122.000000;188.906699_122.000000;188.882775_122.000000;188.858852_122.000000;188.834928_122.000000;188.811005_122.000000;188.787081_122.000000;188.763158_122.000000;188.739234_122.000000;188.715311_122.000000;188.691388_122.000000;188.667464_122.000000;188.643541_122.000000;188.619617_122.000000;188.595694_122.000000;188.571770_122.000000;188.547847_122.000000;188.523923_122.000000;188.500000_122.000000;188.476077_122.000000;188.452153_122.000000;188.428230_122.000000;188.404306_122.000000;188.380383_122.000000;188.356459_122.000000;188.332536_122.000000;188.308612_122.000000;188.284689_122.000000;188.260766_122.000000;188.236842_122.000000;188.212919_122.000000;188.188995_122.000000;188.165072_122.000000;188.141148_122.000000;188.117225_122.000000;188.093301_122.000000;188.069378_122.000000;188.045455_122.000000;188.021531_122.000000;187.997608_122.000000;187.973684_122.000000;187.949761_122.000000;187.925837_122.000000;187.901914_122.000000;187.877990_122.000000;187.854067_122.000000;187.830144_122.000000;187.806220_122.000000;187.782297_122.000000;187.758373_122.000000;187.734450_122.000000;187.710526_122.000000;187.686603_122.000000;187.662679_122.000000;187.638756_122.000000;187.614833_122.000000;187.590909_122.000000;187.566986_122.000000;187.543062_122.000000;187.519139_122.000000;187.495215_122.000000;187.471292_122.000000;187.447368_122.000000;187.423445_122.000000;187.399522_122.000000;187.375598_122.000000;187.351675_122.000000;187.327751_122.000000;187.303828_122.000000;187.279904_122.000000;187.255981_122.000000;187.232057_122.000000;187.208134_122.000000;187.184211_122.000000;187.160287_122.000000;187.136364_122.000000;187.112440_122.000000;187.088517_122.000000;187.064593_122.000000;187.040670_122.000000;187.016746_122.000000;186.992823_122.000000;186.968900_122.000000;186.944976_122.000000;186.921053_122.000000;186.897129_122.000000;186.873206_122.000000;186.849282_122.000000;186.825359_122.000000;186.801435_122.000000;186.777512_122.000000;186.753589_122.000000;186.729665_122.000000;186.705742_122.000000;186.681818_122.000000;186.657895_122.000000;186.633971_122.000000;186.610048_122.000000;186.586124_122.000000;186.562201_122.000000;186.538278_122.000000;186.514354_122.000000;186.490431_122.000000;186.466507_122.000000;186.442584_122.000000;186.418660_122.000000;186.394737_122.000000;186.370813_122.000000;186.346890_122.000000;186.322967_122.000000;186.299043_122.000000;186.275120_122.000000;186.251196_122.000000;186.227273_122.000000;186.203349_122.000000;</t>
   </si>
   <si>
-    <t>(185.923039,122.000129);(185.769116,122.000323);(185.615194,122.000400);(185.461271,122.000382);(185.307349,122.000293);(185.153426,122.000158);(184.999504,121.999999);(184.845581,121.999841);(184.691659,121.999706);(184.537736,121.999618);(184.383813,121.999601);(184.229891,121.999677);(184.075968,121.999872);(183.922046,122.000197);(183.768124,122.000603);(183.614202,122.000985);(183.460280,122.001224);(183.306357,122.001202);(183.152435,122.000804);(182.998515,121.999919);(182.844599,121.998581);(182.690684,121.997087);(182.536766,121.995875);(182.382845,121.995388);(182.228926,121.996079);(182.075025,121.998415);(181.921166,122.002690);(181.767345,122.008261);(181.613515,122.013553);(181.459637,122.016826);(181.305736,122.016428);(181.151951,122.010873);(180.998538,121.998990);(180.845645,121.981420);(180.692994,121.961694);(180.540043,121.944719);(180.386509,121.936005);(180.233135,121.942532);(180.083245,121.973076);(179.943836,122.034849);(179.820334,122.125164);(179.711598,122.233600);(179.612960,122.351620);(179.519606,122.473979);(179.427147,122.597033);(179.331289,122.717387);(179.227406,122.830661);(179.110582,122.929901);(178.977532,123.004625);(178.831096,123.047837);(178.678553,123.063280);(178.524893,123.059988);(178.371694,123.045770);(178.218968,123.026666);(178.066218,123.007786);(177.913001,122.993551);(177.759317,122.985832);(177.605435,122.983822);(177.451540,122.985997);(177.297690,122.990623);(177.143857,122.995852);(176.989991,122.999848);(176.836084,123.001576);(176.682164,123.001350);(176.528247,123.000085);(176.374331,122.998690);(176.220412,122.998070);(176.066498,122.999152);(175.912621,123.002603);(175.758789,123.007855);(175.604959,123.013157);(175.451084,123.016567);(175.297185,123.016233);(175.143411,123.010493);(174.990046,122.998071);(174.837242,122.979754);(174.684680,122.959347);(174.531779,122.941971);(174.378256,122.933413);(174.224992,122.941096);(174.075803,122.974313);(173.938345,123.040057);(173.817869,123.134390);(173.712367,123.246015);(173.616575,123.366381);(173.525372,123.490361);(173.434111,123.614297);(173.338135,123.734512);(173.232312,123.845819);(173.111396,123.939552);(172.973235,124.003294);(172.823287,124.031756);(172.669800,124.033710);(172.516424,124.021778);(172.363345,124.005737);(172.209949,123.994171);(172.056498,123.996955);(171.906176,124.024908);(171.764481,124.082349);(171.635389,124.164863);</t>
+    <t>185.923039_122.000129;185.769116_122.000323;185.615194_122.000400;185.461271_122.000382;185.307349_122.000293;185.153426_122.000158;184.999504_121.999999;184.845581_121.999841;184.691659_121.999706;184.537736_121.999618;184.383813_121.999601;184.229891_121.999677;184.075968_121.999872;183.922046_122.000197;183.768124_122.000603;183.614202_122.000985;183.460280_122.001224;183.306357_122.001202;183.152435_122.000804;182.998515_121.999919;182.844599_121.998581;182.690684_121.997087;182.536766_121.995875;182.382845_121.995388;182.228926_121.996079;182.075025_121.998415;181.921166_122.002690;181.767345_122.008261;181.613515_122.013553;181.459637_122.016826;181.305736_122.016428;181.151951_122.010873;180.998538_121.998990;180.845645_121.981420;180.692994_121.961694;180.540043_121.944719;180.386509_121.936005;180.233135_121.942532;180.083245_121.973076;179.943836_122.034849;179.820334_122.125164;179.711598_122.233600;179.612960_122.351620;179.519606_122.473979;179.427147_122.597033;179.331289_122.717387;179.227406_122.830661;179.110582_122.929901;178.977532_123.004625;178.831096_123.047837;178.678553_123.063280;178.524893_123.059988;178.371694_123.045770;178.218968_123.026666;178.066218_123.007786;177.913001_122.993551;177.759317_122.985832;177.605435_122.983822;177.451540_122.985997;177.297690_122.990623;177.143857_122.995852;176.989991_122.999848;176.836084_123.001576;176.682164_123.001350;176.528247_123.000085;176.374331_122.998690;176.220412_122.998070;176.066498_122.999152;175.912621_123.002603;175.758789_123.007855;175.604959_123.013157;175.451084_123.016567;175.297185_123.016233;175.143411_123.010493;174.990046_122.998071;174.837242_122.979754;174.684680_122.959347;174.531779_122.941971;174.378256_122.933413;174.224992_122.941096;174.075803_122.974313;173.938345_123.040057;173.817869_123.134390;173.712367_123.246015;173.616575_123.366381;173.525372_123.490361;173.434111_123.614297;173.338135_123.734512;173.232312_123.845819;173.111396_123.939552;172.973235_124.003294;172.823287_124.031756;172.669800_124.033710;172.516424_124.021778;172.363345_124.005737;172.209949_123.994171;172.056498_123.996955;171.906176_124.024908;171.764481_124.082349;171.635389_124.164863;</t>
   </si>
   <si>
-    <t>(171.635389,124.164863);(171.519522,124.265556);(171.415251,124.378478);(171.320188,124.499393);(171.231989,124.625473);(171.148589,124.754816);(171.068191,124.886065);(170.989184,125.018162);(170.910032,125.150172);(170.829166,125.281130);(170.744900,125.409903);(170.655332,125.535000);(170.558269,125.654284);(170.451253,125.764542);(170.331924,125.860974);(170.199073,125.937050);(170.054278,125.985859);(169.902466,126.004946);(169.748894,126.001338);(169.595734,125.986498);(169.442718,125.969935);(169.289242,125.960627);(169.136274,125.969651);(168.989728,126.010531);(168.858779,126.088095);(168.746357,126.192185);(168.647795,126.310126);(168.557044,126.434394);(168.468707,126.560442);(168.377731,126.684541);(168.278690,126.802063);(168.165527,126.905297);(168.033720,126.981232);(167.886480,127.018781);(167.733329,127.023100);(167.580140,127.009556);(167.427400,126.990574);(167.274238,126.976612);(167.121027,126.979968);(166.973409,127.016107);(166.841036,127.090918);(166.727508,127.193700);(166.628383,127.311136);(166.537513,127.435310);(166.449396,127.561511);(166.358927,127.685986);(166.260670,127.804183);(166.148534,127.908581);(166.017778,127.986441);(165.871264,128.027187);(165.718276,128.035531);(165.564846,128.025454);(165.411881,128.008409);(165.258716,127.993763);(165.105191,127.991774);(164.954245,128.015223);(164.812390,128.071378);(164.684601,128.155651);(164.570901,128.258789);(164.468339,128.373330);(164.373331,128.494354);(164.282580,128.618662);(164.193156,128.743942);(164.102329,128.868195);(164.007408,128.989298);(163.906553,129.105472);(163.799963,129.216443);(163.689106,129.323188);(163.575554,129.427088);(163.460910,129.529795);(163.346860,129.633154);(163.235258,129.739119);(163.128215,129.849631);(163.028138,129.966411);(162.937095,130.090324);(162.855383,130.220627);(162.781749,130.355708);(162.714640,130.494181);(162.652482,130.634971);(162.593749,130.777237);(162.536974,130.920304);(162.480742,131.063587);(162.423666,131.206533);(162.364364,131.348561);(162.301441,131.489008);(162.233483,131.627066);(162.159078,131.761728);(162.076882,131.891738);(161.985800,132.015641);(161.886009,132.132672);(161.779339,132.243545);(161.668046,132.349833);(161.554103,132.453306);(161.439281,132.555814);(161.325287,132.659232);(161.213905,132.765427);(161.107141,132.876209);(161.007297,132.993193);(160.916177,133.117068);(160.833903,133.247030);</t>
+    <t>171.635389_124.164863;171.519522_124.265556;171.415251_124.378478;171.320188_124.499393;171.231989_124.625473;171.148589_124.754816;171.068191_124.886065;170.989184_125.018162;170.910032_125.150172;170.829166_125.281130;170.744900_125.409903;170.655332_125.535000;170.558269_125.654284;170.451253_125.764542;170.331924_125.860974;170.199073_125.937050;170.054278_125.985859;169.902466_126.004946;169.748894_126.001338;169.595734_125.986498;169.442718_125.969935;169.289242_125.960627;169.136274_125.969651;168.989728_126.010531;168.858779_126.088095;168.746357_126.192185;168.647795_126.310126;168.557044_126.434394;168.468707_126.560442;168.377731_126.684541;168.278690_126.802063;168.165527_126.905297;168.033720_126.981232;167.886480_127.018781;167.733329_127.023100;167.580140_127.009556;167.427400_126.990574;167.274238_126.976612;167.121027_126.979968;166.973409_127.016107;166.841036_127.090918;166.727508_127.193700;166.628383_127.311136;166.537513_127.435310;166.449396_127.561511;166.358927_127.685986;166.260670_127.804183;166.148534_127.908581;166.017778_127.986441;165.871264_128.027187;165.718276_128.035531;165.564846_128.025454;165.411881_128.008409;165.258716_127.993763;165.105191_127.991774;164.954245_128.015223;164.812390_128.071378;164.684601_128.155651;164.570901_128.258789;164.468339_128.373330;164.373331_128.494354;164.282580_128.618662;164.193156_128.743942;164.102329_128.868195;164.007408_128.989298;163.906553_129.105472;163.799963_129.216443;163.689106_129.323188;163.575554_129.427088;163.460910_129.529795;163.346860_129.633154;163.235258_129.739119;163.128215_129.849631;163.028138_129.966411;162.937095_130.090324;162.855383_130.220627;162.781749_130.355708;162.714640_130.494181;162.652482_130.634971;162.593749_130.777237;162.536974_130.920304;162.480742_131.063587;162.423666_131.206533;162.364364_131.348561;162.301441_131.489008;162.233483_131.627066;162.159078_131.761728;162.076882_131.891738;161.985800_132.015641;161.886009_132.132672;161.779339_132.243545;161.668046_132.349833;161.554103_132.453306;161.439281_132.555814;161.325287_132.659232;161.213905_132.765427;161.107141_132.876209;161.007297_132.993193;160.916177_133.117068;160.833903_133.247030;</t>
   </si>
   <si>
-    <t>(160.833903,133.247030);(160.759388,133.381631);(160.691298,133.519625);(160.628222,133.660003);(160.568734,133.801954);(160.511429,133.944809);(160.454924,134.087985);(160.397845,134.230930);(160.338812,134.373073);(160.276428,134.513763);(160.209277,134.652220);(160.135946,134.787477);(160.055093,134.918336);(159.965699,135.043482);(159.868079,135.162354);(159.763893,135.275572);(159.654979,135.384290);(159.542945,135.489820);(159.429223,135.593543);(159.315132,135.696865);(159.201971,135.801195);(159.091092,135.907928);(158.983952,136.018382);(158.881668,136.133334);(158.784673,136.252783);(158.693055,136.376409);(158.606848,136.503870);(158.526030,136.634818);(158.450534,136.768908);(158.380253,136.905808);(158.315045,137.045200);(158.254745,137.186787);(158.199164,137.330295);(158.148102,137.475476);(158.101350,137.622105);(158.058695,137.769980);(158.019925,137.918923);(157.984829,138.068776);(157.953203,138.219401);(157.924847,138.370677);(157.899570,138.522500);(157.877188,138.674779);(157.857526,138.827433);(157.840418,138.980395);(157.825705,139.133607);(157.813236,139.287018);(157.802870,139.440586);(157.794470,139.594276);(157.787908,139.748055);(157.783063,139.901899);(157.779818,140.055785);(157.778064,140.209695);(157.777694,140.363615);(157.778608,140.517533);(157.780709,140.671440);(157.783906,140.825328);(157.788108,140.979192);(157.793230,141.133029);(157.799188,141.286836);(157.805900,141.440611);(157.813287,141.594356);(157.821271,141.748071);(157.829775,141.901758);(157.838723,142.055420);(157.848040,142.209061);(157.857650,142.362683);(157.867478,142.516292);(157.877446,142.669891);(157.887479,142.823486);(157.897497,142.977082);(157.907420,143.130684);(157.917164,143.284298);(157.926642,143.437929);(157.935766,143.591581);(157.944442,143.745258);(157.952570,143.898966);(157.960045,144.052706);(157.966757,144.206481);(157.972586,144.360293);(157.977403,144.514139);(157.981070,144.668017);(157.983436,144.821919);(157.984336,144.975836);(157.983589,145.129753);(157.980996,145.283649);(157.976333,145.437496);(157.969356,145.591255);(157.959787,145.744872);(157.947317,145.898278);(157.931597,146.051382);(157.912231,146.204064);(157.888774,146.356168);(157.860722,146.507488);(157.827507,146.657750);(157.788495,146.806600);(157.742983,146.953580);(157.690210,147.098097);(157.629382,147.239392);(157.559711,147.376514);(157.480483,147.508312);</t>
+    <t>160.833903_133.247030;160.759388_133.381631;160.691298_133.519625;160.628222_133.660003;160.568734_133.801954;160.511429_133.944809;160.454924_134.087985;160.397845_134.230930;160.338812_134.373073;160.276428_134.513763;160.209277_134.652220;160.135946_134.787477;160.055093_134.918336;159.965699_135.043482;159.868079_135.162354;159.763893_135.275572;159.654979_135.384290;159.542945_135.489820;159.429223_135.593543;159.315132_135.696865;159.201971_135.801195;159.091092_135.907928;158.983952_136.018382;158.881668_136.133334;158.784673_136.252783;158.693055_136.376409;158.606848_136.503870;158.526030_136.634818;158.450534_136.768908;158.380253_136.905808;158.315045_137.045200;158.254745_137.186787;158.199164_137.330295;158.148102_137.475476;158.101350_137.622105;158.058695_137.769980;158.019925_137.918923;157.984829_138.068776;157.953203_138.219401;157.924847_138.370677;157.899570_138.522500;157.877188_138.674779;157.857526_138.827433;157.840418_138.980395;157.825705_139.133607;157.813236_139.287018;157.802870_139.440586;157.794470_139.594276;157.787908_139.748055;157.783063_139.901899;157.779818_140.055785;157.778064_140.209695;157.777694_140.363615;157.778608_140.517533;157.780709_140.671440;157.783906_140.825328;157.788108_140.979192;157.793230_141.133029;157.799188_141.286836;157.805900_141.440611;157.813287_141.594356;157.821271_141.748071;157.829775_141.901758;157.838723_142.055420;157.848040_142.209061;157.857650_142.362683;157.867478_142.516292;157.877446_142.669891;157.887479_142.823486;157.897497_142.977082;157.907420_143.130684;157.917164_143.284298;157.926642_143.437929;157.935766_143.591581;157.944442_143.745258;157.952570_143.898966;157.960045_144.052706;157.966757_144.206481;157.972586_144.360293;157.977403_144.514139;157.981070_144.668017;157.983436_144.821919;157.984336_144.975836;157.983589_145.129753;157.980996_145.283649;157.976333_145.437496;157.969356_145.591255;157.959787_145.744872;157.947317_145.898278;157.931597_146.051382;157.912231_146.204064;157.888774_146.356168;157.860722_146.507488;157.827507_146.657750;157.788495_146.806600;157.742983_146.953580;157.690210_147.098097;157.629382_147.239392;157.559711_147.376514;157.480483_147.508312;</t>
   </si>
   <si>
-    <t>(157.000000,148.066753);(157.000000,148.200258);(157.000000,148.333764);(157.000000,148.467270);(157.000000,148.600775);(157.000000,148.734281);(157.000000,148.867786);(157.000000,149.001292);(157.000000,149.134798);(157.000000,149.268303);(157.000000,149.401809);(157.000000,149.535314);(157.000000,149.668820);(157.000000,149.802326);(157.000000,149.935831);(157.000000,150.069337);(157.000000,150.202842);(157.000000,150.336348);(157.000000,150.469854);(157.000000,150.603359);(157.000000,150.736865);(157.000000,150.870370);(157.000000,151.003876);(157.000000,151.137382);(157.000000,151.270887);(157.000000,151.404393);(157.000000,151.537898);(157.000000,151.671404);(157.000000,151.804910);(157.000000,151.938415);(157.000000,152.071921);(157.000000,152.205426);(157.000000,152.338932);(157.000000,152.472438);(157.000000,152.605943);(157.000000,152.739449);(157.000000,152.872954);(157.000000,153.006460);(157.000000,153.139966);(157.000000,153.273471);(157.000000,153.406977);(157.000000,153.540482);(157.000000,153.673988);(157.000000,153.807494);(157.000000,153.940999);(157.000000,154.074505);(157.000000,154.208010);(157.000000,154.341516);(157.000000,154.475022);(157.000000,154.608527);</t>
+    <t>157.000000_148.066753;157.000000_148.200258;157.000000_148.333764;157.000000_148.467270;157.000000_148.600775;157.000000_148.734281;157.000000_148.867786;157.000000_149.001292;157.000000_149.134798;157.000000_149.268303;157.000000_149.401809;157.000000_149.535314;157.000000_149.668820;157.000000_149.802326;157.000000_149.935831;157.000000_150.069337;157.000000_150.202842;157.000000_150.336348;157.000000_150.469854;157.000000_150.603359;157.000000_150.736865;157.000000_150.870370;157.000000_151.003876;157.000000_151.137382;157.000000_151.270887;157.000000_151.404393;157.000000_151.537898;157.000000_151.671404;157.000000_151.804910;157.000000_151.938415;157.000000_152.071921;157.000000_152.205426;157.000000_152.338932;157.000000_152.472438;157.000000_152.605943;157.000000_152.739449;157.000000_152.872954;157.000000_153.006460;157.000000_153.139966;157.000000_153.273471;157.000000_153.406977;157.000000_153.540482;157.000000_153.673988;157.000000_153.807494;157.000000_153.940999;157.000000_154.074505;157.000000_154.208010;157.000000_154.341516;157.000000_154.475022;157.000000_154.608527;</t>
   </si>
   <si>
-    <t>(157.000000,154.875538);(157.000000,155.009044);(157.000000,155.142550);(157.000000,155.276055);(157.000000,155.409561);(157.000000,155.543066);(157.000000,155.676572);(157.000000,155.810078);(157.000000,155.943583);(157.000000,156.077089);(157.000000,156.210594);(157.000000,156.344100);(157.000000,156.477606);(157.000000,156.611111);(157.000000,156.744617);(157.000000,156.878122);(157.000000,157.011628);(157.000000,157.145134);(157.000000,157.278639);(157.000000,157.412145);(157.000000,157.545650);(157.000000,157.679156);(157.000000,157.812661);(157.000000,157.946167);(157.000000,158.079673);(157.000000,158.213178);(157.000000,158.346684);(157.000000,158.480189);(157.000000,158.613695);(157.000000,158.747201);(157.000000,158.880706);(157.000000,159.014212);(157.000000,159.147717);(157.000000,159.281223);(157.000000,159.414729);(157.000000,159.548234);(157.000000,159.681740);(157.000000,159.815245);(157.000000,159.948751);(157.000000,160.082257);(157.000000,160.215762);(157.000000,160.349268);(157.000000,160.482773);(157.000000,160.616279);(157.000000,160.749785);(157.000000,160.883290);(157.000000,161.016796);(157.000000,161.150301);(157.000000,161.283807);(157.000000,161.417313);</t>
+    <t>157.000000_154.875538;157.000000_155.009044;157.000000_155.142550;157.000000_155.276055;157.000000_155.409561;157.000000_155.543066;157.000000_155.676572;157.000000_155.810078;157.000000_155.943583;157.000000_156.077089;157.000000_156.210594;157.000000_156.344100;157.000000_156.477606;157.000000_156.611111;157.000000_156.744617;157.000000_156.878122;157.000000_157.011628;157.000000_157.145134;157.000000_157.278639;157.000000_157.412145;157.000000_157.545650;157.000000_157.679156;157.000000_157.812661;157.000000_157.946167;157.000000_158.079673;157.000000_158.213178;157.000000_158.346684;157.000000_158.480189;157.000000_158.613695;157.000000_158.747201;157.000000_158.880706;157.000000_159.014212;157.000000_159.147717;157.000000_159.281223;157.000000_159.414729;157.000000_159.548234;157.000000_159.681740;157.000000_159.815245;157.000000_159.948751;157.000000_160.082257;157.000000_160.215762;157.000000_160.349268;157.000000_160.482773;157.000000_160.616279;157.000000_160.749785;157.000000_160.883290;157.000000_161.016796;157.000000_161.150301;157.000000_161.283807;157.000000_161.417313;</t>
   </si>
   <si>
-    <t>(157.000000,161.684324);(157.000000,161.817829);(157.000000,161.951335);(157.000000,162.084841);(157.000000,162.218346);(157.000000,162.351852);(157.000000,162.485357);(157.000000,162.618863);(157.000000,162.752369);(157.000000,162.885874);(157.000000,163.019380);(157.000000,163.152885);(157.000000,163.286391);(157.000000,163.419897);(157.000000,163.553402);(157.000000,163.686908);(157.000000,163.820413);(157.000000,163.953919);(157.000000,164.087425);(157.000000,164.220930);(157.000000,164.354436);(157.000000,164.487941);(157.000000,164.621447);(157.000000,164.754953);(157.000000,164.888458);(157.000000,165.021964);(157.000000,165.155469);(157.000000,165.288975);(157.000000,165.422481);(157.000000,165.555986);(157.000000,165.689492);(157.000000,165.822997);(157.000000,165.956503);(157.000000,166.090009);(157.000000,166.223514);(157.000000,166.357020);(157.000000,166.490525);(157.000000,166.624031);(157.000000,166.757537);(157.000000,166.891042);(157.000000,167.024548);(157.000000,167.158053);(157.000000,167.291559);(157.000000,167.425065);(157.000000,167.558570);(157.000000,167.692076);(157.000000,167.825581);(157.000000,167.959087);(157.000000,168.092593);(157.000000,168.226098);</t>
+    <t>157.000000_161.684324;157.000000_161.817829;157.000000_161.951335;157.000000_162.084841;157.000000_162.218346;157.000000_162.351852;157.000000_162.485357;157.000000_162.618863;157.000000_162.752369;157.000000_162.885874;157.000000_163.019380;157.000000_163.152885;157.000000_163.286391;157.000000_163.419897;157.000000_163.553402;157.000000_163.686908;157.000000_163.820413;157.000000_163.953919;157.000000_164.087425;157.000000_164.220930;157.000000_164.354436;157.000000_164.487941;157.000000_164.621447;157.000000_164.754953;157.000000_164.888458;157.000000_165.021964;157.000000_165.155469;157.000000_165.288975;157.000000_165.422481;157.000000_165.555986;157.000000_165.689492;157.000000_165.822997;157.000000_165.956503;157.000000_166.090009;157.000000_166.223514;157.000000_166.357020;157.000000_166.490525;157.000000_166.624031;157.000000_166.757537;157.000000_166.891042;157.000000_167.024548;157.000000_167.158053;157.000000_167.291559;157.000000_167.425065;157.000000_167.558570;157.000000_167.692076;157.000000_167.825581;157.000000_167.959087;157.000000_168.092593;157.000000_168.226098;</t>
   </si>
   <si>
-    <t>(157.000000,168.493109);(157.000000,168.626615);(157.000000,168.760121);(157.000000,168.893626);(157.000000,169.027132);(157.000000,169.160637);(157.000000,169.294143);(157.000000,169.427649);(157.000000,169.561154);(157.000000,169.694660);(157.000000,169.828165);(157.000000,169.961671);(157.000000,170.095177);(157.000000,170.228682);(157.000000,170.362188);(157.000000,170.495693);(157.000000,170.629199);(157.000000,170.762705);(157.000000,170.896210);(157.000000,171.029716);(157.000000,171.163221);(157.000000,171.296727);(157.000000,171.430233);(157.000000,171.563738);(157.000000,171.697244);(157.000000,171.830749);(157.000000,171.964255);(157.000000,172.097761);(157.000000,172.231266);(157.000000,172.364772);(157.000000,172.498277);(157.000000,172.631783);(157.000000,172.765289);(157.000000,172.898794);(157.000000,173.032300);(157.000000,173.165805);(157.000000,173.299311);(157.000000,173.432817);(157.000000,173.566322);(157.000000,173.699828);(157.000000,173.833333);(157.000000,173.966839);(157.000000,174.100345);(157.000000,174.233850);(157.000000,174.367356);(157.000000,174.500861);(157.000000,174.634367);(157.000000,174.767873);(157.000000,174.901378);(157.000000,175.034884);</t>
+    <t>157.000000_168.493109;157.000000_168.626615;157.000000_168.760121;157.000000_168.893626;157.000000_169.027132;157.000000_169.160637;157.000000_169.294143;157.000000_169.427649;157.000000_169.561154;157.000000_169.694660;157.000000_169.828165;157.000000_169.961671;157.000000_170.095177;157.000000_170.228682;157.000000_170.362188;157.000000_170.495693;157.000000_170.629199;157.000000_170.762705;157.000000_170.896210;157.000000_171.029716;157.000000_171.163221;157.000000_171.296727;157.000000_171.430233;157.000000_171.563738;157.000000_171.697244;157.000000_171.830749;157.000000_171.964255;157.000000_172.097761;157.000000_172.231266;157.000000_172.364772;157.000000_172.498277;157.000000_172.631783;157.000000_172.765289;157.000000_172.898794;157.000000_173.032300;157.000000_173.165805;157.000000_173.299311;157.000000_173.432817;157.000000_173.566322;157.000000_173.699828;157.000000_173.833333;157.000000_173.966839;157.000000_174.100345;157.000000_174.233850;157.000000_174.367356;157.000000_174.500861;157.000000_174.634367;157.000000_174.767873;157.000000_174.901378;157.000000_175.034884;</t>
   </si>
   <si>
-    <t>(157.000000,175.301895);(157.000000,175.435401);(157.000000,175.568906);(157.000000,175.702412);(157.000000,175.835917);(157.000000,175.969423);(157.000000,176.102929);(157.000000,176.236434);(157.000000,176.369940);(157.000000,176.503445);(157.000000,176.636951);(157.000000,176.770457);(157.000000,176.903962);(157.000000,177.037468);(157.000000,177.170973);(157.000000,177.304479);(157.000000,177.437984);(157.000000,177.571490);(157.000000,177.704996);(157.000000,177.838501);(157.000000,177.972007);(157.000000,178.105512);(157.000000,178.239018);(157.000000,178.372524);(157.000000,178.506029);(157.000000,178.639535);(157.000000,178.773040);(157.000000,178.906546);(157.000000,179.040052);(157.000000,179.173557);(157.000000,179.307063);(157.000000,179.440568);(157.000000,179.574074);(157.000000,179.707580);(157.000000,179.841085);(157.000000,179.974591);(157.000000,180.108096);(157.000000,180.241602);(157.000000,180.375108);(157.000000,180.508613);(157.000000,180.642119);(157.000000,180.775624);(157.000000,180.909130);(157.000000,181.042636);(157.000000,181.176141);(157.000000,181.309647);(157.000000,181.443152);(157.000000,181.576658);(157.000000,181.710164);(157.000000,181.843669);</t>
+    <t>157.000000_175.301895;157.000000_175.435401;157.000000_175.568906;157.000000_175.702412;157.000000_175.835917;157.000000_175.969423;157.000000_176.102929;157.000000_176.236434;157.000000_176.369940;157.000000_176.503445;157.000000_176.636951;157.000000_176.770457;157.000000_176.903962;157.000000_177.037468;157.000000_177.170973;157.000000_177.304479;157.000000_177.437984;157.000000_177.571490;157.000000_177.704996;157.000000_177.838501;157.000000_177.972007;157.000000_178.105512;157.000000_178.239018;157.000000_178.372524;157.000000_178.506029;157.000000_178.639535;157.000000_178.773040;157.000000_178.906546;157.000000_179.040052;157.000000_179.173557;157.000000_179.307063;157.000000_179.440568;157.000000_179.574074;157.000000_179.707580;157.000000_179.841085;157.000000_179.974591;157.000000_180.108096;157.000000_180.241602;157.000000_180.375108;157.000000_180.508613;157.000000_180.642119;157.000000_180.775624;157.000000_180.909130;157.000000_181.042636;157.000000_181.176141;157.000000_181.309647;157.000000_181.443152;157.000000_181.576658;157.000000_181.710164;157.000000_181.843669;</t>
   </si>
   <si>
-    <t>(157.000000,182.110680);(157.000000,182.244186);(157.000000,182.377692);(157.000000,182.511197);(157.000000,182.644703);(157.000000,182.778208);(157.000000,182.911714);(157.000000,183.045220);(157.000000,183.178725);(157.000000,183.312231);(157.000000,183.445736);(157.000000,183.579242);(157.000000,183.712748);(157.000000,183.846253);(157.000000,183.979759);(157.000000,184.113264);(157.000000,184.246770);(157.000000,184.380276);(157.000000,184.513781);(157.000000,184.647287);(157.000000,184.780792);(157.000000,184.914298);(157.000000,185.047804);(157.000000,185.181309);(157.000000,185.314815);(157.000000,185.448320);(157.000000,185.581826);(157.000000,185.715332);(157.000000,185.848837);(157.000000,185.982343);(157.000000,186.115848);(157.000000,186.249354);(157.000000,186.382860);(157.000000,186.516365);(157.000000,186.649871);(157.000000,186.783376);(157.000000,186.916882);(157.000000,187.050388);(157.000000,187.183893);(157.000000,187.317399);(157.000000,187.450904);(157.000000,187.584410);(157.000000,187.717916);(157.000000,187.851421);(157.000000,187.984927);(157.000000,188.118432);(157.000000,188.251938);(157.000000,188.385444);(157.000000,188.518949);(157.000000,188.652455);(157.000000,188.785960);(157.000000,188.919466);(157.000000,189.052972);(157.000000,189.186477);(157.000000,189.319983);(157.000000,189.453488);(157.000000,189.586994);(157.000000,189.720500);(157.000000,189.854005);(157.000000,189.987511);</t>
+    <t>157.000000_182.110680;157.000000_182.244186;157.000000_182.377692;157.000000_182.511197;157.000000_182.644703;157.000000_182.778208;157.000000_182.911714;157.000000_183.045220;157.000000_183.178725;157.000000_183.312231;157.000000_183.445736;157.000000_183.579242;157.000000_183.712748;157.000000_183.846253;157.000000_183.979759;157.000000_184.113264;157.000000_184.246770;157.000000_184.380276;157.000000_184.513781;157.000000_184.647287;157.000000_184.780792;157.000000_184.914298;157.000000_185.047804;157.000000_185.181309;157.000000_185.314815;157.000000_185.448320;157.000000_185.581826;157.000000_185.715332;157.000000_185.848837;157.000000_185.982343;157.000000_186.115848;157.000000_186.249354;157.000000_186.382860;157.000000_186.516365;157.000000_186.649871;157.000000_186.783376;157.000000_186.916882;157.000000_187.050388;157.000000_187.183893;157.000000_187.317399;157.000000_187.450904;157.000000_187.584410;157.000000_187.717916;157.000000_187.851421;157.000000_187.984927;157.000000_188.118432;157.000000_188.251938;157.000000_188.385444;157.000000_188.518949;157.000000_188.652455;157.000000_188.785960;157.000000_188.919466;157.000000_189.052972;157.000000_189.186477;157.000000_189.319983;157.000000_189.453488;157.000000_189.586994;157.000000_189.720500;157.000000_189.854005;157.000000_189.987511;</t>
   </si>
   <si>
-    <t>(157.000000,190.254522);(157.000000,190.388028);(157.000000,190.521533);(157.000000,190.655039);(157.000000,190.788544);(157.000000,190.922050);(157.000000,191.055556);(157.000000,191.189061);(157.000000,191.322567);(157.000000,191.456072);(157.000000,191.589578);(157.000000,191.723084);(157.000000,191.856589);(157.000000,191.990095);(157.000000,192.123600);(157.000000,192.257106);(157.000000,192.390612);(157.000000,192.524117);(157.000000,192.657623);(157.000000,192.791128);(157.000000,192.924634);(157.000000,193.058140);(157.000000,193.191645);(157.000000,193.325151);(157.000000,193.458656);(157.000000,193.592162);(157.000000,193.725668);(157.000000,193.859173);(157.000000,193.992679);(157.000000,194.126184);(157.000000,194.259690);(157.000000,194.393196);(157.000000,194.526701);(157.000000,194.660207);(157.000000,194.793712);(157.000000,194.927218);(157.000000,195.060724);(157.000000,195.194229);(157.000000,195.327735);(157.000000,195.461240);(157.000000,195.594746);(157.000000,195.728252);(157.000000,195.861757);(157.000000,195.995263);(157.000000,196.128768);(157.000000,196.262274);(157.000000,196.395780);(157.000000,196.529285);(157.000000,196.662791);(157.000000,196.796296);(157.000000,196.929802);(157.000000,197.063307);(157.000000,197.196813);(157.000000,197.330319);(157.000000,197.463824);(157.000000,197.597330);(157.000000,197.730835);(157.000000,197.864341);(157.000000,197.997847);(157.000000,198.131352);</t>
+    <t>157.000000_190.254522;157.000000_190.388028;157.000000_190.521533;157.000000_190.655039;157.000000_190.788544;157.000000_190.922050;157.000000_191.055556;157.000000_191.189061;157.000000_191.322567;157.000000_191.456072;157.000000_191.589578;157.000000_191.723084;157.000000_191.856589;157.000000_191.990095;157.000000_192.123600;157.000000_192.257106;157.000000_192.390612;157.000000_192.524117;157.000000_192.657623;157.000000_192.791128;157.000000_192.924634;157.000000_193.058140;157.000000_193.191645;157.000000_193.325151;157.000000_193.458656;157.000000_193.592162;157.000000_193.725668;157.000000_193.859173;157.000000_193.992679;157.000000_194.126184;157.000000_194.259690;157.000000_194.393196;157.000000_194.526701;157.000000_194.660207;157.000000_194.793712;157.000000_194.927218;157.000000_195.060724;157.000000_195.194229;157.000000_195.327735;157.000000_195.461240;157.000000_195.594746;157.000000_195.728252;157.000000_195.861757;157.000000_195.995263;157.000000_196.128768;157.000000_196.262274;157.000000_196.395780;157.000000_196.529285;157.000000_196.662791;157.000000_196.796296;157.000000_196.929802;157.000000_197.063307;157.000000_197.196813;157.000000_197.330319;157.000000_197.463824;157.000000_197.597330;157.000000_197.730835;157.000000_197.864341;157.000000_197.997847;157.000000_198.131352;</t>
   </si>
   <si>
-    <t>(157.000000,198.398363);(157.000000,198.531869);(157.000000,198.665375);(157.000000,198.798880);(157.000000,198.932386);(157.000000,199.065891);(157.000000,199.199397);(157.000000,199.332903);(157.000000,199.466408);(157.000000,199.599914);(157.000000,199.733419);(157.000000,199.866925);(157.000000,200.000431);(157.000000,200.133936);(157.000000,200.267442);(157.000000,200.400947);(157.000000,200.534453);(157.000000,200.667959);(157.000000,200.801464);(157.000000,200.934970);(157.000000,201.068475);(157.000000,201.201981);(157.000000,201.335487);(157.000000,201.468992);(157.000000,201.602498);(157.000000,201.736003);(157.000000,201.869509);(157.000000,202.003015);(157.000000,202.136520);(157.000000,202.270026);(157.000000,202.403531);(157.000000,202.537037);(157.000000,202.670543);(157.000000,202.804048);(157.000000,202.937554);(157.000000,203.071059);(157.000000,203.204565);(157.000000,203.338071);(157.000000,203.471576);(157.000000,203.605082);(157.000000,203.738587);(157.000000,203.872093);(157.000000,204.005599);(157.000000,204.139104);(157.000000,204.272610);(157.000000,204.406115);(157.000000,204.539621);(157.000000,204.673127);(157.000000,204.806632);(157.000000,204.940138);</t>
+    <t>157.000000_198.398363;157.000000_198.531869;157.000000_198.665375;157.000000_198.798880;157.000000_198.932386;157.000000_199.065891;157.000000_199.199397;157.000000_199.332903;157.000000_199.466408;157.000000_199.599914;157.000000_199.733419;157.000000_199.866925;157.000000_200.000431;157.000000_200.133936;157.000000_200.267442;157.000000_200.400947;157.000000_200.534453;157.000000_200.667959;157.000000_200.801464;157.000000_200.934970;157.000000_201.068475;157.000000_201.201981;157.000000_201.335487;157.000000_201.468992;157.000000_201.602498;157.000000_201.736003;157.000000_201.869509;157.000000_202.003015;157.000000_202.136520;157.000000_202.270026;157.000000_202.403531;157.000000_202.537037;157.000000_202.670543;157.000000_202.804048;157.000000_202.937554;157.000000_203.071059;157.000000_203.204565;157.000000_203.338071;157.000000_203.471576;157.000000_203.605082;157.000000_203.738587;157.000000_203.872093;157.000000_204.005599;157.000000_204.139104;157.000000_204.272610;157.000000_204.406115;157.000000_204.539621;157.000000_204.673127;157.000000_204.806632;157.000000_204.940138;</t>
   </si>
   <si>
-    <t>(157.000000,205.207149);(157.000000,205.340655);(157.000000,205.474160);(157.000000,205.607666);(157.000000,205.741171);(157.000000,205.874677);(157.000000,206.008183);(157.000000,206.141688);(157.000000,206.275194);(157.000000,206.408699);(157.000000,206.542205);(157.000000,206.675711);(157.000000,206.809216);(157.000000,206.942722);(157.000000,207.076227);(157.000000,207.209733);(157.000000,207.343239);(157.000000,207.476744);(157.000000,207.610250);(157.000000,207.743755);(157.000000,207.877261);(157.000000,208.010767);(157.000000,208.144272);(157.000000,208.277778);(157.000000,208.411283);(157.000000,208.544789);(157.000000,208.678295);(157.000000,208.811800);(157.000000,208.945306);(157.000000,209.078811);(157.000000,209.212317);(157.000000,209.345823);(157.000000,209.479328);(157.000000,209.612834);(157.000000,209.746339);(157.000000,209.879845);(157.000000,210.013351);(157.000000,210.146856);(157.000000,210.280362);(157.000000,210.413867);(157.000000,210.547373);(157.000000,210.680879);(157.000000,210.814384);(157.000000,210.947890);(157.000000,211.081395);(157.000000,211.214901);(157.000000,211.348407);(157.000000,211.481912);(157.000000,211.615418);(157.000000,211.748923);</t>
+    <t>157.000000_205.207149;157.000000_205.340655;157.000000_205.474160;157.000000_205.607666;157.000000_205.741171;157.000000_205.874677;157.000000_206.008183;157.000000_206.141688;157.000000_206.275194;157.000000_206.408699;157.000000_206.542205;157.000000_206.675711;157.000000_206.809216;157.000000_206.942722;157.000000_207.076227;157.000000_207.209733;157.000000_207.343239;157.000000_207.476744;157.000000_207.610250;157.000000_207.743755;157.000000_207.877261;157.000000_208.010767;157.000000_208.144272;157.000000_208.277778;157.000000_208.411283;157.000000_208.544789;157.000000_208.678295;157.000000_208.811800;157.000000_208.945306;157.000000_209.078811;157.000000_209.212317;157.000000_209.345823;157.000000_209.479328;157.000000_209.612834;157.000000_209.746339;157.000000_209.879845;157.000000_210.013351;157.000000_210.146856;157.000000_210.280362;157.000000_210.413867;157.000000_210.547373;157.000000_210.680879;157.000000_210.814384;157.000000_210.947890;157.000000_211.081395;157.000000_211.214901;157.000000_211.348407;157.000000_211.481912;157.000000_211.615418;157.000000_211.748923;</t>
   </si>
   <si>
-    <t>(157.000000,212.015935);(157.000000,212.149440);(157.000000,212.282946);(157.000000,212.416451);(157.000000,212.549957);(157.000000,212.683463);(157.000000,212.816968);(157.000000,212.950474);(157.000000,213.083979);(157.000000,213.217485);(157.000000,213.350991);(157.000000,213.484496);(157.000000,213.618002);(157.000000,213.751507);(157.000000,213.885013);(157.000000,214.018519);(157.000000,214.152024);(157.000000,214.285530);(157.000000,214.419035);(157.000000,214.552541);(157.000000,214.686047);(157.000000,214.819552);(157.000000,214.953058);(157.000000,215.086563);(157.000000,215.220069);(157.000000,215.353575);(157.000000,215.487080);(157.000000,215.620586);(157.000000,215.754091);(157.000000,215.887597);(157.000000,216.021102);(157.000000,216.154608);(157.000000,216.288114);(157.000000,216.421619);(157.000000,216.555125);(157.000000,216.688630);(157.000000,216.822136);(157.000000,216.955642);(157.000000,217.089147);(157.000000,217.222653);(157.000000,217.356158);(157.000000,217.489664);(157.000000,217.623170);(157.000000,217.756675);(157.000000,217.890181);(157.000000,218.023686);(157.000000,218.157192);(157.000000,218.290698);(157.000000,218.424203);(157.000000,218.557709);</t>
+    <t>157.000000_212.015935;157.000000_212.149440;157.000000_212.282946;157.000000_212.416451;157.000000_212.549957;157.000000_212.683463;157.000000_212.816968;157.000000_212.950474;157.000000_213.083979;157.000000_213.217485;157.000000_213.350991;157.000000_213.484496;157.000000_213.618002;157.000000_213.751507;157.000000_213.885013;157.000000_214.018519;157.000000_214.152024;157.000000_214.285530;157.000000_214.419035;157.000000_214.552541;157.000000_214.686047;157.000000_214.819552;157.000000_214.953058;157.000000_215.086563;157.000000_215.220069;157.000000_215.353575;157.000000_215.487080;157.000000_215.620586;157.000000_215.754091;157.000000_215.887597;157.000000_216.021102;157.000000_216.154608;157.000000_216.288114;157.000000_216.421619;157.000000_216.555125;157.000000_216.688630;157.000000_216.822136;157.000000_216.955642;157.000000_217.089147;157.000000_217.222653;157.000000_217.356158;157.000000_217.489664;157.000000_217.623170;157.000000_217.756675;157.000000_217.890181;157.000000_218.023686;157.000000_218.157192;157.000000_218.290698;157.000000_218.424203;157.000000_218.557709;</t>
   </si>
   <si>
-    <t>(157.000000,218.824720);(157.000000,218.958226);(157.000000,219.091731);(157.000000,219.225237);(157.000000,219.358742);(157.000000,219.492248);(157.000000,219.625754);(157.000000,219.759259);(157.000000,219.892765);(157.000000,220.026270);(157.000000,220.159776);(157.000000,220.293282);(157.000000,220.426787);(157.000000,220.560293);(157.000000,220.693798);(157.000000,220.827304);(157.000000,220.960810);(157.000000,221.094315);(157.000000,221.227821);(157.000000,221.361326);(157.000000,221.494832);(157.000000,221.628338);(157.000000,221.761843);(157.000000,221.895349);(157.000000,222.028854);(157.000000,222.162360);(157.000000,222.295866);(157.000000,222.429371);(157.000000,222.562877);(157.000000,222.696382);(157.000000,222.829888);(157.000000,222.963394);(157.000000,223.096899);(157.000000,223.230405);(157.000000,223.363910);(157.000000,223.497416);(157.000000,223.630922);(157.000000,223.764427);(157.000000,223.897933);(157.000000,224.031438);(157.000000,224.164944);(157.000000,224.298450);(157.000000,224.431955);(157.000000,224.565461);(157.000000,224.698966);(157.000000,224.832472);(157.000000,224.965978);(157.000000,225.099483);(157.000000,225.232989);(157.000000,225.366494);</t>
+    <t>157.000000_218.824720;157.000000_218.958226;157.000000_219.091731;157.000000_219.225237;157.000000_219.358742;157.000000_219.492248;157.000000_219.625754;157.000000_219.759259;157.000000_219.892765;157.000000_220.026270;157.000000_220.159776;157.000000_220.293282;157.000000_220.426787;157.000000_220.560293;157.000000_220.693798;157.000000_220.827304;157.000000_220.960810;157.000000_221.094315;157.000000_221.227821;157.000000_221.361326;157.000000_221.494832;157.000000_221.628338;157.000000_221.761843;157.000000_221.895349;157.000000_222.028854;157.000000_222.162360;157.000000_222.295866;157.000000_222.429371;157.000000_222.562877;157.000000_222.696382;157.000000_222.829888;157.000000_222.963394;157.000000_223.096899;157.000000_223.230405;157.000000_223.363910;157.000000_223.497416;157.000000_223.630922;157.000000_223.764427;157.000000_223.897933;157.000000_224.031438;157.000000_224.164944;157.000000_224.298450;157.000000_224.431955;157.000000_224.565461;157.000000_224.698966;157.000000_224.832472;157.000000_224.965978;157.000000_225.099483;157.000000_225.232989;157.000000_225.366494;</t>
   </si>
   <si>
-    <t>(157.000000,225.633506);(157.000000,225.767011);(157.000000,225.900517);(157.000000,226.034022);(157.000000,226.167528);(157.000000,226.301034);(157.000000,226.434539);(157.000000,226.568045);(157.000000,226.701550);(157.000000,226.835056);(157.000000,226.968562);(157.000000,227.102067);(157.000000,227.235573);(157.000000,227.369078);(157.000000,227.502584);(157.000000,227.636090);(157.000000,227.769595);(157.000000,227.903101);(157.000000,228.036606);(157.000000,228.170112);(157.000000,228.303618);(157.000000,228.437123);(157.000000,228.570629);(157.000000,228.704134);(157.000000,228.837640);(157.000000,228.971146);(157.000000,229.104651);(157.000000,229.238157);(157.000000,229.371662);(157.000000,229.505168);(157.000000,229.638674);(157.000000,229.772179);(157.000000,229.905685);(157.000000,230.039190);(157.000000,230.172696);(157.000000,230.306202);(157.000000,230.439707);(157.000000,230.573213);(157.000000,230.706718);(157.000000,230.840224);(157.000000,230.973730);(157.000000,231.107235);(157.000000,231.240741);(157.000000,231.374246);(157.000000,231.507752);(157.000000,231.641258);(157.000000,231.774763);(157.000000,231.908269);(157.000000,232.041774);(157.000000,232.175280);</t>
+    <t>157.000000_225.633506;157.000000_225.767011;157.000000_225.900517;157.000000_226.034022;157.000000_226.167528;157.000000_226.301034;157.000000_226.434539;157.000000_226.568045;157.000000_226.701550;157.000000_226.835056;157.000000_226.968562;157.000000_227.102067;157.000000_227.235573;157.000000_227.369078;157.000000_227.502584;157.000000_227.636090;157.000000_227.769595;157.000000_227.903101;157.000000_228.036606;157.000000_228.170112;157.000000_228.303618;157.000000_228.437123;157.000000_228.570629;157.000000_228.704134;157.000000_228.837640;157.000000_228.971146;157.000000_229.104651;157.000000_229.238157;157.000000_229.371662;157.000000_229.505168;157.000000_229.638674;157.000000_229.772179;157.000000_229.905685;157.000000_230.039190;157.000000_230.172696;157.000000_230.306202;157.000000_230.439707;157.000000_230.573213;157.000000_230.706718;157.000000_230.840224;157.000000_230.973730;157.000000_231.107235;157.000000_231.240741;157.000000_231.374246;157.000000_231.507752;157.000000_231.641258;157.000000_231.774763;157.000000_231.908269;157.000000_232.041774;157.000000_232.175280;</t>
   </si>
   <si>
-    <t>(157.000000,232.442291);(157.000000,232.575797);(157.000000,232.709302);(157.000000,232.842808);(157.000000,232.976314);(157.000000,233.109819);(157.000000,233.243325);(157.000000,233.376830);(157.000000,233.510336);(157.000000,233.643842);(157.000000,233.777347);(157.000000,233.910853);(157.000000,234.044358);(157.000000,234.177864);(157.000000,234.311370);(157.000000,234.444875);(157.000000,234.578381);(157.000000,234.711886);(157.000000,234.845392);(157.000000,234.978898);(157.000000,235.112403);(157.000000,235.245909);(157.000000,235.379414);(157.000000,235.512920);(157.000000,235.646425);(157.000000,235.779931);(157.000000,235.913437);(157.000000,236.046942);(157.000000,236.180448);(157.000000,236.313953);(157.000000,236.447459);(157.000000,236.580965);(157.000000,236.714470);(157.000000,236.847976);(157.000000,236.981481);(157.000000,237.114987);(157.000000,237.248493);(157.000000,237.381998);(157.000000,237.515504);(157.000000,237.649009);(157.000000,237.782515);(157.000000,237.916021);(157.000000,238.049526);(157.000000,238.183032);(157.000000,238.316537);(157.000000,238.450043);(157.000000,238.583549);(157.000000,238.717054);(157.000000,238.850560);(157.000000,238.984065);</t>
+    <t>157.000000_232.442291;157.000000_232.575797;157.000000_232.709302;157.000000_232.842808;157.000000_232.976314;157.000000_233.109819;157.000000_233.243325;157.000000_233.376830;157.000000_233.510336;157.000000_233.643842;157.000000_233.777347;157.000000_233.910853;157.000000_234.044358;157.000000_234.177864;157.000000_234.311370;157.000000_234.444875;157.000000_234.578381;157.000000_234.711886;157.000000_234.845392;157.000000_234.978898;157.000000_235.112403;157.000000_235.245909;157.000000_235.379414;157.000000_235.512920;157.000000_235.646425;157.000000_235.779931;157.000000_235.913437;157.000000_236.046942;157.000000_236.180448;157.000000_236.313953;157.000000_236.447459;157.000000_236.580965;157.000000_236.714470;157.000000_236.847976;157.000000_236.981481;157.000000_237.114987;157.000000_237.248493;157.000000_237.381998;157.000000_237.515504;157.000000_237.649009;157.000000_237.782515;157.000000_237.916021;157.000000_238.049526;157.000000_238.183032;157.000000_238.316537;157.000000_238.450043;157.000000_238.583549;157.000000_238.717054;157.000000_238.850560;157.000000_238.984065;</t>
   </si>
   <si>
-    <t>(157.000000,239.251077);(157.000000,239.384582);(157.000000,239.518088);(157.000000,239.651593);(157.000000,239.785099);(157.000000,239.918605);(157.000000,240.052110);(157.000000,240.185616);(157.000000,240.319121);(157.000000,240.452627);(157.000000,240.586133);(157.000000,240.719638);(157.000000,240.853144);(157.000000,240.986649);(157.000000,241.120155);(157.000000,241.253661);(157.000000,241.387166);(157.000000,241.520672);(157.000000,241.654177);(157.000000,241.787683);(157.000000,241.921189);(157.000000,242.054694);(157.000000,242.188200);(157.000000,242.321705);(157.000000,242.455211);(157.000000,242.588717);(157.000000,242.722222);(157.000000,242.855728);(157.000000,242.989233);(157.000000,243.122739);(157.000000,243.256245);(157.000000,243.389750);(157.000000,243.523256);(157.000000,243.656761);(157.000000,243.790267);(157.000000,243.923773);(157.000000,244.057278);(157.000000,244.190784);(157.000000,244.324289);(157.000000,244.457795);(157.000000,244.591301);(157.000000,244.724806);(157.000000,244.858312);(157.000000,244.991817);(157.000000,245.125323);(157.000000,245.258829);(157.000000,245.392334);(157.000000,245.525840);(157.000000,245.659345);(157.000000,245.792851);</t>
+    <t>157.000000_239.251077;157.000000_239.384582;157.000000_239.518088;157.000000_239.651593;157.000000_239.785099;157.000000_239.918605;157.000000_240.052110;157.000000_240.185616;157.000000_240.319121;157.000000_240.452627;157.000000_240.586133;157.000000_240.719638;157.000000_240.853144;157.000000_240.986649;157.000000_241.120155;157.000000_241.253661;157.000000_241.387166;157.000000_241.520672;157.000000_241.654177;157.000000_241.787683;157.000000_241.921189;157.000000_242.054694;157.000000_242.188200;157.000000_242.321705;157.000000_242.455211;157.000000_242.588717;157.000000_242.722222;157.000000_242.855728;157.000000_242.989233;157.000000_243.122739;157.000000_243.256245;157.000000_243.389750;157.000000_243.523256;157.000000_243.656761;157.000000_243.790267;157.000000_243.923773;157.000000_244.057278;157.000000_244.190784;157.000000_244.324289;157.000000_244.457795;157.000000_244.591301;157.000000_244.724806;157.000000_244.858312;157.000000_244.991817;157.000000_245.125323;157.000000_245.258829;157.000000_245.392334;157.000000_245.525840;157.000000_245.659345;157.000000_245.792851;</t>
   </si>
   <si>
-    <t>(157.000000,246.059862);(157.000000,246.193368);(157.000000,246.326873);(157.000000,246.460379);(157.000000,246.593885);(157.000000,246.727390);(157.000000,246.860896);(157.000000,246.994401);(157.000000,247.127907);(157.000000,247.261413);(157.000000,247.394918);(157.000000,247.528424);(157.000000,247.661929);(157.000000,247.795435);(157.000000,247.928941);(157.000000,248.062446);(157.000000,248.195952);(157.000000,248.329457);(157.000000,248.462963);(157.000000,248.596469);(157.000000,248.729974);(157.000000,248.863480);(157.000000,248.996985);(157.000000,249.130491);(157.000000,249.263997);(157.000000,249.397502);(157.000000,249.531008);(157.000000,249.664513);(157.000000,249.798019);(157.000000,249.931525);(157.000000,250.065030);(157.000000,250.198536);(157.000000,250.332041);(157.000000,250.465547);(157.000000,250.599053);(157.000000,250.732558);(157.000000,250.866064);(157.000000,250.999569);(157.000000,251.133075);(157.000000,251.266581);(157.000000,251.400086);(157.000000,251.533592);(157.000000,251.667097);(157.000000,251.800603);(157.000000,251.934109);(157.000000,252.067614);(157.000000,252.201120);(157.000000,252.334625);(157.000000,252.468131);(157.000000,252.601637);</t>
+    <t>157.000000_246.059862;157.000000_246.193368;157.000000_246.326873;157.000000_246.460379;157.000000_246.593885;157.000000_246.727390;157.000000_246.860896;157.000000_246.994401;157.000000_247.127907;157.000000_247.261413;157.000000_247.394918;157.000000_247.528424;157.000000_247.661929;157.000000_247.795435;157.000000_247.928941;157.000000_248.062446;157.000000_248.195952;157.000000_248.329457;157.000000_248.462963;157.000000_248.596469;157.000000_248.729974;157.000000_248.863480;157.000000_248.996985;157.000000_249.130491;157.000000_249.263997;157.000000_249.397502;157.000000_249.531008;157.000000_249.664513;157.000000_249.798019;157.000000_249.931525;157.000000_250.065030;157.000000_250.198536;157.000000_250.332041;157.000000_250.465547;157.000000_250.599053;157.000000_250.732558;157.000000_250.866064;157.000000_250.999569;157.000000_251.133075;157.000000_251.266581;157.000000_251.400086;157.000000_251.533592;157.000000_251.667097;157.000000_251.800603;157.000000_251.934109;157.000000_252.067614;157.000000_252.201120;157.000000_252.334625;157.000000_252.468131;157.000000_252.601637;</t>
   </si>
   <si>
-    <t>(157.000000,252.868648);(157.000000,253.002153);(157.000000,253.135659);(157.000000,253.269165);(157.000000,253.402670);(157.000000,253.536176);(157.000000,253.669681);(157.000000,253.803187);(157.000000,253.936693);(157.000000,254.070198);(157.000000,254.203704);(157.000000,254.337209);(157.000000,254.470715);(157.000000,254.604220);(157.000000,254.737726);(157.000000,254.871232);(157.000000,255.004737);(157.000000,255.138243);(157.000000,255.271748);(157.000000,255.405254);(157.000000,255.538760);(157.000000,255.672265);(157.000000,255.805771);(157.000000,255.939276);(157.000000,256.072782);(157.000000,256.206288);(157.000000,256.339793);(157.000000,256.473299);(157.000000,256.606804);(157.000000,256.740310);(157.000000,256.873816);(157.000000,257.007321);(157.000000,257.140827);(157.000000,257.274332);(157.000000,257.407838);(157.000000,257.541344);(157.000000,257.674849);(157.000000,257.808355);(157.000000,257.941860);(157.000000,258.075366);(157.000000,258.208872);(157.000000,258.342377);(157.000000,258.475883);(157.000000,258.609388);(157.000000,258.742894);(157.000000,258.876400);(157.000000,259.009905);(157.000000,259.143411);(157.000000,259.276916);(157.000000,259.410422);</t>
+    <t>157.000000_252.868648;157.000000_253.002153;157.000000_253.135659;157.000000_253.269165;157.000000_253.402670;157.000000_253.536176;157.000000_253.669681;157.000000_253.803187;157.000000_253.936693;157.000000_254.070198;157.000000_254.203704;157.000000_254.337209;157.000000_254.470715;157.000000_254.604220;157.000000_254.737726;157.000000_254.871232;157.000000_255.004737;157.000000_255.138243;157.000000_255.271748;157.000000_255.405254;157.000000_255.538760;157.000000_255.672265;157.000000_255.805771;157.000000_255.939276;157.000000_256.072782;157.000000_256.206288;157.000000_256.339793;157.000000_256.473299;157.000000_256.606804;157.000000_256.740310;157.000000_256.873816;157.000000_257.007321;157.000000_257.140827;157.000000_257.274332;157.000000_257.407838;157.000000_257.541344;157.000000_257.674849;157.000000_257.808355;157.000000_257.941860;157.000000_258.075366;157.000000_258.208872;157.000000_258.342377;157.000000_258.475883;157.000000_258.609388;157.000000_258.742894;157.000000_258.876400;157.000000_259.009905;157.000000_259.143411;157.000000_259.276916;157.000000_259.410422;</t>
   </si>
   <si>
-    <t>(157.000000,259.677433);(157.000000,259.810939);(157.000000,259.944444);(157.000000,260.077950);(157.000000,260.211456);(157.000000,260.344961);(157.000000,260.478467);(157.000000,260.611972);(157.000000,260.745478);(157.000000,260.878984);(157.000000,261.012489);(157.000000,261.145995);(157.000000,261.279500);(157.000000,261.413006);(157.000000,261.546512);(157.000000,261.680017);(157.000000,261.813523);(157.000000,261.947028);(157.000000,262.080534);(157.000000,262.214040);(157.000000,262.347545);(157.000000,262.481051);(157.000000,262.614556);(157.000000,262.748062);(157.000000,262.881568);(157.000000,263.015073);(157.000000,263.148579);(157.000000,263.282084);(157.000000,263.415590);(157.000000,263.549096);(157.000000,263.682601);(157.000000,263.816107);(157.000000,263.949612);(157.000000,264.083118);(157.000000,264.216624);(157.000000,264.350129);(157.000000,264.483635);(157.000000,264.617140);(157.000000,264.750646);(157.000000,264.884152);(157.000000,265.017657);(157.000000,265.151163);(157.000000,265.284668);(157.000000,265.418174);(157.000000,265.551680);(157.000000,265.685185);(157.000000,265.818691);(157.000000,265.952196);(157.000000,266.085702);(157.000000,266.219208);(157.000000,266.352713);(157.000000,266.486219);(157.000000,266.619724);(157.000000,266.753230);(157.000000,266.886736);(157.000000,267.020241);(157.000000,267.153747);(157.000000,267.287252);(157.000000,267.420758);(157.000000,267.554264);</t>
+    <t>157.000000_259.677433;157.000000_259.810939;157.000000_259.944444;157.000000_260.077950;157.000000_260.211456;157.000000_260.344961;157.000000_260.478467;157.000000_260.611972;157.000000_260.745478;157.000000_260.878984;157.000000_261.012489;157.000000_261.145995;157.000000_261.279500;157.000000_261.413006;157.000000_261.546512;157.000000_261.680017;157.000000_261.813523;157.000000_261.947028;157.000000_262.080534;157.000000_262.214040;157.000000_262.347545;157.000000_262.481051;157.000000_262.614556;157.000000_262.748062;157.000000_262.881568;157.000000_263.015073;157.000000_263.148579;157.000000_263.282084;157.000000_263.415590;157.000000_263.549096;157.000000_263.682601;157.000000_263.816107;157.000000_263.949612;157.000000_264.083118;157.000000_264.216624;157.000000_264.350129;157.000000_264.483635;157.000000_264.617140;157.000000_264.750646;157.000000_264.884152;157.000000_265.017657;157.000000_265.151163;157.000000_265.284668;157.000000_265.418174;157.000000_265.551680;157.000000_265.685185;157.000000_265.818691;157.000000_265.952196;157.000000_266.085702;157.000000_266.219208;157.000000_266.352713;157.000000_266.486219;157.000000_266.619724;157.000000_266.753230;157.000000_266.886736;157.000000_267.020241;157.000000_267.153747;157.000000_267.287252;157.000000_267.420758;157.000000_267.554264;</t>
   </si>
   <si>
-    <t>(157.000000,267.821275);(157.000000,267.954780);(157.000000,268.088286);(157.000000,268.221792);(157.000000,268.355297);(157.000000,268.488803);(157.000000,268.622308);(157.000000,268.755814);(157.000000,268.889320);(157.000000,269.022825);(157.000000,269.156331);(157.000000,269.289836);(157.000000,269.423342);(157.000000,269.556848);(157.000000,269.690353);(157.000000,269.823859);(157.000000,269.957364);(157.000000,270.090870);(157.000000,270.224376);(157.000000,270.357881);(157.000000,270.491387);(157.000000,270.624892);(157.000000,270.758398);(157.000000,270.891904);(157.000000,271.025409);(157.000000,271.158915);(157.000000,271.292420);(157.000000,271.425926);(157.000000,271.559432);(157.000000,271.692937);(157.000000,271.826443);(157.000000,271.959948);(157.000000,272.093454);(157.000000,272.226960);(157.000000,272.360465);(157.000000,272.493971);(157.000000,272.627476);(157.000000,272.760982);(157.000000,272.894488);(157.000000,273.027993);(157.000000,273.161499);(157.000000,273.295004);(157.000000,273.428510);(157.000000,273.562016);(157.000000,273.695521);(157.000000,273.829027);(157.000000,273.962532);(157.000000,274.096038);(157.000000,274.229543);(157.000000,274.363049);(157.000000,274.496555);(157.000000,274.630060);(157.000000,274.763566);(157.000000,274.897071);(157.000000,275.030577);(157.000000,275.164083);(157.000000,275.297588);(157.000000,275.431094);(157.000000,275.564599);(157.000000,275.698105);</t>
+    <t>157.000000_267.821275;157.000000_267.954780;157.000000_268.088286;157.000000_268.221792;157.000000_268.355297;157.000000_268.488803;157.000000_268.622308;157.000000_268.755814;157.000000_268.889320;157.000000_269.022825;157.000000_269.156331;157.000000_269.289836;157.000000_269.423342;157.000000_269.556848;157.000000_269.690353;157.000000_269.823859;157.000000_269.957364;157.000000_270.090870;157.000000_270.224376;157.000000_270.357881;157.000000_270.491387;157.000000_270.624892;157.000000_270.758398;157.000000_270.891904;157.000000_271.025409;157.000000_271.158915;157.000000_271.292420;157.000000_271.425926;157.000000_271.559432;157.000000_271.692937;157.000000_271.826443;157.000000_271.959948;157.000000_272.093454;157.000000_272.226960;157.000000_272.360465;157.000000_272.493971;157.000000_272.627476;157.000000_272.760982;157.000000_272.894488;157.000000_273.027993;157.000000_273.161499;157.000000_273.295004;157.000000_273.428510;157.000000_273.562016;157.000000_273.695521;157.000000_273.829027;157.000000_273.962532;157.000000_274.096038;157.000000_274.229543;157.000000_274.363049;157.000000_274.496555;157.000000_274.630060;157.000000_274.763566;157.000000_274.897071;157.000000_275.030577;157.000000_275.164083;157.000000_275.297588;157.000000_275.431094;157.000000_275.564599;157.000000_275.698105;</t>
   </si>
   <si>
-    <t>(157.000000,275.965116);(157.000000,276.098622);(157.000000,276.232127);(157.000000,276.365633);(157.000000,276.499139);(157.000000,276.632644);(157.000000,276.766150);(157.000000,276.899655);(157.000000,277.033161);(157.000000,277.166667);(157.000000,277.300172);(157.000000,277.433678);(157.000000,277.567183);(157.000000,277.700689);(157.000000,277.834195);(157.000000,277.967700);(157.000000,278.101206);(157.000000,278.234711);(157.000000,278.368217);(157.000000,278.501723);(157.000000,278.635228);(157.000000,278.768734);(157.000000,278.902239);(157.000000,279.035745);(157.000000,279.169251);(157.000000,279.302756);(157.000000,279.436262);(157.000000,279.569767);(157.000000,279.703273);(157.000000,279.836779);(157.000000,279.970284);(157.000000,280.103790);(157.000000,280.237295);(157.000000,280.370801);(157.000000,280.504307);(157.000000,280.637812);(157.000000,280.771318);(157.000000,280.904823);(157.000000,281.038329);(157.000000,281.171835);(157.000000,281.305340);(157.000000,281.438846);(157.000000,281.572351);(157.000000,281.705857);(157.000000,281.839363);(157.000000,281.972868);(157.000000,282.106374);(157.000000,282.239879);(157.000000,282.373385);(157.000000,282.506891);</t>
+    <t>157.000000_275.965116;157.000000_276.098622;157.000000_276.232127;157.000000_276.365633;157.000000_276.499139;157.000000_276.632644;157.000000_276.766150;157.000000_276.899655;157.000000_277.033161;157.000000_277.166667;157.000000_277.300172;157.000000_277.433678;157.000000_277.567183;157.000000_277.700689;157.000000_277.834195;157.000000_277.967700;157.000000_278.101206;157.000000_278.234711;157.000000_278.368217;157.000000_278.501723;157.000000_278.635228;157.000000_278.768734;157.000000_278.902239;157.000000_279.035745;157.000000_279.169251;157.000000_279.302756;157.000000_279.436262;157.000000_279.569767;157.000000_279.703273;157.000000_279.836779;157.000000_279.970284;157.000000_280.103790;157.000000_280.237295;157.000000_280.370801;157.000000_280.504307;157.000000_280.637812;157.000000_280.771318;157.000000_280.904823;157.000000_281.038329;157.000000_281.171835;157.000000_281.305340;157.000000_281.438846;157.000000_281.572351;157.000000_281.705857;157.000000_281.839363;157.000000_281.972868;157.000000_282.106374;157.000000_282.239879;157.000000_282.373385;157.000000_282.506891;</t>
   </si>
   <si>
-    <t>(157.000000,282.773902);(157.000000,282.907407);(157.000000,283.040913);(157.000000,283.174419);(157.000000,283.307924);(157.000000,283.441430);(157.000000,283.574935);(157.000000,283.708441);(157.000000,283.841947);(157.000000,283.975452);(157.000000,284.108958);(157.000000,284.242463);(157.000000,284.375969);(157.000000,284.509475);(157.000000,284.642980);(157.000000,284.776486);(157.000000,284.909991);(157.000000,285.043497);(157.000000,285.177003);(157.000000,285.310508);(157.000000,285.444014);(157.000000,285.577519);(157.000000,285.711025);(157.000000,285.844531);(157.000000,285.978036);(157.000000,286.111542);(157.000000,286.245047);(157.000000,286.378553);(157.000000,286.512059);(157.000000,286.645564);(157.000000,286.779070);(157.000000,286.912575);(157.000000,287.046081);(157.000000,287.179587);(157.000000,287.313092);(157.000000,287.446598);(157.000000,287.580103);(157.000000,287.713609);(157.000000,287.847115);(157.000000,287.980620);(157.000000,288.114126);(157.000000,288.247631);(157.000000,288.381137);(157.000000,288.514643);(157.000000,288.648148);(157.000000,288.781654);(157.000000,288.915159);(157.000000,289.048665);(157.000000,289.182171);(157.000000,289.315676);</t>
+    <t>157.000000_282.773902;157.000000_282.907407;157.000000_283.040913;157.000000_283.174419;157.000000_283.307924;157.000000_283.441430;157.000000_283.574935;157.000000_283.708441;157.000000_283.841947;157.000000_283.975452;157.000000_284.108958;157.000000_284.242463;157.000000_284.375969;157.000000_284.509475;157.000000_284.642980;157.000000_284.776486;157.000000_284.909991;157.000000_285.043497;157.000000_285.177003;157.000000_285.310508;157.000000_285.444014;157.000000_285.577519;157.000000_285.711025;157.000000_285.844531;157.000000_285.978036;157.000000_286.111542;157.000000_286.245047;157.000000_286.378553;157.000000_286.512059;157.000000_286.645564;157.000000_286.779070;157.000000_286.912575;157.000000_287.046081;157.000000_287.179587;157.000000_287.313092;157.000000_287.446598;157.000000_287.580103;157.000000_287.713609;157.000000_287.847115;157.000000_287.980620;157.000000_288.114126;157.000000_288.247631;157.000000_288.381137;157.000000_288.514643;157.000000_288.648148;157.000000_288.781654;157.000000_288.915159;157.000000_289.048665;157.000000_289.182171;157.000000_289.315676;</t>
   </si>
   <si>
-    <t>(157.000000,289.582687);(157.000000,289.716193);(157.000000,289.849699);(157.000000,289.983204);(157.000000,290.116710);(157.000000,290.250215);(157.000000,290.383721);(157.000000,290.517227);(157.000000,290.650732);(157.000000,290.784238);(157.000000,290.917743);(157.000000,291.051249);(157.000000,291.184755);(157.000000,291.318260);(157.000000,291.451766);(157.000000,291.585271);(157.000000,291.718777);(157.000000,291.852283);(157.000000,291.985788);(157.000000,292.119294);(157.000000,292.252799);(157.000000,292.386305);(157.000000,292.519811);(157.000000,292.653316);(157.000000,292.786822);(157.000000,292.920327);(157.000000,293.053833);(157.000000,293.187339);(157.000000,293.320844);(157.000000,293.454350);(157.000000,293.587855);(157.000000,293.721361);(157.000000,293.854866);(157.000000,293.988372);(157.000000,294.121878);(157.000000,294.255383);(157.000000,294.388889);(157.000000,294.522394);(157.000000,294.655900);(157.000000,294.789406);(157.000000,294.922911);(157.000000,295.056417);(157.000000,295.189922);(157.000000,295.323428);(157.000000,295.456934);(157.000000,295.590439);(157.000000,295.723945);(157.000000,295.857450);(157.000000,295.990956);(157.000000,296.124462);</t>
+    <t>157.000000_289.582687;157.000000_289.716193;157.000000_289.849699;157.000000_289.983204;157.000000_290.116710;157.000000_290.250215;157.000000_290.383721;157.000000_290.517227;157.000000_290.650732;157.000000_290.784238;157.000000_290.917743;157.000000_291.051249;157.000000_291.184755;157.000000_291.318260;157.000000_291.451766;157.000000_291.585271;157.000000_291.718777;157.000000_291.852283;157.000000_291.985788;157.000000_292.119294;157.000000_292.252799;157.000000_292.386305;157.000000_292.519811;157.000000_292.653316;157.000000_292.786822;157.000000_292.920327;157.000000_293.053833;157.000000_293.187339;157.000000_293.320844;157.000000_293.454350;157.000000_293.587855;157.000000_293.721361;157.000000_293.854866;157.000000_293.988372;157.000000_294.121878;157.000000_294.255383;157.000000_294.388889;157.000000_294.522394;157.000000_294.655900;157.000000_294.789406;157.000000_294.922911;157.000000_295.056417;157.000000_295.189922;157.000000_295.323428;157.000000_295.456934;157.000000_295.590439;157.000000_295.723945;157.000000_295.857450;157.000000_295.990956;157.000000_296.124462;</t>
   </si>
   <si>
-    <t>(157.000000,296.391473);(157.000000,296.524978);(157.000000,296.658484);(157.000000,296.791990);(157.000000,296.925495);(157.000000,297.059001);(157.000000,297.192506);(157.000000,297.326012);(157.000000,297.459518);(157.000000,297.593023);(157.000000,297.726529);(157.000000,297.860034);(157.000000,297.993540);(157.000000,298.127046);(157.000000,298.260551);(157.000000,298.394057);(157.000000,298.527562);(157.000000,298.661068);(157.000000,298.794574);(157.000000,298.928079);(157.000000,299.061585);(157.000000,299.195090);(157.000000,299.328596);(157.000000,299.462102);(157.000000,299.595607);(157.000000,299.729113);(157.000000,299.862618);(157.000000,299.996124);(157.000000,300.129630);(157.000000,300.263135);(157.000000,300.396641);(157.000000,300.530146);(157.000000,300.663652);(157.000000,300.797158);(157.000000,300.930663);(157.000000,301.064169);(157.000000,301.197674);(157.000000,301.331180);(157.000000,301.464686);(157.000000,301.598191);(157.000000,301.731697);(157.000000,301.865202);(157.000000,301.998708);(157.000000,302.132214);(157.000000,302.265719);(157.000000,302.399225);(157.000000,302.532730);(157.000000,302.666236);(157.000000,302.799742);(157.000000,302.933247);</t>
+    <t>157.000000_296.391473;157.000000_296.524978;157.000000_296.658484;157.000000_296.791990;157.000000_296.925495;157.000000_297.059001;157.000000_297.192506;157.000000_297.326012;157.000000_297.459518;157.000000_297.593023;157.000000_297.726529;157.000000_297.860034;157.000000_297.993540;157.000000_298.127046;157.000000_298.260551;157.000000_298.394057;157.000000_298.527562;157.000000_298.661068;157.000000_298.794574;157.000000_298.928079;157.000000_299.061585;157.000000_299.195090;157.000000_299.328596;157.000000_299.462102;157.000000_299.595607;157.000000_299.729113;157.000000_299.862618;157.000000_299.996124;157.000000_300.129630;157.000000_300.263135;157.000000_300.396641;157.000000_300.530146;157.000000_300.663652;157.000000_300.797158;157.000000_300.930663;157.000000_301.064169;157.000000_301.197674;157.000000_301.331180;157.000000_301.464686;157.000000_301.598191;157.000000_301.731697;157.000000_301.865202;157.000000_301.998708;157.000000_302.132214;157.000000_302.265719;157.000000_302.399225;157.000000_302.532730;157.000000_302.666236;157.000000_302.799742;157.000000_302.933247;</t>
   </si>
   <si>
-    <t>(156.872845,303.098728);(156.625884,303.304977);(156.394601,303.528630);(156.180822,303.769048);(155.986016,304.025080);(155.811139,304.295131);(155.656544,304.577310);(155.521980,304.869609);(155.406659,305.170059);(155.309391,305.476868);(155.228717,305.788486);(155.163039,306.103637);(155.110723,306.421305);(155.070161,306.740707);(155.039820,307.061257);(155.018255,307.382531);(155.004123,307.704227);(154.996174,308.026143);(154.993243,308.348150);(154.994240,308.670173);(154.998132,308.992176);(155.003935,309.314153);(155.010696,309.636113);(155.017480,309.958072);(155.023356,310.280047);(155.027385,310.602050);(155.028606,310.924072);(155.026024,311.246083);(155.018596,311.568012);(155.005222,311.889743);(154.984924,312.211105);(154.957354,312.531926);(154.922733,312.852065);(154.881390,313.171408);(154.833696,313.489866);(154.780052,313.807379);(154.720886,314.123913);(154.656649,314.439458);(154.587809,314.754034);(154.514850,315.067682);(154.438262,315.380467);(154.358544,315.692469);(154.276195,316.003789);(154.191718,316.314540);(154.105612,316.624844);(154.018371,316.934831);(153.930278,317.244578);(153.841053,317.554000);(153.750026,317.862894);(153.656494,318.171038);(153.559759,318.478188);(153.459124,318.784079);(153.353895,319.088417);(153.243383,319.390871);(153.126906,319.691074);(153.003810,319.988618);(152.873859,320.283232);(152.737628,320.575005);(152.596130,320.864267);(152.450377,321.151415);(152.301360,321.436887);(152.150049,321.721152);(151.997398,322.004703);(151.844445,322.288091);(151.692392,322.571961);(151.542542,322.856997);(151.396229,323.143857);(151.254830,323.433161);(151.119776,323.725468);(150.992518,324.021239);(150.873739,324.320518);(150.762714,324.622773);(150.657994,324.927282);(150.558064,325.233405);(150.461385,325.540577);</t>
+    <t>156.872845_303.098728;156.625884_303.304977;156.394601_303.528630;156.180822_303.769048;155.986016_304.025080;155.811139_304.295131;155.656544_304.577310;155.521980_304.869609;155.406659_305.170059;155.309391_305.476868;155.228717_305.788486;155.163039_306.103637;155.110723_306.421305;155.070161_306.740707;155.039820_307.061257;155.018255_307.382531;155.004123_307.704227;154.996174_308.026143;154.993243_308.348150;154.994240_308.670173;154.998132_308.992176;155.003935_309.314153;155.010696_309.636113;155.017480_309.958072;155.023356_310.280047;155.027385_310.602050;155.028606_310.924072;155.026024_311.246083;155.018596_311.568012;155.005222_311.889743;154.984924_312.211105;154.957354_312.531926;154.922733_312.852065;154.881390_313.171408;154.833696_313.489866;154.780052_313.807379;154.720886_314.123913;154.656649_314.439458;154.587809_314.754034;154.514850_315.067682;154.438262_315.380467;154.358544_315.692469;154.276195_316.003789;154.191718_316.314540;154.105612_316.624844;154.018371_316.934831;153.930278_317.244578;153.841053_317.554000;153.750026_317.862894;153.656494_318.171038;153.559759_318.478188;153.459124_318.784079;153.353895_319.088417;153.243383_319.390871;153.126906_319.691074;153.003810_319.988618;152.873859_320.283232;152.737628_320.575005;152.596130_320.864267;152.450377_321.151415;152.301360_321.436887;152.150049_321.721152;151.997398_322.004703;151.844445_322.288091;151.692392_322.571961;151.542542_322.856997;151.396229_323.143857;151.254830_323.433161;151.119776_323.725468;150.992518_324.021239;150.873739_324.320518;150.762714_324.622773;150.657994_324.927282;150.558064_325.233405;150.461385_325.540577;</t>
   </si>
   <si>
-    <t>(150.461385,325.540577);(150.366415,325.848284);(150.271623,326.156047);(150.175502,326.463395);(150.076575,326.769846);(149.973371,327.074876);(149.864068,327.377757);(149.746320,327.677427);(149.617566,327.972496);(149.475225,328.261201);(149.316756,328.541304);(149.139819,328.810030);(148.942844,329.064359);(148.727704,329.303664);(148.500001,329.531251);(148.265817,329.752272);(148.030574,329.972186);(147.798177,330.195083);(147.569383,330.421690);(147.342924,330.650640);(147.117327,330.880443);(146.891248,331.109770);(146.664136,331.338076);(146.436260,331.565619);(146.208052,331.792830);(145.979932,332.020128);(145.752127,332.247743);(145.524549,332.475584);(145.296959,332.703414);(145.069119,332.930993);(144.840895,333.158188);(144.612511,333.385222);(144.384465,333.612594);(144.157288,333.840834);(143.931406,334.070354);(143.706379,334.300715);(143.480671,334.530406);(143.252404,334.757539);(143.019731,334.980131);(142.782763,335.198169);(142.545952,335.416372);(142.316276,335.641925);(142.100554,335.880646);(141.902293,336.134088);(141.712768,336.394410);(141.511563,336.645191);(141.274337,336.858462);(140.987343,336.984926);(140.670560,337.009257);(140.349331,336.989495);(140.032082,337.010826);(139.744018,337.134121);(139.505897,337.346222);(139.303541,337.596114);(139.111000,337.854201);(138.906063,338.102062);(138.681078,338.332009);(138.445213,338.551214);(138.212444,338.773572);(137.995967,339.011360);(137.798079,339.265151);(137.603349,339.521519);(137.387256,339.758616);(137.125833,339.936763);(136.820697,340.011941);(136.499944,340.005724);(136.178893,339.994404);(135.868952,340.054129);(135.597186,340.215226);(135.374306,340.444773);(135.185760,340.705208);(135.013960,340.977503);(134.844060,341.251032);(134.661000,341.515519);(134.446461,341.753326);</t>
+    <t>150.461385_325.540577;150.366415_325.848284;150.271623_326.156047;150.175502_326.463395;150.076575_326.769846;149.973371_327.074876;149.864068_327.377757;149.746320_327.677427;149.617566_327.972496;149.475225_328.261201;149.316756_328.541304;149.139819_328.810030;148.942844_329.064359;148.727704_329.303664;148.500001_329.531251;148.265817_329.752272;148.030574_329.972186;147.798177_330.195083;147.569383_330.421690;147.342924_330.650640;147.117327_330.880443;146.891248_331.109770;146.664136_331.338076;146.436260_331.565619;146.208052_331.792830;145.979932_332.020128;145.752127_332.247743;145.524549_332.475584;145.296959_332.703414;145.069119_332.930993;144.840895_333.158188;144.612511_333.385222;144.384465_333.612594;144.157288_333.840834;143.931406_334.070354;143.706379_334.300715;143.480671_334.530406;143.252404_334.757539;143.019731_334.980131;142.782763_335.198169;142.545952_335.416372;142.316276_335.641925;142.100554_335.880646;141.902293_336.134088;141.712768_336.394410;141.511563_336.645191;141.274337_336.858462;140.987343_336.984926;140.670560_337.009257;140.349331_336.989495;140.032082_337.010826;139.744018_337.134121;139.505897_337.346222;139.303541_337.596114;139.111000_337.854201;138.906063_338.102062;138.681078_338.332009;138.445213_338.551214;138.212444_338.773572;137.995967_339.011360;137.798079_339.265151;137.603349_339.521519;137.387256_339.758616;137.125833_339.936763;136.820697_340.011941;136.499944_340.005724;136.178893_339.994404;135.868952_340.054129;135.597186_340.215226;135.374306_340.444773;135.185760_340.705208;135.013960_340.977503;134.844060_341.251032;134.661000_341.515519;134.446461_341.753326;</t>
   </si>
   <si>
-    <t>(134.446461,341.753326);(134.182813,341.927930);(133.876505,341.998419);(133.555970,341.987169);(133.235389,341.975132);(132.933329,342.052146);(132.683453,342.243609);(132.479679,342.492036);(132.280217,342.744401);(132.042098,342.953653);(131.749189,343.061885);(131.430463,343.067081);(131.112211,343.020764);(130.795274,342.963975);(130.475979,342.929254);(130.160036,342.959611);(129.877910,343.095605);(129.648236,343.317276);(129.446665,343.568234);(129.234618,343.809318);(128.976589,343.990615);(128.671688,344.067237);(128.351809,344.055994);(128.033888,344.006068);(127.716398,343.952802);(127.396540,343.929537);(127.085458,343.983590);(126.815924,344.144711);(126.596723,344.378361);(126.396220,344.630258);(126.175678,344.862450);(125.904305,345.020115);(125.592387,345.070641);(125.272575,345.045647);(124.955142,344.991968);(124.637142,344.942697);(124.317318,344.933604);(124.013606,345.014019);(123.757537,345.198487);(123.546581,345.440644);(123.344711,345.691332);(123.113323,345.910882);(122.829371,346.042827);(122.512865,346.069725);(122.193617,346.033821);(121.876535,345.977795);(121.557987,345.933817);(121.239314,345.942028);(120.946259,346.051467);(120.706073,346.258938);(120.503325,346.508665);(120.297987,346.756001);(120.050670,346.953076);(119.751842,347.045561);(119.431867,347.044528);(119.111463,347.013076);(118.790327,346.996325);(118.468438,347.001089);(118.146614,347.002698);(117.825754,346.980613);(117.505357,346.949904);(117.186842,346.962695);(116.897475,347.079081);(116.662865,347.293571);(116.462812,347.545603);(116.255506,347.790919);(116.001532,347.977104);(115.697819,348.054779);(115.377533,348.044901);(115.057568,348.009104);(114.736666,347.986647);(114.414805,347.986271);(114.092940,347.996195);(113.771026,348.003815);(113.449015,348.004863);</t>
+    <t>134.446461_341.753326;134.182813_341.927930;133.876505_341.998419;133.555970_341.987169;133.235389_341.975132;132.933329_342.052146;132.683453_342.243609;132.479679_342.492036;132.280217_342.744401;132.042098_342.953653;131.749189_343.061885;131.430463_343.067081;131.112211_343.020764;130.795274_342.963975;130.475979_342.929254;130.160036_342.959611;129.877910_343.095605;129.648236_343.317276;129.446665_343.568234;129.234618_343.809318;128.976589_343.990615;128.671688_344.067237;128.351809_344.055994;128.033888_344.006068;127.716398_343.952802;127.396540_343.929537;127.085458_343.983590;126.815924_344.144711;126.596723_344.378361;126.396220_344.630258;126.175678_344.862450;125.904305_345.020115;125.592387_345.070641;125.272575_345.045647;124.955142_344.991968;124.637142_344.942697;124.317318_344.933604;124.013606_345.014019;123.757537_345.198487;123.546581_345.440644;123.344711_345.691332;123.113323_345.910882;122.829371_346.042827;122.512865_346.069725;122.193617_346.033821;121.876535_345.977795;121.557987_345.933817;121.239314_345.942028;120.946259_346.051467;120.706073_346.258938;120.503325_346.508665;120.297987_346.756001;120.050670_346.953076;119.751842_347.045561;119.431867_347.044528;119.111463_347.013076;118.790327_346.996325;118.468438_347.001089;118.146614_347.002698;117.825754_346.980613;117.505357_346.949904;117.186842_346.962695;116.897475_347.079081;116.662865_347.293571;116.462812_347.545603;116.255506_347.790919;116.001532_347.977104;115.697819_348.054779;115.377533_348.044901;115.057568_348.009104;114.736666_347.986647;114.414805_347.986271;114.092940_347.996195;113.771026_348.003815;113.449015_348.004863;</t>
   </si>
   <si>
-    <t>(111.895973,348.000000);(111.687919,348.000000);(111.479866,348.000000);(111.271812,348.000000);(111.063758,348.000000);(110.855705,348.000000);(110.647651,348.000000);(110.439597,348.000000);(110.231544,348.000000);(110.023490,348.000000);(109.815436,348.000000);(109.607383,348.000000);(109.399329,348.000000);(109.191275,348.000000);(108.983221,348.000000);(108.775168,348.000000);(108.567114,348.000000);(108.359060,348.000000);(108.151007,348.000000);(107.942953,348.000000);(107.734899,348.000000);(107.526846,348.000000);(107.318792,348.000000);(107.110738,348.000000);(106.902685,348.000000);(106.694631,348.000000);(106.486577,348.000000);(106.278523,348.000000);(106.070470,348.000000);(105.862416,348.000000);(105.654362,348.000000);(105.446309,348.000000);(105.238255,348.000000);(105.030201,348.000000);(104.822148,348.000000);(104.614094,348.000000);(104.406040,348.000000);(104.197987,348.000000);(103.989933,348.000000);(103.781879,348.000000);(103.573826,348.000000);(103.365772,348.000000);(103.157718,348.000000);(102.949664,348.000000);(102.741611,348.000000);(102.533557,348.000000);(102.325503,348.000000);(102.117450,348.000000);(101.909396,348.000000);(101.701342,348.000000);</t>
+    <t>111.895973_348.000000;111.687919_348.000000;111.479866_348.000000;111.271812_348.000000;111.063758_348.000000;110.855705_348.000000;110.647651_348.000000;110.439597_348.000000;110.231544_348.000000;110.023490_348.000000;109.815436_348.000000;109.607383_348.000000;109.399329_348.000000;109.191275_348.000000;108.983221_348.000000;108.775168_348.000000;108.567114_348.000000;108.359060_348.000000;108.151007_348.000000;107.942953_348.000000;107.734899_348.000000;107.526846_348.000000;107.318792_348.000000;107.110738_348.000000;106.902685_348.000000;106.694631_348.000000;106.486577_348.000000;106.278523_348.000000;106.070470_348.000000;105.862416_348.000000;105.654362_348.000000;105.446309_348.000000;105.238255_348.000000;105.030201_348.000000;104.822148_348.000000;104.614094_348.000000;104.406040_348.000000;104.197987_348.000000;103.989933_348.000000;103.781879_348.000000;103.573826_348.000000;103.365772_348.000000;103.157718_348.000000;102.949664_348.000000;102.741611_348.000000;102.533557_348.000000;102.325503_348.000000;102.117450_348.000000;101.909396_348.000000;101.701342_348.000000;</t>
   </si>
   <si>
-    <t>(101.701342,348.000000);(101.493289,348.000000);(101.285235,348.000000);(101.077181,348.000000);(100.869128,348.000000);(100.661074,348.000000);(100.453020,348.000000);(100.244966,348.000000);(100.036913,348.000000);(99.828859,348.000000);(99.620805,348.000000);(99.412752,348.000000);(99.204698,348.000000);(98.996644,348.000000);(98.788591,348.000000);(98.580537,348.000000);(98.372483,348.000000);(98.164430,348.000000);(97.956376,348.000000);(97.748322,348.000000);(97.540268,348.000000);(97.332215,348.000000);(97.124161,348.000000);(96.916107,348.000000);(96.708054,348.000000);(96.500000,348.000000);(96.291946,348.000000);(96.083893,348.000000);(95.875839,348.000000);(95.667785,348.000000);(95.459732,348.000000);(95.251678,348.000000);(95.043624,348.000000);(94.835570,348.000000);(94.627517,348.000000);(94.419463,348.000000);(94.211409,348.000000);(94.003356,348.000000);(93.795302,348.000000);(93.587248,348.000000);(93.379195,348.000000);(93.171141,348.000000);(92.963087,348.000000);(92.755034,348.000000);(92.546980,348.000000);(92.338926,348.000000);(92.130872,348.000000);(91.922819,348.000000);(91.714765,348.000000);(91.506711,348.000000);</t>
+    <t>101.701342_348.000000;101.493289_348.000000;101.285235_348.000000;101.077181_348.000000;100.869128_348.000000;100.661074_348.000000;100.453020_348.000000;100.244966_348.000000;100.036913_348.000000;99.828859_348.000000;99.620805_348.000000;99.412752_348.000000;99.204698_348.000000;98.996644_348.000000;98.788591_348.000000;98.580537_348.000000;98.372483_348.000000;98.164430_348.000000;97.956376_348.000000;97.748322_348.000000;97.540268_348.000000;97.332215_348.000000;97.124161_348.000000;96.916107_348.000000;96.708054_348.000000;96.500000_348.000000;96.291946_348.000000;96.083893_348.000000;95.875839_348.000000;95.667785_348.000000;95.459732_348.000000;95.251678_348.000000;95.043624_348.000000;94.835570_348.000000;94.627517_348.000000;94.419463_348.000000;94.211409_348.000000;94.003356_348.000000;93.795302_348.000000;93.587248_348.000000;93.379195_348.000000;93.171141_348.000000;92.963087_348.000000;92.755034_348.000000;92.546980_348.000000;92.338926_348.000000;92.130872_348.000000;91.922819_348.000000;91.714765_348.000000;91.506711_348.000000;</t>
   </si>
   <si>
-    <t>(91.506711,348.000000);(91.298658,348.000000);(91.090604,348.000000);(90.882550,348.000000);(90.674497,348.000000);(90.466443,348.000000);(90.258389,348.000000);(90.050336,348.000000);(89.842282,348.000000);(89.634228,348.000000);(89.426174,348.000000);(89.218121,348.000000);(89.010067,348.000000);(88.802013,348.000000);(88.593960,348.000000);(88.385906,348.000000);(88.177852,348.000000);(87.969799,348.000000);(87.761745,348.000000);(87.553691,348.000000);(87.345638,348.000000);(87.137584,348.000000);(86.929530,348.000000);(86.721477,348.000000);(86.513423,348.000000);(86.305369,348.000000);(86.097315,348.000000);(85.889262,348.000000);(85.681208,348.000000);(85.473154,348.000000);(85.265101,348.000000);(85.057047,348.000000);(84.848993,348.000000);(84.640940,348.000000);(84.432886,348.000000);(84.224832,348.000000);(84.016779,348.000000);(83.808725,348.000000);(83.600671,348.000000);(83.392617,348.000000);(83.184564,348.000000);(82.976510,348.000000);(82.768456,348.000000);(82.560403,348.000000);(82.352349,348.000000);(82.144295,348.000000);(81.936242,348.000000);(81.728188,348.000000);(81.520134,348.000000);(81.312081,348.000000);</t>
+    <t>91.506711_348.000000;91.298658_348.000000;91.090604_348.000000;90.882550_348.000000;90.674497_348.000000;90.466443_348.000000;90.258389_348.000000;90.050336_348.000000;89.842282_348.000000;89.634228_348.000000;89.426174_348.000000;89.218121_348.000000;89.010067_348.000000;88.802013_348.000000;88.593960_348.000000;88.385906_348.000000;88.177852_348.000000;87.969799_348.000000;87.761745_348.000000;87.553691_348.000000;87.345638_348.000000;87.137584_348.000000;86.929530_348.000000;86.721477_348.000000;86.513423_348.000000;86.305369_348.000000;86.097315_348.000000;85.889262_348.000000;85.681208_348.000000;85.473154_348.000000;85.265101_348.000000;85.057047_348.000000;84.848993_348.000000;84.640940_348.000000;84.432886_348.000000;84.224832_348.000000;84.016779_348.000000;83.808725_348.000000;83.600671_348.000000;83.392617_348.000000;83.184564_348.000000;82.976510_348.000000;82.768456_348.000000;82.560403_348.000000;82.352349_348.000000;82.144295_348.000000;81.936242_348.000000;81.728188_348.000000;81.520134_348.000000;81.312081_348.000000;</t>
   </si>
   <si>
-    <t>(81.312081,348.000000);(81.104027,348.000000);(80.895973,348.000000);(80.687919,348.000000);(80.479866,348.000000);(80.271812,348.000000);(80.063758,348.000000);(79.855705,348.000000);(79.647651,348.000000);(79.439597,348.000000);(79.231544,348.000000);(79.023490,348.000000);(78.815436,348.000000);(78.607383,348.000000);(78.399329,348.000000);(78.191275,348.000000);(77.983221,348.000000);(77.775168,348.000000);(77.567114,348.000000);(77.359060,348.000000);(77.151007,348.000000);(76.942953,348.000000);(76.734899,348.000000);(76.526846,348.000000);(76.318792,348.000000);(76.110738,348.000000);(75.902685,348.000000);(75.694631,348.000000);(75.486577,348.000000);(75.278523,348.000000);(75.070470,348.000000);(74.862416,348.000000);(74.654362,348.000000);(74.446309,348.000000);(74.238255,348.000000);(74.030201,348.000000);(73.822148,348.000000);(73.614094,348.000000);(73.406040,348.000000);(73.197987,348.000000);(72.989933,348.000000);(72.781879,348.000000);(72.573826,348.000000);</t>
+    <t>81.312081_348.000000;81.104027_348.000000;80.895973_348.000000;80.687919_348.000000;80.479866_348.000000;80.271812_348.000000;80.063758_348.000000;79.855705_348.000000;79.647651_348.000000;79.439597_348.000000;79.231544_348.000000;79.023490_348.000000;78.815436_348.000000;78.607383_348.000000;78.399329_348.000000;78.191275_348.000000;77.983221_348.000000;77.775168_348.000000;77.567114_348.000000;77.359060_348.000000;77.151007_348.000000;76.942953_348.000000;76.734899_348.000000;76.526846_348.000000;76.318792_348.000000;76.110738_348.000000;75.902685_348.000000;75.694631_348.000000;75.486577_348.000000;75.278523_348.000000;75.070470_348.000000;74.862416_348.000000;74.654362_348.000000;74.446309_348.000000;74.238255_348.000000;74.030201_348.000000;73.822148_348.000000;73.614094_348.000000;73.406040_348.000000;73.197987_348.000000;72.989933_348.000000;72.781879_348.000000;72.573826_348.000000;</t>
   </si>
   <si>
-    <t>(72.573826,348.000000);(72.365772,348.000000);(72.157718,348.000000);(71.949664,348.000000);(71.741611,348.000000);(71.533557,348.000000);(71.325503,348.000000);(71.117450,348.000000);(70.909396,348.000000);(70.701342,348.000000);(70.493289,348.000000);(70.285235,348.000000);(70.077181,348.000000);(69.869128,348.000000);(69.661074,348.000000);(69.453020,348.000000);(69.244966,348.000000);(69.036913,348.000000);(68.828859,348.000000);(68.620805,348.000000);(68.412752,348.000000);(68.204698,348.000000);(67.996644,348.000000);(67.788591,348.000000);(67.580537,348.000000);(67.372483,348.000000);(67.164430,348.000000);(66.956376,348.000000);(66.748322,348.000000);(66.540268,348.000000);(66.332215,348.000000);(66.124161,348.000000);(65.916107,348.000000);(65.708054,348.000000);(65.500000,348.000000);(65.291946,348.000000);(65.083893,348.000000);(64.875839,348.000000);(64.667785,348.000000);(64.459732,348.000000);(64.251678,348.000000);(64.043624,348.000000);(63.835570,348.000000);(63.627517,348.000000);(63.419463,348.000000);(63.211409,348.000000);(63.003356,348.000000);(62.795302,348.000000);(62.587248,348.000000);(62.379195,348.000000);</t>
+    <t>72.573826_348.000000;72.365772_348.000000;72.157718_348.000000;71.949664_348.000000;71.741611_348.000000;71.533557_348.000000;71.325503_348.000000;71.117450_348.000000;70.909396_348.000000;70.701342_348.000000;70.493289_348.000000;70.285235_348.000000;70.077181_348.000000;69.869128_348.000000;69.661074_348.000000;69.453020_348.000000;69.244966_348.000000;69.036913_348.000000;68.828859_348.000000;68.620805_348.000000;68.412752_348.000000;68.204698_348.000000;67.996644_348.000000;67.788591_348.000000;67.580537_348.000000;67.372483_348.000000;67.164430_348.000000;66.956376_348.000000;66.748322_348.000000;66.540268_348.000000;66.332215_348.000000;66.124161_348.000000;65.916107_348.000000;65.708054_348.000000;65.500000_348.000000;65.291946_348.000000;65.083893_348.000000;64.875839_348.000000;64.667785_348.000000;64.459732_348.000000;64.251678_348.000000;64.043624_348.000000;63.835570_348.000000;63.627517_348.000000;63.419463_348.000000;63.211409_348.000000;63.003356_348.000000;62.795302_348.000000;62.587248_348.000000;62.379195_348.000000;</t>
   </si>
   <si>
-    <t>(62.379195,348.000000);(62.171141,348.000000);(61.963087,348.000000);(61.755034,348.000000);(61.546980,348.000000);(61.338926,348.000000);(61.130872,348.000000);(60.922819,348.000000);(60.714765,348.000000);(60.506711,348.000000);(60.298658,348.000000);(60.090604,348.000000);(59.882550,348.000000);(59.674497,348.000000);(59.466443,348.000000);(59.258389,348.000000);(59.050336,348.000000);(58.842282,348.000000);(58.634228,348.000000);(58.426174,348.000000);(58.218121,348.000000);(58.010067,348.000000);(57.802013,348.000000);(57.593960,348.000000);(57.385906,348.000000);(57.177852,348.000000);(56.969799,348.000000);(56.761745,348.000000);(56.553691,348.000000);(56.345638,348.000000);(56.137584,348.000000);(55.929530,348.000000);(55.721477,348.000000);(55.513423,348.000000);(55.305369,348.000000);(55.097315,348.000000);(54.889262,348.000000);(54.681208,348.000000);(54.473154,348.000000);(54.265101,348.000000);(54.057047,348.000000);(53.848993,348.000000);(53.640940,348.000000);(53.432886,348.000000);(53.224832,348.000000);(53.016779,348.000000);(52.808725,348.000000);(52.600671,348.000000);(52.392617,348.000000);(52.184564,348.000000);</t>
+    <t>62.379195_348.000000;62.171141_348.000000;61.963087_348.000000;61.755034_348.000000;61.546980_348.000000;61.338926_348.000000;61.130872_348.000000;60.922819_348.000000;60.714765_348.000000;60.506711_348.000000;60.298658_348.000000;60.090604_348.000000;59.882550_348.000000;59.674497_348.000000;59.466443_348.000000;59.258389_348.000000;59.050336_348.000000;58.842282_348.000000;58.634228_348.000000;58.426174_348.000000;58.218121_348.000000;58.010067_348.000000;57.802013_348.000000;57.593960_348.000000;57.385906_348.000000;57.177852_348.000000;56.969799_348.000000;56.761745_348.000000;56.553691_348.000000;56.345638_348.000000;56.137584_348.000000;55.929530_348.000000;55.721477_348.000000;55.513423_348.000000;55.305369_348.000000;55.097315_348.000000;54.889262_348.000000;54.681208_348.000000;54.473154_348.000000;54.265101_348.000000;54.057047_348.000000;53.848993_348.000000;53.640940_348.000000;53.432886_348.000000;53.224832_348.000000;53.016779_348.000000;52.808725_348.000000;52.600671_348.000000;52.392617_348.000000;52.184564_348.000000;</t>
   </si>
   <si>
-    <t>(49.947733,347.845849);(49.814359,347.550828);(49.616335,347.297477);(49.352775,347.115458);(49.046233,347.016138);(48.723547,346.981454);(48.397955,346.982887);(48.072357,346.995961);(47.746638,347.004034);(47.420782,347.003743);(47.094921,347.001050);(46.769055,347.001105);(46.443187,347.003026);(46.117342,347.001229);(45.791614,346.992410);(45.465890,346.984112);(45.140429,346.992233);(44.816425,347.024365);(44.492645,347.058502);(44.171829,347.038604);(43.887027,346.905352);(43.661615,346.674970);(43.465922,346.414565);(43.251094,346.172306);(42.977972,346.018542);(42.660927,345.990191);(42.336525,346.017124);(42.021578,345.980616);(41.755680,345.815179);(41.548980,345.565440);(41.355474,345.303593);(41.121565,345.085634);(40.825961,344.987873);(40.502602,344.999910);(40.179163,345.012796);(39.882951,344.916774);(39.648372,344.699824);(39.454889,344.437980);(39.248746,344.187726);(38.983482,344.021313);(38.668802,343.984525);(38.344456,344.011984);(38.027931,343.982644);(37.757472,343.825396);(37.546613,343.579555);(37.352673,343.317916);(37.123477,343.093104);(36.832744,342.978749);(36.510014,342.976758);(36.185433,342.998192);(35.870363,342.949533);(35.593986,342.791080);(35.369865,342.557758);(35.181678,342.292335);(35.009399,342.015780);(34.836828,341.739411);(34.648800,341.473797);(34.427695,341.236969);(34.157558,341.065226);(33.846340,340.995443);(33.521627,341.002898);(33.196823,341.011860);(32.885647,340.943693);(32.616595,340.770960);(32.394990,340.534114);(32.199016,340.273968);(32.005473,340.011887);(31.798538,339.760519);(31.574872,339.523819);(31.338709,339.299431);(31.095186,339.082928);(30.849624,338.868705);(30.607346,338.650832);(30.373605,338.423953);(30.153384,338.184073);</t>
+    <t>49.947733_347.845849;49.814359_347.550828;49.616335_347.297477;49.352775_347.115458;49.046233_347.016138;48.723547_346.981454;48.397955_346.982887;48.072357_346.995961;47.746638_347.004034;47.420782_347.003743;47.094921_347.001050;46.769055_347.001105;46.443187_347.003026;46.117342_347.001229;45.791614_346.992410;45.465890_346.984112;45.140429_346.992233;44.816425_347.024365;44.492645_347.058502;44.171829_347.038604;43.887027_346.905352;43.661615_346.674970;43.465922_346.414565;43.251094_346.172306;42.977972_346.018542;42.660927_345.990191;42.336525_346.017124;42.021578_345.980616;41.755680_345.815179;41.548980_345.565440;41.355474_345.303593;41.121565_345.085634;40.825961_344.987873;40.502602_344.999910;40.179163_345.012796;39.882951_344.916774;39.648372_344.699824;39.454889_344.437980;39.248746_344.187726;38.983482_344.021313;38.668802_343.984525;38.344456_344.011984;38.027931_343.982644;37.757472_343.825396;37.546613_343.579555;37.352673_343.317916;37.123477_343.093104;36.832744_342.978749;36.510014_342.976758;36.185433_342.998192;35.870363_342.949533;35.593986_342.791080;35.369865_342.557758;35.181678_342.292335;35.009399_342.015780;34.836828_341.739411;34.648800_341.473797;34.427695_341.236969;34.157558_341.065226;33.846340_340.995443;33.521627_341.002898;33.196823_341.011860;32.885647_340.943693;32.616595_340.770960;32.394990_340.534114;32.199016_340.273968;32.005473_340.011887;31.798538_339.760519;31.574872_339.523819;31.338709_339.299431;31.095186_339.082928;30.849624_338.868705;30.607346_338.650832;30.373605_338.423953;30.153384_338.184073;</t>
   </si>
   <si>
-    <t>(30.153384,338.184073);(29.950014,337.929774);(29.757407,337.666954);(29.557581,337.409931);(29.326874,337.182852);(29.046601,337.031840);(28.729905,336.986511);(28.404804,337.002600);(28.081087,336.997885);(27.775553,336.906626);(27.513250,336.720837);(27.298174,336.478270);(27.118390,336.207216);(26.961883,335.921639);(26.820375,335.628193);(26.688011,335.330439);(26.558552,335.031386);(26.424599,334.734366);(26.278024,334.443523);(26.110857,334.164277);(25.917672,333.902573);(25.700810,333.659817);(25.468759,333.431197);(25.229554,333.209919);(24.989788,332.989235);(24.753730,332.764615);(24.522040,332.535477);(24.293505,332.303179);(24.066735,332.069152);(23.840300,331.834798);(23.612840,331.601443);(23.383086,331.370355);(23.149832,331.142812);(22.912348,330.919691);(22.672655,330.698919);(22.436012,330.474941);(22.209010,330.241380);(21.999227,329.992526);(21.812139,329.726247);(21.647131,329.445561);(21.499652,329.155132);(21.364526,328.858658);(21.236489,328.559004);(21.110326,328.258544);(20.980995,327.959453);(20.845468,327.663128);(20.703913,327.369623);(20.557855,327.078323);(20.408858,326.788509);(20.258488,326.499401);(20.108314,326.210192);(19.959812,325.920124);(19.813568,325.628911);(19.668989,325.336865);(19.525094,325.044481);(19.380901,324.752243);(19.235437,324.460639);(19.087734,324.170164);(18.937049,323.881228);(18.783923,323.593573);(18.630308,323.306177);(18.478501,323.017827);(18.330842,322.727346);(18.189742,322.433645);(18.057710,322.135788);(17.936834,321.833250);(17.826947,321.526523);(17.725665,321.216818);(17.630157,320.905264);(17.537572,320.592820);(17.445058,320.280354);(17.349767,319.968734);(17.248856,319.658906);(17.139511,319.351983);(17.019011,319.049305);</t>
+    <t>30.153384_338.184073;29.950014_337.929774;29.757407_337.666954;29.557581_337.409931;29.326874_337.182852;29.046601_337.031840;28.729905_336.986511;28.404804_337.002600;28.081087_336.997885;27.775553_336.906626;27.513250_336.720837;27.298174_336.478270;27.118390_336.207216;26.961883_335.921639;26.820375_335.628193;26.688011_335.330439;26.558552_335.031386;26.424599_334.734366;26.278024_334.443523;26.110857_334.164277;25.917672_333.902573;25.700810_333.659817;25.468759_333.431197;25.229554_333.209919;24.989788_332.989235;24.753730_332.764615;24.522040_332.535477;24.293505_332.303179;24.066735_332.069152;23.840300_331.834798;23.612840_331.601443;23.383086_331.370355;23.149832_331.142812;22.912348_330.919691;22.672655_330.698919;22.436012_330.474941;22.209010_330.241380;21.999227_329.992526;21.812139_329.726247;21.647131_329.445561;21.499652_329.155132;21.364526_328.858658;21.236489_328.559004;21.110326_328.258544;20.980995_327.959453;20.845468_327.663128;20.703913_327.369623;20.557855_327.078323;20.408858_326.788509;20.258488_326.499401;20.108314_326.210192;19.959812_325.920124;19.813568_325.628911;19.668989_325.336865;19.525094_325.044481;19.380901_324.752243;19.235437_324.460639;19.087734_324.170164;18.937049_323.881228;18.783923_323.593573;18.630308_323.306177;18.478501_323.017827;18.330842_322.727346;18.189742_322.433645;18.057710_322.135788;17.936834_321.833250;17.826947_321.526523;17.725665_321.216818;17.630157_320.905264;17.537572_320.592820;17.445058_320.280354;17.349767_319.968734;17.248856_319.658906;17.139511_319.351983;17.019011_319.049305;</t>
   </si>
   <si>
-    <t>(17.019011,319.049305);(16.886060,318.751887);(16.742617,318.459333);(16.592609,318.170053);(16.439956,317.882146);(16.288507,317.593609);(16.142179,317.302472);(16.005030,317.006950);(15.880102,316.706085);(15.768043,316.400180);(15.668064,316.090101);(15.579199,315.776641);(15.500408,315.460486);(15.430608,315.142213);(15.368696,314.822303);(15.313572,314.501145);(15.264143,314.179054);(15.219334,313.856284);(15.178089,313.533034);(15.139367,313.209470);(15.102141,312.885729);(15.065392,312.561933);(15.028100,312.238199);(14.989285,311.914646);(14.948360,311.591354);(14.905264,311.268343);(14.860121,310.945613);(14.813052,310.623157);(14.764183,310.300968);(14.713643,309.979038);(14.661558,309.657353);(14.608059,309.335901);(14.553276,309.014664);(14.497341,308.693627);(14.440387,308.372768);(14.382546,308.052067);(14.323955,307.731503);(14.264746,307.411052);(14.205057,307.090691);(14.145022,306.770393);(14.084780,306.450135);(14.024467,306.129890);(13.964221,305.809633);(13.904180,305.489337);(13.844484,305.168976);(13.785270,304.848526);(13.726678,304.527962);(13.668849,304.207260);(13.611920,303.886397);(13.556033,303.565350);(13.501328,303.244101);(13.447943,302.922629);(13.396020,302.600919);(13.345697,302.278954);(13.297113,301.956723);(13.250406,301.634215);(13.205716,301.311421);(13.163177,300.988337);(13.122925,300.664960);(13.085096,300.341292);(13.049820,300.017335);(13.017229,299.693098);(12.987450,299.368591);(12.960610,299.043828);(12.936831,298.718827);(12.916233,298.393609);(12.898931,298.068199);(12.885037,297.742627);(12.874660,297.416924);(12.867902,297.091126);(12.864860,296.765272);(12.865629,296.439406);(12.870293,296.113572);(12.878935,295.787820);(12.891629,295.462201);</t>
+    <t>17.019011_319.049305;16.886060_318.751887;16.742617_318.459333;16.592609_318.170053;16.439956_317.882146;16.288507_317.593609;16.142179_317.302472;16.005030_317.006950;15.880102_316.706085;15.768043_316.400180;15.668064_316.090101;15.579199_315.776641;15.500408_315.460486;15.430608_315.142213;15.368696_314.822303;15.313572_314.501145;15.264143_314.179054;15.219334_313.856284;15.178089_313.533034;15.139367_313.209470;15.102141_312.885729;15.065392_312.561933;15.028100_312.238199;14.989285_311.914646;14.948360_311.591354;14.905264_311.268343;14.860121_310.945613;14.813052_310.623157;14.764183_310.300968;14.713643_309.979038;14.661558_309.657353;14.608059_309.335901;14.553276_309.014664;14.497341_308.693627;14.440387_308.372768;14.382546_308.052067;14.323955_307.731503;14.264746_307.411052;14.205057_307.090691;14.145022_306.770393;14.084780_306.450135;14.024467_306.129890;13.964221_305.809633;13.904180_305.489337;13.844484_305.168976;13.785270_304.848526;13.726678_304.527962;13.668849_304.207260;13.611920_303.886397;13.556033_303.565350;13.501328_303.244101;13.447943_302.922629;13.396020_302.600919;13.345697_302.278954;13.297113_301.956723;13.250406_301.634215;13.205716_301.311421;13.163177_300.988337;13.122925_300.664960;13.085096_300.341292;13.049820_300.017335;13.017229_299.693098;12.987450_299.368591;12.960610_299.043828;12.936831_298.718827;12.916233_298.393609;12.898931_298.068199;12.885037_297.742627;12.874660_297.416924;12.867902_297.091126;12.864860_296.765272;12.865629_296.439406;12.870293_296.113572;12.878935_295.787820;12.891629_295.462201;</t>
   </si>
   <si>
-    <t>(12.968310,293.891650);(12.906773,293.674428);(12.848956,293.456187);(12.794917,293.236981);(12.744712,293.016864);(12.698390,292.795898);(12.655993,292.574146);(12.617559,292.351673);(12.583114,292.128547);(12.552679,291.904839);(12.526267,291.680621);(12.503882,291.455965);(12.485517,291.230944);(12.471161,291.005632);(12.460789,290.780101);(12.454371,290.554423);(12.451867,290.328667);(12.453229,290.102901);(12.458399,289.877190);(12.467313,289.651596);(12.479900,289.426176);(12.496082,289.200985);(12.515773,288.976074);(12.538882,288.751487);(12.565314,288.527267);(12.594968,288.303449);(12.627739,288.080067);(12.663519,287.857146);(12.702196,287.634709);(12.743657,287.412773);(12.787786,287.191352);(12.834465,286.970454);(12.883576,286.750084);(12.934999,286.530241);(12.988615,286.310922);(13.044302,286.092120);(13.101943,285.873824);(13.161416,285.656019);(13.222603,285.438689);(13.285385,285.221815);(13.349645,285.005374);(13.415266,284.789341);(13.482131,284.573689);(13.550126,284.358391);(13.619136,284.143416);(13.689049,283.928733);(13.759751,283.714308);(13.831133,283.500109);(13.903082,283.286099);(13.975489,283.072243);(14.048246,282.858507);(14.121242,282.644852);(14.194371,282.431242);(14.267524,282.217640);(14.340595,282.004010);(14.413475,281.790316);(14.486059,281.576520);(14.558239,281.362588);(14.629909,281.148485);(14.700962,280.934176);(14.771291,280.719629);(14.840788,280.504811);(14.909347,280.289691);(14.976860,280.074242);(15.043284,279.858454);(15.108806,279.642390);(15.173801,279.426166);(15.238671,279.209905);(15.303818,278.993728);(15.369644,278.777756);(15.436552,278.562119);(15.504945,278.346948);(15.575225,278.132388);(15.647793,277.918592);(15.723047,277.705729);</t>
+    <t>12.968310_293.891650;12.906773_293.674428;12.848956_293.456187;12.794917_293.236981;12.744712_293.016864;12.698390_292.795898;12.655993_292.574146;12.617559_292.351673;12.583114_292.128547;12.552679_291.904839;12.526267_291.680621;12.503882_291.455965;12.485517_291.230944;12.471161_291.005632;12.460789_290.780101;12.454371_290.554423;12.451867_290.328667;12.453229_290.102901;12.458399_289.877190;12.467313_289.651596;12.479900_289.426176;12.496082_289.200985;12.515773_288.976074;12.538882_288.751487;12.565314_288.527267;12.594968_288.303449;12.627739_288.080067;12.663519_287.857146;12.702196_287.634709;12.743657_287.412773;12.787786_287.191352;12.834465_286.970454;12.883576_286.750084;12.934999_286.530241;12.988615_286.310922;13.044302_286.092120;13.101943_285.873824;13.161416_285.656019;13.222603_285.438689;13.285385_285.221815;13.349645_285.005374;13.415266_284.789341;13.482131_284.573689;13.550126_284.358391;13.619136_284.143416;13.689049_283.928733;13.759751_283.714308;13.831133_283.500109;13.903082_283.286099;13.975489_283.072243;14.048246_282.858507;14.121242_282.644852;14.194371_282.431242;14.267524_282.217640;14.340595_282.004010;14.413475_281.790316;14.486059_281.576520;14.558239_281.362588;14.629909_281.148485;14.700962_280.934176;14.771291_280.719629;14.840788_280.504811;14.909347_280.289691;14.976860_280.074242;15.043284_279.858454;15.108806_279.642390;15.173801_279.426166;15.238671_279.209905;15.303818_278.993728;15.369644_278.777756;15.436552_278.562119;15.504945_278.346948;15.575225_278.132388;15.647793_277.918592;15.723047_277.705729;</t>
   </si>
   <si>
-    <t>(15.883189,277.283556);(15.968842,277.074668);(16.058589,276.867507);(16.152230,276.662073);(16.249206,276.458189);(16.348916,276.255624);(16.450773,276.054128);(16.554205,275.853434);(16.658645,275.653262);(16.763537,275.453325);(16.868327,275.253335);(16.972462,275.053004);(17.075513,274.852114);(17.177428,274.650645);(17.278441,274.448721);(17.378818,274.246481);(17.478829,274.044058);(17.578741,273.841588);(17.678827,273.639202);(17.779357,273.437038);(17.880602,273.235230);(17.982830,273.033920);(18.086161,272.833173);(18.190339,272.632864);(18.294866,272.432737);(18.399223,272.232521);(18.502891,272.031948);(18.605353,271.830757);(18.706091,271.628700);(18.804589,271.425543);(18.900334,271.221077);(18.992830,271.015125);(19.082095,270.807748);(19.169234,270.599462);(19.255973,270.391007);(19.344073,270.183129);(19.435305,269.976617);(19.531459,269.772369);(19.634333,269.571447);(19.745697,269.375141);(19.867219,269.185002);(20.000297,269.002816);(20.144937,268.829644);(20.298973,268.664685);(20.459429,268.505896);(20.623656,268.350972);(20.789270,268.197516);(20.953994,268.043114);(21.116058,267.885936);(21.275340,267.725928);(21.433065,267.564375);(21.590660,267.402695);(21.749562,267.242307);(21.911158,267.084649);(22.076414,266.930842);(22.244474,266.780077);(22.412691,266.629483);(22.577998,266.475745);(22.737053,266.315634);(22.885995,266.146208);(23.020582,265.965311);(23.138828,265.773285);(23.242792,265.573028);(23.336367,265.367621);(23.423543,265.159368);(23.508261,264.950085);(23.594463,264.741420);(23.686207,264.535177);(23.787749,264.333670);(23.903468,264.140114);(24.037068,263.958627);(24.187864,263.790993);(24.350081,263.634089);(24.517163,263.482245);(24.683549,263.329656);</t>
+    <t>15.883189_277.283556;15.968842_277.074668;16.058589_276.867507;16.152230_276.662073;16.249206_276.458189;16.348916_276.255624;16.450773_276.054128;16.554205_275.853434;16.658645_275.653262;16.763537_275.453325;16.868327_275.253335;16.972462_275.053004;17.075513_274.852114;17.177428_274.650645;17.278441_274.448721;17.378818_274.246481;17.478829_274.044058;17.578741_273.841588;17.678827_273.639202;17.779357_273.437038;17.880602_273.235230;17.982830_273.033920;18.086161_272.833173;18.190339_272.632864;18.294866_272.432737;18.399223_272.232521;18.502891_272.031948;18.605353_271.830757;18.706091_271.628700;18.804589_271.425543;18.900334_271.221077;18.992830_271.015125;19.082095_270.807748;19.169234_270.599462;19.255973_270.391007;19.344073_270.183129;19.435305_269.976617;19.531459_269.772369;19.634333_269.571447;19.745697_269.375141;19.867219_269.185002;20.000297_269.002816;20.144937_268.829644;20.298973_268.664685;20.459429_268.505896;20.623656_268.350972;20.789270_268.197516;20.953994_268.043114;21.116058_267.885936;21.275340_267.725928;21.433065_267.564375;21.590660_267.402695;21.749562_267.242307;21.911158_267.084649;22.076414_266.930842;22.244474_266.780077;22.412691_266.629483;22.577998_266.475745;22.737053_266.315634;22.885995_266.146208;23.020582_265.965311;23.138828_265.773285;23.242792_265.573028;23.336367_265.367621;23.423543_265.159368;23.508261_264.950085;23.594463_264.741420;23.686207_264.535177;23.787749_264.333670;23.903468_264.140114;24.037068_263.958627;24.187864_263.790993;24.350081_263.634089;24.517163_263.482245;24.683549_263.329656;</t>
   </si>
   <si>
-    <t>(24.994549,263.002995);(25.133243,262.825011);(25.265418,262.641977);(25.399556,262.460428);(25.545045,262.288244);(25.712459,262.138733);(25.909011,262.034603);(26.127595,261.994126);(26.352460,262.002619);(26.577052,262.025340);(26.801829,262.030254);(27.017126,261.979832);(27.202322,261.858638);(27.353498,261.692401);(27.486802,261.510310);(27.619411,261.327679);(27.768406,261.159290);(27.950646,261.033241);(28.164372,260.978925);(28.388953,260.984091);(28.613373,261.008388);(28.838053,261.016309);(29.053793,260.968186);(29.241026,260.849546);(29.395787,260.686623);(29.532445,260.507064);(29.666665,260.325566);(29.813696,260.155022);(29.989321,260.017572);(30.196569,259.938746);(30.419634,259.919124);(30.644143,259.937253);(30.866772,259.974217);(31.088467,260.016945);(31.310955,260.054897);(31.535290,260.076576);(31.759475,260.065922);(31.972821,260.002663);(32.159359,259.880897);(32.316800,259.720312);(32.457643,259.544005);(32.595724,259.365408);(32.744507,259.196172);(32.918052,259.054938);(33.122051,258.967689);(33.344063,258.939697);(33.569143,258.949525);(33.793425,258.975095);(34.017785,258.999875);(34.243003,259.013749);(34.468701,259.015865);(34.694399,259.010526);(34.920048,259.002875);(35.145752,258.997437);(35.371518,258.995663);(35.597295,258.996449);(35.823067,258.998395);(36.048840,259.000181);(36.274619,259.001062);(36.500399,259.001105);(36.726179,259.000673);(36.951960,259.000135);(37.177740,258.999781);(37.403521,258.999683);(37.629302,258.999755);(37.855082,258.999902);(38.080863,259.000030);(38.306644,259.000094);(38.532425,259.000098);(38.758206,259.000062);(38.983986,259.000004);(39.209767,258.999946);(39.435548,258.999905);(39.661329,258.999902);(39.887110,258.999956);</t>
+    <t>24.994549_263.002995;25.133243_262.825011;25.265418_262.641977;25.399556_262.460428;25.545045_262.288244;25.712459_262.138733;25.909011_262.034603;26.127595_261.994126;26.352460_262.002619;26.577052_262.025340;26.801829_262.030254;27.017126_261.979832;27.202322_261.858638;27.353498_261.692401;27.486802_261.510310;27.619411_261.327679;27.768406_261.159290;27.950646_261.033241;28.164372_260.978925;28.388953_260.984091;28.613373_261.008388;28.838053_261.016309;29.053793_260.968186;29.241026_260.849546;29.395787_260.686623;29.532445_260.507064;29.666665_260.325566;29.813696_260.155022;29.989321_260.017572;30.196569_259.938746;30.419634_259.919124;30.644143_259.937253;30.866772_259.974217;31.088467_260.016945;31.310955_260.054897;31.535290_260.076576;31.759475_260.065922;31.972821_260.002663;32.159359_259.880897;32.316800_259.720312;32.457643_259.544005;32.595724_259.365408;32.744507_259.196172;32.918052_259.054938;33.122051_258.967689;33.344063_258.939697;33.569143_258.949525;33.793425_258.975095;34.017785_258.999875;34.243003_259.013749;34.468701_259.015865;34.694399_259.010526;34.920048_259.002875;35.145752_258.997437;35.371518_258.995663;35.597295_258.996449;35.823067_258.998395;36.048840_259.000181;36.274619_259.001062;36.500399_259.001105;36.726179_259.000673;36.951960_259.000135;37.177740_258.999781;37.403521_258.999683;37.629302_258.999755;37.855082_258.999902;38.080863_259.000030;38.306644_259.000094;38.532425_259.000098;38.758206_259.000062;38.983986_259.000004;39.209767_258.999946;39.435548_258.999905;39.661329_258.999902;39.887110_258.999956;</t>
   </si>
   <si>
-    <t>(40.025835,259.155942);(40.105493,259.460214);(40.258517,259.730160);(40.501124,259.915255);(40.801951,259.990084);(41.117133,259.990228);(41.432631,259.967447);(41.747904,259.965894);(42.051277,260.034681);(42.318415,260.194424);(42.542881,260.415217);(42.741437,260.661219);(42.933671,260.912463);(43.135157,261.156115);(43.351083,261.387110);(43.577608,261.607874);(43.809212,261.823390);(44.040403,262.039347);(44.267939,262.259138);(44.491971,262.482517);(44.713961,262.707934);(44.935374,262.933919);(45.157420,263.159282);(45.380500,263.383622);(45.604390,263.607153);(45.828793,263.830171);(46.053409,264.052974);(46.277947,264.275855);(46.502126,264.499097);(46.725667,264.722978);(46.948289,264.947771);(47.169992,265.173472);(47.391574,265.399292);(47.614405,265.623874);(47.839878,265.845793);(48.069039,266.063892);(48.300602,266.279463);(48.530347,266.496940);(48.752895,266.721658);(48.962184,266.958575);(49.152940,267.210540);(49.323906,267.476421);(49.477146,267.752995);(49.615402,268.037429);(49.741599,268.327469);(49.858691,268.621340);(49.969609,268.917620);(50.076865,269.215256);(50.181754,269.513735);(50.284646,269.812910);(50.385820,270.112670);(50.485564,270.412910);(50.584175,270.713524);(50.681958,271.014409);(50.779221,271.315463);(50.876276,271.616584);(50.973436,271.917671);(51.070966,272.218638);(51.168992,272.519444);(51.267533,272.820082);(51.366596,273.120548);(51.466192,273.420838);(51.566327,273.720949);(51.667010,274.020876);(51.768251,274.320615);(51.870059,274.620162);(51.972442,274.919513);(52.075357,275.218682);(52.178597,275.517739);(52.281831,275.816797);(52.384717,276.115976);(52.486910,276.415392);(52.588065,276.715159);(52.687833,277.015391);(52.785867,277.316192);</t>
+    <t>40.025835_259.155942;40.105493_259.460214;40.258517_259.730160;40.501124_259.915255;40.801951_259.990084;41.117133_259.990228;41.432631_259.967447;41.747904_259.965894;42.051277_260.034681;42.318415_260.194424;42.542881_260.415217;42.741437_260.661219;42.933671_260.912463;43.135157_261.156115;43.351083_261.387110;43.577608_261.607874;43.809212_261.823390;44.040403_262.039347;44.267939_262.259138;44.491971_262.482517;44.713961_262.707934;44.935374_262.933919;45.157420_263.159282;45.380500_263.383622;45.604390_263.607153;45.828793_263.830171;46.053409_264.052974;46.277947_264.275855;46.502126_264.499097;46.725667_264.722978;46.948289_264.947771;47.169992_265.173472;47.391574_265.399292;47.614405_265.623874;47.839878_265.845793;48.069039_266.063892;48.300602_266.279463;48.530347_266.496940;48.752895_266.721658;48.962184_266.958575;49.152940_267.210540;49.323906_267.476421;49.477146_267.752995;49.615402_268.037429;49.741599_268.327469;49.858691_268.621340;49.969609_268.917620;50.076865_269.215256;50.181754_269.513735;50.284646_269.812910;50.385820_270.112670;50.485564_270.412910;50.584175_270.713524;50.681958_271.014409;50.779221_271.315463;50.876276_271.616584;50.973436_271.917671;51.070966_272.218638;51.168992_272.519444;51.267533_272.820082;51.366596_273.120548;51.466192_273.420838;51.566327_273.720949;51.667010_274.020876;51.768251_274.320615;51.870059_274.620162;51.972442_274.919513;52.075357_275.218682;52.178597_275.517739;52.281831_275.816797;52.384717_276.115976;52.486910_276.415392;52.588065_276.715159;52.687833_277.015391;52.785867_277.316192;</t>
   </si>
   <si>
-    <t>(52.975321,277.919902);(53.066112,278.222966);(53.154137,278.526845);(53.239519,278.831477);(53.322402,279.136800);(53.402930,279.442752);(53.481249,279.749278);(53.557504,280.056324);(53.631843,280.363840);(53.704412,280.671778);(53.775357,280.980095);(53.844827,281.288748);(53.912969,281.597698);(53.979929,281.906905);(54.045848,282.216337);(54.110839,282.525964);(54.174994,282.835767);(54.238403,283.145722);(54.301157,283.455812);(54.363346,283.766015);(54.425061,284.076312);(54.486393,284.386686);(54.547433,284.697117);(54.608272,285.007588);(54.669001,285.318080);(54.729712,285.628576);(54.790496,285.939058);(54.851444,286.249507);(54.912647,286.559906);(54.974196,286.870237);(55.036164,287.180484);(55.098546,287.490648);(55.161267,287.800744);(55.224242,288.110789);(55.287385,288.420799);(55.350609,288.730793);(55.413830,289.040788);(55.476961,289.350800);(55.539917,289.660849);(55.602611,289.970950);(55.664959,290.281121);(55.726873,290.591379);(55.788269,290.901740);(55.849059,291.212220);(55.909159,291.522835);(55.968480,291.833599);(56.026947,292.144525);(56.084532,292.455615);(56.141262,292.766862);(56.197173,293.078258);(56.252304,293.389792);(56.306693,293.701458);(56.360376,294.013245);(56.413392,294.325147);(56.465779,294.637155);(56.517574,294.949261);(56.568816,295.261459);(56.619542,295.573742);(56.669791,295.886101);(56.719599,296.198531);(56.769006,296.511025);(56.818049,296.823576);(56.866767,297.136178);(56.915196,297.448825);(56.963377,297.761510);(57.011343,298.074229);(57.059116,298.386976);(57.106689,298.699755);(57.154049,299.012565);(57.201183,299.325410);(57.248077,299.638291);(57.294717,299.951210);(57.341090,300.264168);(57.387182,300.577168);(57.432980,300.890211);</t>
+    <t>52.975321_277.919902;53.066112_278.222966;53.154137_278.526845;53.239519_278.831477;53.322402_279.136800;53.402930_279.442752;53.481249_279.749278;53.557504_280.056324;53.631843_280.363840;53.704412_280.671778;53.775357_280.980095;53.844827_281.288748;53.912969_281.597698;53.979929_281.906905;54.045848_282.216337;54.110839_282.525964;54.174994_282.835767;54.238403_283.145722;54.301157_283.455812;54.363346_283.766015;54.425061_284.076312;54.486393_284.386686;54.547433_284.697117;54.608272_285.007588;54.669001_285.318080;54.729712_285.628576;54.790496_285.939058;54.851444_286.249507;54.912647_286.559906;54.974196_286.870237;55.036164_287.180484;55.098546_287.490648;55.161267_287.800744;55.224242_288.110789;55.287385_288.420799;55.350609_288.730793;55.413830_289.040788;55.476961_289.350800;55.539917_289.660849;55.602611_289.970950;55.664959_290.281121;55.726873_290.591379;55.788269_290.901740;55.849059_291.212220;55.909159_291.522835;55.968480_291.833599;56.026947_292.144525;56.084532_292.455615;56.141262_292.766862;56.197173_293.078258;56.252304_293.389792;56.306693_293.701458;56.360376_294.013245;56.413392_294.325147;56.465779_294.637155;56.517574_294.949261;56.568816_295.261459;56.619542_295.573742;56.669791_295.886101;56.719599_296.198531;56.769006_296.511025;56.818049_296.823576;56.866767_297.136178;56.915196_297.448825;56.963377_297.761510;57.011343_298.074229;57.059116_298.386976;57.106689_298.699755;57.154049_299.012565;57.201183_299.325410;57.248077_299.638291;57.294717_299.951210;57.341090_300.264168;57.387182_300.577168;57.432980_300.890211;</t>
   </si>
   <si>
-    <t>(57.523638,301.516434);(57.568471,301.829617);(57.612955,302.142849);(57.657076,302.456133);(57.700821,302.769469);(57.744176,303.082860);(57.787128,303.396306);(57.829662,303.709810);(57.871765,304.023371);(57.913423,304.336992);(57.954623,304.650673);(57.995350,304.964416);(58.035591,305.278222);(58.075332,305.592091);(58.114560,305.906025);(58.153260,306.220025);(58.191419,306.534091);(58.229023,306.848223);(58.266058,307.162423);(58.302510,307.476692);(58.338366,307.791029);(58.373611,308.105435);(58.408232,308.419910);(58.442215,308.734455);(58.475546,309.049070);(58.508211,309.363754);(58.540196,309.678508);(58.571487,309.993332);(58.602071,310.308226);(58.631934,310.623189);(58.661061,310.938220);(58.689439,311.253320);(58.717054,311.568488);(58.743893,311.883722);(58.769940,312.199024);(58.795184,312.514390);(58.819608,312.829821);(58.843201,313.145315);(58.865948,313.460872);(58.887835,313.776489);(58.908849,314.092165);(58.928976,314.407899);(58.948202,314.723690);(58.966513,315.039535);(58.983897,315.355432);(59.000338,315.671379);(59.015825,315.987375);(59.030343,316.303417);(59.043879,316.619502);(59.056419,316.935628);(59.067950,317.251793);(59.078459,317.567994);(59.087932,317.884227);(59.096357,318.200489);(59.103720,318.516779);(59.110009,318.833091);(59.115209,319.149423);(59.119309,319.465771);(59.122295,319.782132);(59.124155,320.098502);(59.124876,320.414876);(59.124446,320.731250);(59.122852,321.047621);(59.120082,321.363984);(59.116123,321.680334);(59.110964,321.996666);(59.104592,322.312977);(59.096996,322.629260);(59.088164,322.945512);(59.078084,323.261726);(59.066745,323.577897);(59.054135,323.894020);(59.040244,324.210090);(59.025059,324.526100);(59.008571,324.842045);</t>
+    <t>57.523638_301.516434;57.568471_301.829617;57.612955_302.142849;57.657076_302.456133;57.700821_302.769469;57.744176_303.082860;57.787128_303.396306;57.829662_303.709810;57.871765_304.023371;57.913423_304.336992;57.954623_304.650673;57.995350_304.964416;58.035591_305.278222;58.075332_305.592091;58.114560_305.906025;58.153260_306.220025;58.191419_306.534091;58.229023_306.848223;58.266058_307.162423;58.302510_307.476692;58.338366_307.791029;58.373611_308.105435;58.408232_308.419910;58.442215_308.734455;58.475546_309.049070;58.508211_309.363754;58.540196_309.678508;58.571487_309.993332;58.602071_310.308226;58.631934_310.623189;58.661061_310.938220;58.689439_311.253320;58.717054_311.568488;58.743893_311.883722;58.769940_312.199024;58.795184_312.514390;58.819608_312.829821;58.843201_313.145315;58.865948_313.460872;58.887835_313.776489;58.908849_314.092165;58.928976_314.407899;58.948202_314.723690;58.966513_315.039535;58.983897_315.355432;59.000338_315.671379;59.015825_315.987375;59.030343_316.303417;59.043879_316.619502;59.056419_316.935628;59.067950_317.251793;59.078459_317.567994;59.087932_317.884227;59.096357_318.200489;59.103720_318.516779;59.110009_318.833091;59.115209_319.149423;59.119309_319.465771;59.122295_319.782132;59.124155_320.098502;59.124876_320.414876;59.124446_320.731250;59.122852_321.047621;59.120082_321.363984;59.116123_321.680334;59.110964_321.996666;59.104592_322.312977;59.096996_322.629260;59.088164_322.945512;59.078084_323.261726;59.066745_323.577897;59.054135_323.894020;59.040244_324.210090;59.025059_324.526100;59.008571_324.842045;</t>
   </si>
   <si>
-    <t>(58.948500,325.142382);(58.850761,325.428938);(58.764025,325.719004);(58.689272,326.012373);(58.627528,326.308739);(58.579840,326.607673);(58.547244,326.908612);(58.530719,327.210844);(58.531132,327.513513);(58.549183,327.815631);(58.585340,328.116112);(58.639798,328.413816);(58.712449,328.707610);(58.802881,328.996433);(58.910400,329.279351);(59.034079,329.555602);(59.172819,329.824621);(59.325414,330.086051);(59.490614,330.339723);(59.667176,330.585643);(59.853902,330.823955);(60.049667,331.054917);(60.253430,331.278870);(60.464242,331.496216);(60.681244,331.707393);(60.903664,331.912867);(61.130246,332.113768);(61.357425,332.314002);(61.579276,332.520002);(61.788617,332.738430);(61.976721,332.974984);(62.137306,333.230978);(62.273114,333.501320);(62.393315,333.779192);(62.507710,334.059584);(62.625982,334.338310);(62.757805,334.610686);(62.912601,334.870300);(63.096580,335.109826);(63.305357,335.328666);(63.526608,335.535364);(63.748412,335.741488);(63.958521,335.959067);(64.145229,336.196597);(64.304938,336.453304);(64.442623,336.722757);(64.565765,336.999340);(64.682148,337.278910);(64.798913,337.558317);(64.922179,337.834866);(65.057160,338.105797);(65.210058,338.366785);(65.389928,338.609273);(65.608106,338.815816);(65.871133,338.954522);(66.165076,339.000152);(66.466699,338.982110);(66.768019,338.970928);(67.051279,339.045719);(67.284153,339.228359);(67.472645,339.464491);(67.655635,339.705461);(67.872767,339.910667);(68.143923,340.018900);(68.443583,340.025924);(68.745262,340.001883);(69.043166,340.023511);(69.315275,340.139435);(69.541755,340.335762);(69.729272,340.572446);(69.894417,340.826076);(70.051378,341.085047);(70.212431,341.341402);(70.390726,341.585527);(70.602253,341.799370);</t>
+    <t>58.948500_325.142382;58.850761_325.428938;58.764025_325.719004;58.689272_326.012373;58.627528_326.308739;58.579840_326.607673;58.547244_326.908612;58.530719_327.210844;58.531132_327.513513;58.549183_327.815631;58.585340_328.116112;58.639798_328.413816;58.712449_328.707610;58.802881_328.996433;58.910400_329.279351;59.034079_329.555602;59.172819_329.824621;59.325414_330.086051;59.490614_330.339723;59.667176_330.585643;59.853902_330.823955;60.049667_331.054917;60.253430_331.278870;60.464242_331.496216;60.681244_331.707393;60.903664_331.912867;61.130246_332.113768;61.357425_332.314002;61.579276_332.520002;61.788617_332.738430;61.976721_332.974984;62.137306_333.230978;62.273114_333.501320;62.393315_333.779192;62.507710_334.059584;62.625982_334.338310;62.757805_334.610686;62.912601_334.870300;63.096580_335.109826;63.305357_335.328666;63.526608_335.535364;63.748412_335.741488;63.958521_335.959067;64.145229_336.196597;64.304938_336.453304;64.442623_336.722757;64.565765_336.999340;64.682148_337.278910;64.798913_337.558317;64.922179_337.834866;65.057160_338.105797;65.210058_338.366785;65.389928_338.609273;65.608106_338.815816;65.871133_338.954522;66.165076_339.000152;66.466699_338.982110;66.768019_338.970928;67.051279_339.045719;67.284153_339.228359;67.472645_339.464491;67.655635_339.705461;67.872767_339.910667;68.143923_340.018900;68.443583_340.025924;68.745262_340.001883;69.043166_340.023511;69.315275_340.139435;69.541755_340.335762;69.729272_340.572446;69.894417_340.826076;70.051378_341.085047;70.212431_341.341402;70.390726_341.585527;70.602253_341.799370;</t>
   </si>
   <si>
-    <t>(71.151679,342.000382);(71.453313,341.984803);(71.754843,341.971935);(72.041239,342.038752);(72.280607,342.212248);(72.474203,342.443920);(72.657608,342.684729);(72.868467,342.898215);(73.131642,343.028311);(73.428777,343.056725);(73.730091,343.030796);(74.031340,343.002071);(74.333727,342.995511);(74.636442,343.002918);(74.938943,342.999498);(75.240421,342.973797);(75.541777,342.946739);(75.840585,342.966337);(76.110621,343.082600);(76.330173,343.286197);(76.517966,343.523457);(76.709159,343.757677);(76.938448,343.948108);(77.216663,344.044150);(77.517109,344.050051);(77.818327,344.020015);(78.119997,343.997777);(78.422609,343.997921);(78.725325,344.004482);(79.027568,343.993957);(79.328799,343.964037);(79.630332,343.944872);(79.924326,343.989618);(80.180299,344.135592);(80.386948,344.354407);(80.572142,344.593916);(80.771067,344.820774);(81.015778,344.987141);(81.304168,345.053002);(81.605605,345.042655);(81.906757,345.011417);(82.208763,344.995664);(82.511460,345.000220);(82.814146,345.003903);(83.116079,344.986601);(83.417253,344.955547);(83.718576,344.948949);(84.004814,345.022061);(84.246095,345.194329);(84.443382,345.422857);(84.629251,345.661821);(84.838486,345.877864);(85.097194,346.018933);(85.392177,346.059893);(85.693548,346.038459);(85.994292,346.003445);(86.296146,345.982923);(86.598815,345.982502);(86.901359,345.994804);(87.203790,346.010320);(87.506419,346.019187);(87.808960,346.012388);(88.110340,345.985210);(88.411124,345.950665);(88.712336,345.944566);(88.998417,346.018835);(89.239745,346.191267);(89.437364,346.419515);(89.623515,346.658263);(89.832655,346.874481);(90.090960,347.016468);(90.385728,347.058506);(90.687160,347.037924);(90.988045,347.004224);(91.290018,346.985817);</t>
+    <t>71.151679_342.000382;71.453313_341.984803;71.754843_341.971935;72.041239_342.038752;72.280607_342.212248;72.474203_342.443920;72.657608_342.684729;72.868467_342.898215;73.131642_343.028311;73.428777_343.056725;73.730091_343.030796;74.031340_343.002071;74.333727_342.995511;74.636442_343.002918;74.938943_342.999498;75.240421_342.973797;75.541777_342.946739;75.840585_342.966337;76.110621_343.082600;76.330173_343.286197;76.517966_343.523457;76.709159_343.757677;76.938448_343.948108;77.216663_344.044150;77.517109_344.050051;77.818327_344.020015;78.119997_343.997777;78.422609_343.997921;78.725325_344.004482;79.027568_343.993957;79.328799_343.964037;79.630332_343.944872;79.924326_343.989618;80.180299_344.135592;80.386948_344.354407;80.572142_344.593916;80.771067_344.820774;81.015778_344.987141;81.304168_345.053002;81.605605_345.042655;81.906757_345.011417;82.208763_344.995664;82.511460_345.000220;82.814146_345.003903;83.116079_344.986601;83.417253_344.955547;83.718576_344.948949;84.004814_345.022061;84.246095_345.194329;84.443382_345.422857;84.629251_345.661821;84.838486_345.877864;85.097194_346.018933;85.392177_346.059893;85.693548_346.038459;85.994292_346.003445;86.296146_345.982923;86.598815_345.982502;86.901359_345.994804;87.203790_346.010320;87.506419_346.019187;87.808960_346.012388;88.110340_345.985210;88.411124_345.950665;88.712336_345.944566;88.998417_346.018835;89.239745_346.191267;89.437364_346.419515;89.623515_346.658263;89.832655_346.874481;90.090960_347.016468;90.385728_347.058506;90.687160_347.037924;90.988045_347.004224;91.290018_346.985817;</t>
   </si>
   <si>
-    <t>(91.895407,346.996020);(92.198138,347.002968);(92.500957,347.004008);(92.803782,347.001825);(93.106607,346.999600);(93.409440,346.998881);(93.712274,346.999300);(94.015108,346.999958);(94.317942,347.000271);(94.620777,347.000219);(94.923611,347.000054);(95.226446,346.999977);(95.529280,347.000004);(95.832115,347.000019);(96.134950,346.999917);(96.437784,346.999754);(96.740619,346.999753);(97.043453,347.000152);(97.346287,347.000828);(97.649121,347.001098);(97.951952,347.000066);(98.254777,346.997659);(98.557603,346.995829);(98.860412,346.997897);(99.163122,347.005854);(99.465814,347.014552);(99.768476,347.012378);(100.070189,346.989939);(100.371033,346.955724);(100.672461,346.942833);(100.962635,347.003196);(101.211068,347.163546);(101.412896,347.387571);(101.598513,347.626770);(101.802448,347.848608);(102.053988,348.003389);(102.345741,348.057886);(102.647195,348.042368);(102.948041,348.008175);(103.249836,347.986965);(103.552516,347.985789);(103.855204,347.994741);(104.157920,348.002404);(104.460733,348.004138);(104.763559,348.002182);(105.066383,347.999822);(105.369215,347.998886);(105.672049,347.999205);(105.974883,347.999884);(106.277717,348.000269);(106.580552,348.000260);(106.883386,348.000083);(107.186221,347.999946);(107.489055,347.999922);(107.791890,347.999963);(108.094725,348.000007);(108.397559,348.000022);(108.700394,348.000014);(109.003229,348.000001);(109.306063,347.999995);(109.608898,347.999995);(109.911732,347.999999);(110.214567,348.000001);(110.517402,348.000001);(110.820236,348.000001);(111.123071,348.000000);(111.425906,348.000000);(111.728740,348.000000);(112.031575,348.000000);(112.334410,348.000000);(112.637244,348.000000);(112.940079,348.000000);(113.242913,348.000000);(113.545748,348.000000);(113.848583,348.000000);</t>
+    <t>91.895407_346.996020;92.198138_347.002968;92.500957_347.004008;92.803782_347.001825;93.106607_346.999600;93.409440_346.998881;93.712274_346.999300;94.015108_346.999958;94.317942_347.000271;94.620777_347.000219;94.923611_347.000054;95.226446_346.999977;95.529280_347.000004;95.832115_347.000019;96.134950_346.999917;96.437784_346.999754;96.740619_346.999753;97.043453_347.000152;97.346287_347.000828;97.649121_347.001098;97.951952_347.000066;98.254777_346.997659;98.557603_346.995829;98.860412_346.997897;99.163122_347.005854;99.465814_347.014552;99.768476_347.012378;100.070189_346.989939;100.371033_346.955724;100.672461_346.942833;100.962635_347.003196;101.211068_347.163546;101.412896_347.387571;101.598513_347.626770;101.802448_347.848608;102.053988_348.003389;102.345741_348.057886;102.647195_348.042368;102.948041_348.008175;103.249836_347.986965;103.552516_347.985789;103.855204_347.994741;104.157920_348.002404;104.460733_348.004138;104.763559_348.002182;105.066383_347.999822;105.369215_347.998886;105.672049_347.999205;105.974883_347.999884;106.277717_348.000269;106.580552_348.000260;106.883386_348.000083;107.186221_347.999946;107.489055_347.999922;107.791890_347.999963;108.094725_348.000007;108.397559_348.000022;108.700394_348.000014;109.003229_348.000001;109.306063_347.999995;109.608898_347.999995;109.911732_347.999999;110.214567_348.000001;110.517402_348.000001;110.820236_348.000001;111.123071_348.000000;111.425906_348.000000;111.728740_348.000000;112.031575_348.000000;112.334410_348.000000;112.637244_348.000000;112.940079_348.000000;113.242913_348.000000;113.545748_348.000000;113.848583_348.000000;</t>
   </si>
   <si>
-    <t>(156.752786,291.961942);(156.255431,291.961438);(155.755233,292.037185);(155.257426,292.040058);(154.821550,291.838508);(154.477511,291.472929);(154.123473,291.120932);(153.675031,290.949562);(153.175135,290.972489);(152.674837,291.046720);(152.181463,291.022288);(151.760915,290.786970);(151.425361,290.410787);(151.057610,290.079159);(150.595830,289.942995);(150.094943,289.984727);(149.594356,290.053888);(149.107809,289.998611);(148.703122,289.731306);(148.372278,289.349590);(147.989363,289.042709);(147.515809,288.941489);(147.014816,288.997594);(146.513903,289.057953);(146.036457,288.969433);(145.647722,288.672659);(145.317620,288.290094);(144.918849,288.011556);(144.435415,287.944206);(143.934700,288.010558);(143.433700,288.058106);(142.967364,287.934942);(142.594123,287.612004);(142.260765,287.233209);(141.846050,286.985794);(141.354931,286.950291);(140.854553,287.023130);(140.354164,287.053603);(139.900784,286.895047);(139.542182,286.549725);(139.201634,286.179755);(138.770953,285.966736);(138.274186,285.960142);(137.773371,286.031816);(137.273660,286.039051);(136.824376,285.858577);(136.463662,285.511545);(136.124476,285.137684);(135.708004,284.891559);(135.234981,284.911926);</t>
+    <t>156.752786_291.961942;156.255431_291.961438;155.755233_292.037185;155.257426_292.040058;154.821550_291.838508;154.477511_291.472929;154.123473_291.120932;153.675031_290.949562;153.175135_290.972489;152.674837_291.046720;152.181463_291.022288;151.760915_290.786970;151.425361_290.410787;151.057610_290.079159;150.595830_289.942995;150.094943_289.984727;149.594356_290.053888;149.107809_289.998611;148.703122_289.731306;148.372278_289.349590;147.989363_289.042709;147.515809_288.941489;147.014816_288.997594;146.513903_289.057953;146.036457_288.969433;145.647722_288.672659;145.317620_288.290094;144.918849_288.011556;144.435415_287.944206;143.934700_288.010558;143.433700_288.058106;142.967364_287.934942;142.594123_287.612004;142.260765_287.233209;141.846050_286.985794;141.354931_286.950291;140.854553_287.023130;140.354164_287.053603;139.900784_286.895047;139.542182_286.549725;139.201634_286.179755;138.770953_285.966736;138.274186_285.960142;137.773371_286.031816;137.273660_286.039051;136.824376_285.858577;136.463662_285.511545;136.124476_285.137684;135.708004_284.891559;135.234981_284.911926;</t>
   </si>
   <si>
-    <t>(134.000000,284.898026);(134.000000,284.694079);(134.000000,284.490132);(134.000000,284.286184);(134.000000,284.082237);(134.000000,283.878289);(134.000000,283.674342);(134.000000,283.470395);(134.000000,283.266447);(134.000000,283.062500);(134.000000,282.858553);(134.000000,282.654605);(134.000000,282.450658);(134.000000,282.246711);(134.000000,282.042763);(134.000000,281.838816);(134.000000,281.634868);(134.000000,281.430921);(134.000000,281.226974);(134.000000,281.023026);(134.000000,280.819079);(134.000000,280.615132);(134.000000,280.411184);(134.000000,280.207237);(134.000000,280.003289);(134.000000,279.799342);(134.000000,279.595395);(134.000000,279.391447);(134.000000,279.187500);(134.000000,278.983553);(134.000000,278.779605);(134.000000,278.575658);(134.000000,278.371711);(134.000000,278.167763);(134.000000,277.963816);(134.000000,277.759868);(134.000000,277.555921);(134.000000,277.351974);(134.000000,277.148026);(134.000000,276.944079);(134.000000,276.740132);(134.000000,276.536184);(134.000000,276.332237);(134.000000,276.128289);(134.000000,275.924342);(134.000000,275.720395);(134.000000,275.516447);(134.000000,275.312500);(134.000000,275.108553);(134.000000,274.904605);</t>
+    <t>134.000000_284.898026;134.000000_284.694079;134.000000_284.490132;134.000000_284.286184;134.000000_284.082237;134.000000_283.878289;134.000000_283.674342;134.000000_283.470395;134.000000_283.266447;134.000000_283.062500;134.000000_282.858553;134.000000_282.654605;134.000000_282.450658;134.000000_282.246711;134.000000_282.042763;134.000000_281.838816;134.000000_281.634868;134.000000_281.430921;134.000000_281.226974;134.000000_281.023026;134.000000_280.819079;134.000000_280.615132;134.000000_280.411184;134.000000_280.207237;134.000000_280.003289;134.000000_279.799342;134.000000_279.595395;134.000000_279.391447;134.000000_279.187500;134.000000_278.983553;134.000000_278.779605;134.000000_278.575658;134.000000_278.371711;134.000000_278.167763;134.000000_277.963816;134.000000_277.759868;134.000000_277.555921;134.000000_277.351974;134.000000_277.148026;134.000000_276.944079;134.000000_276.740132;134.000000_276.536184;134.000000_276.332237;134.000000_276.128289;134.000000_275.924342;134.000000_275.720395;134.000000_275.516447;134.000000_275.312500;134.000000_275.108553;134.000000_274.904605;</t>
   </si>
   <si>
-    <t>(134.000000,274.904605);(134.000000,274.700658);(134.000000,274.496711);(134.000000,274.292763);(134.000000,274.088816);(134.000000,273.884868);(134.000000,273.680921);(134.000000,273.476974);(134.000000,273.273026);(134.000000,273.069079);(134.000000,272.865132);(134.000000,272.661184);(134.000000,272.457237);(134.000000,272.253289);(134.000000,272.049342);(134.000000,271.845395);(134.000000,271.641447);(134.000000,271.437500);(134.000000,271.233553);(134.000000,271.029605);(134.000000,270.825658);(134.000000,270.621711);(134.000000,270.417763);(134.000000,270.213816);(134.000000,270.009868);(134.000000,269.805921);(134.000000,269.601974);(134.000000,269.398026);(134.000000,269.194079);(134.000000,268.990132);(134.000000,268.786184);(134.000000,268.582237);(134.000000,268.378289);(134.000000,268.174342);(134.000000,267.970395);(134.000000,267.766447);(134.000000,267.562500);(134.000000,267.358553);(134.000000,267.154605);(134.000000,266.950658);(134.000000,266.746711);(134.000000,266.542763);(134.000000,266.338816);(134.000000,266.134868);(134.000000,265.930921);(134.000000,265.726974);(134.000000,265.523026);(134.000000,265.319079);(134.000000,265.115132);(134.000000,264.911184);</t>
+    <t>134.000000_274.904605;134.000000_274.700658;134.000000_274.496711;134.000000_274.292763;134.000000_274.088816;134.000000_273.884868;134.000000_273.680921;134.000000_273.476974;134.000000_273.273026;134.000000_273.069079;134.000000_272.865132;134.000000_272.661184;134.000000_272.457237;134.000000_272.253289;134.000000_272.049342;134.000000_271.845395;134.000000_271.641447;134.000000_271.437500;134.000000_271.233553;134.000000_271.029605;134.000000_270.825658;134.000000_270.621711;134.000000_270.417763;134.000000_270.213816;134.000000_270.009868;134.000000_269.805921;134.000000_269.601974;134.000000_269.398026;134.000000_269.194079;134.000000_268.990132;134.000000_268.786184;134.000000_268.582237;134.000000_268.378289;134.000000_268.174342;134.000000_267.970395;134.000000_267.766447;134.000000_267.562500;134.000000_267.358553;134.000000_267.154605;134.000000_266.950658;134.000000_266.746711;134.000000_266.542763;134.000000_266.338816;134.000000_266.134868;134.000000_265.930921;134.000000_265.726974;134.000000_265.523026;134.000000_265.319079;134.000000_265.115132;134.000000_264.911184;</t>
   </si>
   <si>
-    <t>(134.000000,264.911184);(134.000000,264.707237);(134.000000,264.503289);(134.000000,264.299342);(134.000000,264.095395);(134.000000,263.891447);(134.000000,263.687500);(134.000000,263.483553);(134.000000,263.279605);(134.000000,263.075658);(134.000000,262.871711);(134.000000,262.667763);(134.000000,262.463816);(134.000000,262.259868);(134.000000,262.055921);(134.000000,261.851974);(134.000000,261.648026);(134.000000,261.444079);(134.000000,261.240132);(134.000000,261.036184);(134.000000,260.832237);(134.000000,260.628289);(134.000000,260.424342);(134.000000,260.220395);(134.000000,260.016447);(134.000000,259.812500);(134.000000,259.608553);(134.000000,259.404605);(134.000000,259.200658);(134.000000,258.996711);(134.000000,258.792763);(134.000000,258.588816);(134.000000,258.384868);(134.000000,258.180921);(134.000000,257.976974);(134.000000,257.773026);(134.000000,257.569079);(134.000000,257.365132);(134.000000,257.161184);(134.000000,256.957237);(134.000000,256.753289);(134.000000,256.549342);(134.000000,256.345395);(134.000000,256.141447);(134.000000,255.937500);(134.000000,255.733553);(134.000000,255.529605);(134.000000,255.325658);(134.000000,255.121711);(134.000000,254.917763);</t>
+    <t>134.000000_264.911184;134.000000_264.707237;134.000000_264.503289;134.000000_264.299342;134.000000_264.095395;134.000000_263.891447;134.000000_263.687500;134.000000_263.483553;134.000000_263.279605;134.000000_263.075658;134.000000_262.871711;134.000000_262.667763;134.000000_262.463816;134.000000_262.259868;134.000000_262.055921;134.000000_261.851974;134.000000_261.648026;134.000000_261.444079;134.000000_261.240132;134.000000_261.036184;134.000000_260.832237;134.000000_260.628289;134.000000_260.424342;134.000000_260.220395;134.000000_260.016447;134.000000_259.812500;134.000000_259.608553;134.000000_259.404605;134.000000_259.200658;134.000000_258.996711;134.000000_258.792763;134.000000_258.588816;134.000000_258.384868;134.000000_258.180921;134.000000_257.976974;134.000000_257.773026;134.000000_257.569079;134.000000_257.365132;134.000000_257.161184;134.000000_256.957237;134.000000_256.753289;134.000000_256.549342;134.000000_256.345395;134.000000_256.141447;134.000000_255.937500;134.000000_255.733553;134.000000_255.529605;134.000000_255.325658;134.000000_255.121711;134.000000_254.917763;</t>
   </si>
   <si>
-    <t>(135.235613,254.098512);(135.709845,254.120834);(136.118854,253.852119);(136.448371,253.456996);(136.823844,253.123109);(137.296845,253.002927);(137.807212,252.995066);(138.248678,252.803154);(138.591335,252.424246);(138.956742,252.078034);(139.423514,251.939464);(139.933190,251.988326);(140.442855,252.056521);(140.932917,251.981486);(141.334926,251.690706);(141.672093,251.301950);(142.076058,251.014781);(142.567245,250.943905);(143.076820,251.013444);(143.586378,251.060551);(144.050818,250.916679);(144.413084,250.566307);(144.756936,250.189502);(145.201182,250.006875);(145.711886,250.001443);(146.172809,249.859565);(146.531043,249.503684);(146.878369,249.131583);(147.326549,248.946889);(147.834783,248.972346);(148.343984,249.049122);(148.843847,249.013954);(149.265443,248.761156);(149.605363,248.375627);(149.990032,248.054415);(150.468515,247.941166);(150.978418,247.996976);(151.488085,248.061244);(151.968423,247.962589);(152.350041,247.643484);(152.683305,247.253096);(153.107715,247.024695);(153.613051,247.003078);(154.090898,246.904670);(154.468642,246.581531);(154.803829,246.193471);(155.231986,245.963345);(155.735787,245.957308);(156.244290,246.039948);(156.749225,246.040963);</t>
+    <t>135.235613_254.098512;135.709845_254.120834;136.118854_253.852119;136.448371_253.456996;136.823844_253.123109;137.296845_253.002927;137.807212_252.995066;138.248678_252.803154;138.591335_252.424246;138.956742_252.078034;139.423514_251.939464;139.933190_251.988326;140.442855_252.056521;140.932917_251.981486;141.334926_251.690706;141.672093_251.301950;142.076058_251.014781;142.567245_250.943905;143.076820_251.013444;143.586378_251.060551;144.050818_250.916679;144.413084_250.566307;144.756936_250.189502;145.201182_250.006875;145.711886_250.001443;146.172809_249.859565;146.531043_249.503684;146.878369_249.131583;147.326549_248.946889;147.834783_248.972346;148.343984_249.049122;148.843847_249.013954;149.265443_248.761156;149.605363_248.375627;149.990032_248.054415;150.468515_247.941166;150.978418_247.996976;151.488085_248.061244;151.968423_247.962589;152.350041_247.643484;152.683305_247.253096;153.107715_247.024695;153.613051_247.003078;154.090898_246.904670;154.468642_246.581531;154.803829_246.193471;155.231986_245.963345;155.735787_245.957308;156.244290_246.039948;156.749225_246.040963;</t>
   </si>
   <si>
-    <t>(156.749225,208.959037);(156.244290,208.960052);(155.735787,209.042692);(155.231986,209.036655);(154.803829,208.806529);(154.468642,208.418469);(154.090898,208.095330);(153.613051,207.996922);(153.107715,207.975305);(152.683305,207.746904);(152.350041,207.356516);(151.968423,207.037411);(151.488085,206.938756);(150.978418,207.003024);(150.468515,207.058834);(149.990032,206.945585);(149.605363,206.624373);(149.265443,206.238844);(148.843847,205.986046);(148.343984,205.950878);(147.834783,206.027654);(147.326549,206.053111);(146.878369,205.868417);(146.531043,205.496316);(146.172809,205.140435);(145.711886,204.998557);(145.201182,204.993125);(144.756936,204.810498);(144.413084,204.433693);(144.050818,204.083321);(143.586378,203.939449);(143.076820,203.986556);(142.567245,204.056095);(142.076058,203.985219);(141.672093,203.698050);(141.334926,203.309294);(140.932917,203.018514);(140.442855,202.943479);(139.933190,203.011674);(139.423514,203.060536);(138.956742,202.921966);(138.591335,202.575754);(138.248678,202.196846);(137.807212,202.004934);(137.296845,201.997073);(136.823844,201.876891);(136.448371,201.543004);(136.118854,201.147881);(135.709845,200.879166);(135.235613,200.901488);</t>
+    <t>156.749225_208.959037;156.244290_208.960052;155.735787_209.042692;155.231986_209.036655;154.803829_208.806529;154.468642_208.418469;154.090898_208.095330;153.613051_207.996922;153.107715_207.975305;152.683305_207.746904;152.350041_207.356516;151.968423_207.037411;151.488085_206.938756;150.978418_207.003024;150.468515_207.058834;149.990032_206.945585;149.605363_206.624373;149.265443_206.238844;148.843847_205.986046;148.343984_205.950878;147.834783_206.027654;147.326549_206.053111;146.878369_205.868417;146.531043_205.496316;146.172809_205.140435;145.711886_204.998557;145.201182_204.993125;144.756936_204.810498;144.413084_204.433693;144.050818_204.083321;143.586378_203.939449;143.076820_203.986556;142.567245_204.056095;142.076058_203.985219;141.672093_203.698050;141.334926_203.309294;140.932917_203.018514;140.442855_202.943479;139.933190_203.011674;139.423514_203.060536;138.956742_202.921966;138.591335_202.575754;138.248678_202.196846;137.807212_202.004934;137.296845_201.997073;136.823844_201.876891;136.448371_201.543004;136.118854_201.147881;135.709845_200.879166;135.235613_200.901488;</t>
   </si>
   <si>
-    <t>(134.000000,200.904605);(134.000000,200.713816);(134.000000,200.523026);(134.000000,200.332237);(134.000000,200.141447);(134.000000,199.950658);(134.000000,199.759868);(134.000000,199.569079);(134.000000,199.378289);(134.000000,199.187500);(134.000000,198.996711);(134.000000,198.805921);(134.000000,198.615132);(134.000000,198.424342);(134.000000,198.233553);(134.000000,198.042763);(134.000000,197.851974);(134.000000,197.661184);(134.000000,197.470395);(134.000000,197.279605);(134.000000,197.088816);(134.000000,196.898026);(134.000000,196.707237);(134.000000,196.516447);(134.000000,196.325658);(134.000000,196.134868);(134.000000,195.944079);(134.000000,195.753289);(134.000000,195.562500);(134.000000,195.371711);(134.000000,195.180921);(134.000000,194.990132);(134.000000,194.799342);(134.000000,194.608553);(134.000000,194.417763);(134.000000,194.226974);(134.000000,194.036184);(134.000000,193.845395);(134.000000,193.654605);(134.000000,193.463816);(134.000000,193.273026);(134.000000,193.082237);(134.000000,192.891447);(134.000000,192.700658);(134.000000,192.509868);(134.000000,192.319079);(134.000000,192.128289);(134.000000,191.937500);(134.000000,191.746711);(134.000000,191.555921);</t>
+    <t>134.000000_200.904605;134.000000_200.713816;134.000000_200.523026;134.000000_200.332237;134.000000_200.141447;134.000000_199.950658;134.000000_199.759868;134.000000_199.569079;134.000000_199.378289;134.000000_199.187500;134.000000_198.996711;134.000000_198.805921;134.000000_198.615132;134.000000_198.424342;134.000000_198.233553;134.000000_198.042763;134.000000_197.851974;134.000000_197.661184;134.000000_197.470395;134.000000_197.279605;134.000000_197.088816;134.000000_196.898026;134.000000_196.707237;134.000000_196.516447;134.000000_196.325658;134.000000_196.134868;134.000000_195.944079;134.000000_195.753289;134.000000_195.562500;134.000000_195.371711;134.000000_195.180921;134.000000_194.990132;134.000000_194.799342;134.000000_194.608553;134.000000_194.417763;134.000000_194.226974;134.000000_194.036184;134.000000_193.845395;134.000000_193.654605;134.000000_193.463816;134.000000_193.273026;134.000000_193.082237;134.000000_192.891447;134.000000_192.700658;134.000000_192.509868;134.000000_192.319079;134.000000_192.128289;134.000000_191.937500;134.000000_191.746711;134.000000_191.555921;</t>
   </si>
   <si>
-    <t>(134.000000,191.555921);(134.000000,191.365132);(134.000000,191.174342);(134.000000,190.983553);(134.000000,190.792763);(134.000000,190.601974);(134.000000,190.411184);(134.000000,190.220395);(134.000000,190.029605);(134.000000,189.838816);(134.000000,189.648026);(134.000000,189.457237);(134.000000,189.266447);(134.000000,189.075658);(134.000000,188.884868);(134.000000,188.694079);(134.000000,188.503289);(134.000000,188.312500);(134.000000,188.121711);(134.000000,187.930921);(134.000000,187.740132);(134.000000,187.549342);(134.000000,187.358553);(134.000000,187.167763);(134.000000,186.976974);(134.000000,186.786184);(134.000000,186.595395);(134.000000,186.404605);(134.000000,186.213816);(134.000000,186.023026);(134.000000,185.832237);(134.000000,185.641447);(134.000000,185.450658);(134.000000,185.259868);(134.000000,185.069079);(134.000000,184.878289);(134.000000,184.687500);(134.000000,184.496711);(134.000000,184.305921);(134.000000,184.115132);(134.000000,183.924342);(134.000000,183.733553);(134.000000,183.542763);(134.000000,183.351974);(134.000000,183.161184);(134.000000,182.970395);(134.000000,182.779605);(134.000000,182.588816);(134.000000,182.398026);(134.000000,182.207237);</t>
+    <t>134.000000_191.555921;134.000000_191.365132;134.000000_191.174342;134.000000_190.983553;134.000000_190.792763;134.000000_190.601974;134.000000_190.411184;134.000000_190.220395;134.000000_190.029605;134.000000_189.838816;134.000000_189.648026;134.000000_189.457237;134.000000_189.266447;134.000000_189.075658;134.000000_188.884868;134.000000_188.694079;134.000000_188.503289;134.000000_188.312500;134.000000_188.121711;134.000000_187.930921;134.000000_187.740132;134.000000_187.549342;134.000000_187.358553;134.000000_187.167763;134.000000_186.976974;134.000000_186.786184;134.000000_186.595395;134.000000_186.404605;134.000000_186.213816;134.000000_186.023026;134.000000_185.832237;134.000000_185.641447;134.000000_185.450658;134.000000_185.259868;134.000000_185.069079;134.000000_184.878289;134.000000_184.687500;134.000000_184.496711;134.000000_184.305921;134.000000_184.115132;134.000000_183.924342;134.000000_183.733553;134.000000_183.542763;134.000000_183.351974;134.000000_183.161184;134.000000_182.970395;134.000000_182.779605;134.000000_182.588816;134.000000_182.398026;134.000000_182.207237;</t>
   </si>
   <si>
-    <t>(134.000000,182.207237);(134.000000,182.016447);(134.000000,181.825658);(134.000000,181.634868);(134.000000,181.444079);(134.000000,181.253289);(134.000000,181.062500);(134.000000,180.871711);(134.000000,180.680921);(134.000000,180.490132);(134.000000,180.299342);(134.000000,180.108553);(134.000000,179.917763);(134.000000,179.726974);(134.000000,179.536184);(134.000000,179.345395);(134.000000,179.154605);(134.000000,178.963816);(134.000000,178.773026);(134.000000,178.582237);(134.000000,178.391447);(134.000000,178.200658);(134.000000,178.009868);(134.000000,177.819079);(134.000000,177.628289);(134.000000,177.437500);(134.000000,177.246711);(134.000000,177.055921);(134.000000,176.865132);(134.000000,176.674342);(134.000000,176.483553);(134.000000,176.292763);(134.000000,176.101974);(134.000000,175.911184);(134.000000,175.720395);(134.000000,175.529605);(134.000000,175.338816);(134.000000,175.148026);(134.000000,174.957237);(134.000000,174.766447);(134.000000,174.575658);(134.000000,174.384868);(134.000000,174.194079);(134.000000,174.003289);(134.000000,173.812500);(134.000000,173.621711);(134.000000,173.430921);(134.000000,173.240132);(134.000000,173.049342);(134.000000,172.858553);</t>
+    <t>134.000000_182.207237;134.000000_182.016447;134.000000_181.825658;134.000000_181.634868;134.000000_181.444079;134.000000_181.253289;134.000000_181.062500;134.000000_180.871711;134.000000_180.680921;134.000000_180.490132;134.000000_180.299342;134.000000_180.108553;134.000000_179.917763;134.000000_179.726974;134.000000_179.536184;134.000000_179.345395;134.000000_179.154605;134.000000_178.963816;134.000000_178.773026;134.000000_178.582237;134.000000_178.391447;134.000000_178.200658;134.000000_178.009868;134.000000_177.819079;134.000000_177.628289;134.000000_177.437500;134.000000_177.246711;134.000000_177.055921;134.000000_176.865132;134.000000_176.674342;134.000000_176.483553;134.000000_176.292763;134.000000_176.101974;134.000000_175.911184;134.000000_175.720395;134.000000_175.529605;134.000000_175.338816;134.000000_175.148026;134.000000_174.957237;134.000000_174.766447;134.000000_174.575658;134.000000_174.384868;134.000000_174.194079;134.000000_174.003289;134.000000_173.812500;134.000000_173.621711;134.000000_173.430921;134.000000_173.240132;134.000000_173.049342;134.000000_172.858553;</t>
   </si>
   <si>
-    <t>(135.236776,171.960408);(135.713758,171.955928);(136.193463,172.031331);(136.673363,172.054162);(137.105177,171.891984);(137.445118,171.555059);(137.768118,171.195952);(138.178063,170.984731);(138.655123,170.965559);(139.139346,170.997298);(139.624835,170.998695);(140.109395,171.016722);(140.593164,171.044576);(141.042164,170.931043);(141.399657,170.622419);(141.713352,170.253068);(142.104826,170.005719);(142.574930,169.959212);(143.059068,169.993805);(143.544271,169.999543);(144.029132,170.011252);(144.513224,170.044456);(144.973430,169.964143);(145.346968,169.683013);(145.658358,169.311092);(146.033510,169.032870);(146.494718,168.955740);(146.978821,168.989248);(147.463713,169.000377);(147.948886,169.006605);(148.433025,169.041241);(148.902347,168.991836);(149.292200,168.741306);(149.605473,168.371483);(149.964535,168.065439);(150.414741,167.955313);(150.898570,167.983856);(151.383161,168.001076);(151.868612,168.002945);(152.352770,168.035699);(152.828988,168.013820);(153.235564,167.796930);(153.555592,167.434765);(153.898832,167.103571);(154.335215,166.955390);(154.817547,166.975849);(155.301334,167.013139);(155.786726,167.009394);(156.272131,166.988470);(156.757428,166.989316);</t>
+    <t>135.236776_171.960408;135.713758_171.955928;136.193463_172.031331;136.673363_172.054162;137.105177_171.891984;137.445118_171.555059;137.768118_171.195952;138.178063_170.984731;138.655123_170.965559;139.139346_170.997298;139.624835_170.998695;140.109395_171.016722;140.593164_171.044576;141.042164_170.931043;141.399657_170.622419;141.713352_170.253068;142.104826_170.005719;142.574930_169.959212;143.059068_169.993805;143.544271_169.999543;144.029132_170.011252;144.513224_170.044456;144.973430_169.964143;145.346968_169.683013;145.658358_169.311092;146.033510_169.032870;146.494718_168.955740;146.978821_168.989248;147.463713_169.000377;147.948886_169.006605;148.433025_169.041241;148.902347_168.991836;149.292200_168.741306;149.605473_168.371483;149.964535_168.065439;150.414741_167.955313;150.898570_167.983856;151.383161_168.001076;151.868612_168.002945;152.352770_168.035699;152.828988_168.013820;153.235564_167.796930;153.555592_167.434765;153.898832_167.103571;154.335215_166.955390;154.817547_166.975849;155.301334_167.013139;155.786726_167.009394;156.272131_166.988470;156.757428_166.989316;</t>
   </si>
   <si>
-    <t>(317.069017,146.529257);(317.220696,145.589970);(317.397424,144.655032);(317.594684,143.724176);(317.807926,142.796823);(318.032611,141.872157);(318.264226,140.949190);(318.498284,140.026835);(318.730313,139.103971);(318.955880,138.179518);(319.173472,137.253151);(319.389278,136.326360);(319.614761,135.401920);(319.861790,134.483102);(320.139321,133.573100);(320.441653,132.670876);(320.748280,131.770061);(321.036390,130.863311);(321.293871,129.947416);(321.525621,129.024556);(321.743764,128.098320);(321.960609,127.171774);(322.185104,126.247065);(322.417461,125.324285);(322.651991,124.402051);(322.882510,123.478816);(323.104295,122.553452);(323.320263,121.626697);(323.541154,120.701126);(323.779309,119.779928);(324.046112,118.866729);(324.341771,117.962358);(324.649588,117.061938);(324.946174,116.157862);(325.214392,115.245076);(325.453733,114.324191);(325.675082,113.398733);(325.890383,112.471822);(326.110266,111.546001);(326.338457,110.622188);(326.571713,109.699632);(326.805368,108.777176);(327.035029,107.853723);(327.259799,106.929064);(327.484149,106.004302);(327.714716,105.081086);(327.958157,104.161215);(328.221068,103.246768);(328.509893,102.340242);(328.830789,101.444650);</t>
+    <t>317.069017_146.529257;317.220696_145.589970;317.397424_144.655032;317.594684_143.724176;317.807926_142.796823;318.032611_141.872157;318.264226_140.949190;318.498284_140.026835;318.730313_139.103971;318.955880_138.179518;319.173472_137.253151;319.389278_136.326360;319.614761_135.401920;319.861790_134.483102;320.139321_133.573100;320.441653_132.670876;320.748280_131.770061;321.036390_130.863311;321.293871_129.947416;321.525621_129.024556;321.743764_128.098320;321.960609_127.171774;322.185104_126.247065;322.417461_125.324285;322.651991_124.402051;322.882510_123.478816;323.104295_122.553452;323.320263_121.626697;323.541154_120.701126;323.779309_119.779928;324.046112_118.866729;324.341771_117.962358;324.649588_117.061938;324.946174_116.157862;325.214392_115.245076;325.453733_114.324191;325.675082_113.398733;325.890383_112.471822;326.110266_111.546001;326.338457_110.622188;326.571713_109.699632;326.805368_108.777176;327.035029_107.853723;327.259799_106.929064;327.484149_106.004302;327.714716_105.081086;327.958157_104.161215;328.221068_103.246768;328.509893_102.340242;328.830789_101.444650;</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -735,6 +735,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8478,9 +8479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:P79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8641,7 +8642,7 @@
       <c r="O3" s="2">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="11" t="s">
         <v>108</v>
       </c>
     </row>
@@ -8691,7 +8692,7 @@
       <c r="O4" s="2">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="11" t="s">
         <v>109</v>
       </c>
     </row>
@@ -8741,7 +8742,7 @@
       <c r="O5" s="2">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="11" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8791,7 +8792,7 @@
       <c r="O6" s="2">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="11" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8841,7 +8842,7 @@
       <c r="O7" s="2">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="11" t="s">
         <v>112</v>
       </c>
     </row>
@@ -8891,7 +8892,7 @@
       <c r="O8" s="2">
         <v>0</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="11" t="s">
         <v>113</v>
       </c>
     </row>
@@ -8941,7 +8942,7 @@
       <c r="O9" s="2">
         <v>0</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="11" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8991,7 +8992,7 @@
       <c r="O10" s="2">
         <v>0</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="11" t="s">
         <v>115</v>
       </c>
     </row>
@@ -9041,7 +9042,7 @@
       <c r="O11" s="2">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -9091,7 +9092,7 @@
       <c r="O12" s="2">
         <v>0</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="11" t="s">
         <v>117</v>
       </c>
     </row>
@@ -9141,7 +9142,7 @@
       <c r="O13" s="2">
         <v>0</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="11" t="s">
         <v>118</v>
       </c>
     </row>
@@ -9191,7 +9192,7 @@
       <c r="O14" s="2">
         <v>0</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="11" t="s">
         <v>119</v>
       </c>
     </row>
@@ -9241,7 +9242,7 @@
       <c r="O15" s="2">
         <v>0</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="11" t="s">
         <v>120</v>
       </c>
     </row>
@@ -9291,7 +9292,7 @@
       <c r="O16" s="2">
         <v>0</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="11" t="s">
         <v>121</v>
       </c>
     </row>
@@ -9341,7 +9342,7 @@
       <c r="O17" s="2">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="11" t="s">
         <v>122</v>
       </c>
     </row>
@@ -9391,7 +9392,7 @@
       <c r="O18" s="2">
         <v>0</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="11" t="s">
         <v>123</v>
       </c>
     </row>
@@ -9441,7 +9442,7 @@
       <c r="O19" s="2">
         <v>0</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -9491,7 +9492,7 @@
       <c r="O20" s="2">
         <v>0</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="11" t="s">
         <v>125</v>
       </c>
     </row>
@@ -9541,7 +9542,7 @@
       <c r="O21" s="2">
         <v>0</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="11" t="s">
         <v>126</v>
       </c>
     </row>
@@ -9591,7 +9592,7 @@
       <c r="O22" s="2">
         <v>0</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="11" t="s">
         <v>127</v>
       </c>
     </row>
@@ -9641,7 +9642,7 @@
       <c r="O23" s="2">
         <v>0</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="11" t="s">
         <v>128</v>
       </c>
     </row>
@@ -9691,7 +9692,7 @@
       <c r="O24" s="2">
         <v>0</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="11" t="s">
         <v>129</v>
       </c>
     </row>
@@ -9741,7 +9742,7 @@
       <c r="O25" s="2">
         <v>0</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="11" t="s">
         <v>130</v>
       </c>
     </row>
@@ -9791,7 +9792,7 @@
       <c r="O26" s="2">
         <v>1</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="11" t="s">
         <v>131</v>
       </c>
     </row>
@@ -9841,7 +9842,7 @@
       <c r="O27" s="2">
         <v>1</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P27" s="11" t="s">
         <v>132</v>
       </c>
     </row>
@@ -9891,7 +9892,7 @@
       <c r="O28" s="2">
         <v>1</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P28" s="11" t="s">
         <v>133</v>
       </c>
     </row>
@@ -9941,7 +9942,7 @@
       <c r="O29" s="2">
         <v>1</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P29" s="11" t="s">
         <v>134</v>
       </c>
     </row>
@@ -9991,7 +9992,7 @@
       <c r="O30" s="2">
         <v>1</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="11" t="s">
         <v>135</v>
       </c>
     </row>
@@ -10041,7 +10042,7 @@
       <c r="O31" s="2">
         <v>1</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P31" s="11" t="s">
         <v>136</v>
       </c>
     </row>
@@ -10091,7 +10092,7 @@
       <c r="O32" s="2">
         <v>1</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P32" s="11" t="s">
         <v>137</v>
       </c>
     </row>
@@ -10141,7 +10142,7 @@
       <c r="O33" s="2">
         <v>1</v>
       </c>
-      <c r="P33" t="s">
+      <c r="P33" s="11" t="s">
         <v>138</v>
       </c>
     </row>
@@ -10191,7 +10192,7 @@
       <c r="O34" s="2">
         <v>1</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P34" s="11" t="s">
         <v>139</v>
       </c>
     </row>
@@ -10241,7 +10242,7 @@
       <c r="O35" s="2">
         <v>1</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="11" t="s">
         <v>140</v>
       </c>
     </row>
@@ -10291,7 +10292,7 @@
       <c r="O36" s="2">
         <v>1</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="11" t="s">
         <v>141</v>
       </c>
     </row>
@@ -10341,7 +10342,7 @@
       <c r="O37" s="2">
         <v>1</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="11" t="s">
         <v>142</v>
       </c>
     </row>
@@ -10391,7 +10392,7 @@
       <c r="O38" s="2">
         <v>1</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P38" s="11" t="s">
         <v>143</v>
       </c>
     </row>
@@ -10441,7 +10442,7 @@
       <c r="O39" s="2">
         <v>1</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P39" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -10491,7 +10492,7 @@
       <c r="O40" s="2">
         <v>1</v>
       </c>
-      <c r="P40" t="s">
+      <c r="P40" s="11" t="s">
         <v>145</v>
       </c>
     </row>
@@ -10541,7 +10542,7 @@
       <c r="O41" s="2">
         <v>1</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" s="11" t="s">
         <v>146</v>
       </c>
     </row>
@@ -10591,7 +10592,7 @@
       <c r="O42" s="2">
         <v>1</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P42" s="11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -10641,7 +10642,7 @@
       <c r="O43" s="2">
         <v>1</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="11" t="s">
         <v>148</v>
       </c>
     </row>
@@ -10691,7 +10692,7 @@
       <c r="O44" s="2">
         <v>1</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="11" t="s">
         <v>149</v>
       </c>
     </row>
@@ -10741,7 +10742,7 @@
       <c r="O45" s="2">
         <v>1</v>
       </c>
-      <c r="P45" t="s">
+      <c r="P45" s="11" t="s">
         <v>150</v>
       </c>
     </row>
@@ -10791,7 +10792,7 @@
       <c r="O46" s="2">
         <v>1</v>
       </c>
-      <c r="P46" t="s">
+      <c r="P46" s="11" t="s">
         <v>151</v>
       </c>
     </row>
@@ -10841,7 +10842,7 @@
       <c r="O47" s="2">
         <v>1</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="11" t="s">
         <v>152</v>
       </c>
     </row>
@@ -10891,7 +10892,7 @@
       <c r="O48" s="2">
         <v>1</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P48" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -10941,7 +10942,7 @@
       <c r="O49" s="2">
         <v>0</v>
       </c>
-      <c r="P49" t="s">
+      <c r="P49" s="11" t="s">
         <v>154</v>
       </c>
     </row>
@@ -10991,7 +10992,7 @@
       <c r="O50" s="2">
         <v>0</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P50" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -11041,7 +11042,7 @@
       <c r="O51" s="2">
         <v>0</v>
       </c>
-      <c r="P51" t="s">
+      <c r="P51" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -11091,7 +11092,7 @@
       <c r="O52" s="2">
         <v>0</v>
       </c>
-      <c r="P52" t="s">
+      <c r="P52" s="11" t="s">
         <v>157</v>
       </c>
     </row>
@@ -11141,7 +11142,7 @@
       <c r="O53" s="2">
         <v>0</v>
       </c>
-      <c r="P53" t="s">
+      <c r="P53" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -11191,7 +11192,7 @@
       <c r="O54" s="2">
         <v>0</v>
       </c>
-      <c r="P54" t="s">
+      <c r="P54" s="11" t="s">
         <v>159</v>
       </c>
     </row>
@@ -11241,7 +11242,7 @@
       <c r="O55" s="2">
         <v>0</v>
       </c>
-      <c r="P55" t="s">
+      <c r="P55" s="11" t="s">
         <v>160</v>
       </c>
     </row>
@@ -11291,7 +11292,7 @@
       <c r="O56" s="2">
         <v>0</v>
       </c>
-      <c r="P56" t="s">
+      <c r="P56" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -11341,7 +11342,7 @@
       <c r="O57" s="2">
         <v>0</v>
       </c>
-      <c r="P57" t="s">
+      <c r="P57" s="11" t="s">
         <v>162</v>
       </c>
     </row>
@@ -11391,7 +11392,7 @@
       <c r="O58" s="2">
         <v>0</v>
       </c>
-      <c r="P58" t="s">
+      <c r="P58" s="11" t="s">
         <v>163</v>
       </c>
     </row>
@@ -11441,7 +11442,7 @@
       <c r="O59" s="2">
         <v>0</v>
       </c>
-      <c r="P59" t="s">
+      <c r="P59" s="11" t="s">
         <v>164</v>
       </c>
     </row>
@@ -11491,7 +11492,7 @@
       <c r="O60" s="2">
         <v>0</v>
       </c>
-      <c r="P60" t="s">
+      <c r="P60" s="11" t="s">
         <v>165</v>
       </c>
     </row>
@@ -11541,7 +11542,7 @@
       <c r="O61" s="2">
         <v>0</v>
       </c>
-      <c r="P61" t="s">
+      <c r="P61" s="11" t="s">
         <v>166</v>
       </c>
     </row>
@@ -11591,7 +11592,7 @@
       <c r="O62" s="2">
         <v>0</v>
       </c>
-      <c r="P62" t="s">
+      <c r="P62" s="11" t="s">
         <v>167</v>
       </c>
     </row>
@@ -11641,7 +11642,7 @@
       <c r="O63" s="2">
         <v>0</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P63" s="11" t="s">
         <v>168</v>
       </c>
     </row>
@@ -11691,7 +11692,7 @@
       <c r="O64" s="2">
         <v>0</v>
       </c>
-      <c r="P64" t="s">
+      <c r="P64" s="11" t="s">
         <v>169</v>
       </c>
     </row>
@@ -11741,7 +11742,7 @@
       <c r="O65" s="2">
         <v>0</v>
       </c>
-      <c r="P65" t="s">
+      <c r="P65" s="11" t="s">
         <v>170</v>
       </c>
     </row>
@@ -11791,7 +11792,7 @@
       <c r="O66" s="2">
         <v>0</v>
       </c>
-      <c r="P66" t="s">
+      <c r="P66" s="11" t="s">
         <v>171</v>
       </c>
     </row>
@@ -11841,7 +11842,7 @@
       <c r="O67" s="2">
         <v>0</v>
       </c>
-      <c r="P67" t="s">
+      <c r="P67" s="11" t="s">
         <v>172</v>
       </c>
     </row>
@@ -11891,7 +11892,7 @@
       <c r="O68" s="2">
         <v>0</v>
       </c>
-      <c r="P68" t="s">
+      <c r="P68" s="11" t="s">
         <v>173</v>
       </c>
     </row>
@@ -11941,7 +11942,7 @@
       <c r="O69" s="2">
         <v>1</v>
       </c>
-      <c r="P69" t="s">
+      <c r="P69" s="11" t="s">
         <v>174</v>
       </c>
     </row>
@@ -11991,7 +11992,7 @@
       <c r="O70" s="2">
         <v>1</v>
       </c>
-      <c r="P70" t="s">
+      <c r="P70" s="11" t="s">
         <v>175</v>
       </c>
     </row>
@@ -12041,7 +12042,7 @@
       <c r="O71" s="2">
         <v>1</v>
       </c>
-      <c r="P71" t="s">
+      <c r="P71" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -12091,7 +12092,7 @@
       <c r="O72" s="2">
         <v>1</v>
       </c>
-      <c r="P72" t="s">
+      <c r="P72" s="11" t="s">
         <v>177</v>
       </c>
     </row>
@@ -12141,7 +12142,7 @@
       <c r="O73" s="2">
         <v>1</v>
       </c>
-      <c r="P73" t="s">
+      <c r="P73" s="11" t="s">
         <v>178</v>
       </c>
     </row>
@@ -12191,7 +12192,7 @@
       <c r="O74" s="2">
         <v>1</v>
       </c>
-      <c r="P74" t="s">
+      <c r="P74" s="11" t="s">
         <v>179</v>
       </c>
     </row>
@@ -12241,7 +12242,7 @@
       <c r="O75" s="2">
         <v>1</v>
       </c>
-      <c r="P75" t="s">
+      <c r="P75" s="11" t="s">
         <v>180</v>
       </c>
     </row>
@@ -12291,7 +12292,7 @@
       <c r="O76" s="2">
         <v>1</v>
       </c>
-      <c r="P76" t="s">
+      <c r="P76" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -12341,7 +12342,7 @@
       <c r="O77" s="2">
         <v>1</v>
       </c>
-      <c r="P77" t="s">
+      <c r="P77" s="11" t="s">
         <v>182</v>
       </c>
     </row>
@@ -12391,7 +12392,7 @@
       <c r="O78" s="2">
         <v>1</v>
       </c>
-      <c r="P78" t="s">
+      <c r="P78" s="11" t="s">
         <v>183</v>
       </c>
     </row>
@@ -12441,7 +12442,7 @@
       <c r="O79" s="2">
         <v>0</v>
       </c>
-      <c r="P79" t="s">
+      <c r="P79" s="11" t="s">
         <v>184</v>
       </c>
     </row>
@@ -20817,8 +20818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="K52" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20873,7 +20874,7 @@
       <c r="O1" s="2">
         <v>0</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="11" t="s">
         <v>108</v>
       </c>
     </row>
@@ -20923,7 +20924,7 @@
       <c r="O2" s="2">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="11" t="s">
         <v>109</v>
       </c>
     </row>
@@ -20973,7 +20974,7 @@
       <c r="O3" s="2">
         <v>0</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="11" t="s">
         <v>110</v>
       </c>
     </row>
@@ -21023,7 +21024,7 @@
       <c r="O4" s="2">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="11" t="s">
         <v>111</v>
       </c>
     </row>
@@ -21073,7 +21074,7 @@
       <c r="O5" s="2">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="11" t="s">
         <v>112</v>
       </c>
     </row>
@@ -21123,7 +21124,7 @@
       <c r="O6" s="2">
         <v>0</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="11" t="s">
         <v>113</v>
       </c>
     </row>
@@ -21173,7 +21174,7 @@
       <c r="O7" s="2">
         <v>0</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="11" t="s">
         <v>114</v>
       </c>
     </row>
@@ -21223,7 +21224,7 @@
       <c r="O8" s="2">
         <v>0</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="11" t="s">
         <v>115</v>
       </c>
     </row>
@@ -21273,7 +21274,7 @@
       <c r="O9" s="2">
         <v>0</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="11" t="s">
         <v>116</v>
       </c>
     </row>
@@ -21323,7 +21324,7 @@
       <c r="O10" s="2">
         <v>0</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="11" t="s">
         <v>117</v>
       </c>
     </row>
@@ -21373,7 +21374,7 @@
       <c r="O11" s="2">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="11" t="s">
         <v>118</v>
       </c>
     </row>
@@ -21423,7 +21424,7 @@
       <c r="O12" s="2">
         <v>0</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="11" t="s">
         <v>119</v>
       </c>
     </row>
@@ -21473,7 +21474,7 @@
       <c r="O13" s="2">
         <v>0</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="11" t="s">
         <v>120</v>
       </c>
     </row>
@@ -21523,7 +21524,7 @@
       <c r="O14" s="2">
         <v>0</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="11" t="s">
         <v>121</v>
       </c>
     </row>
@@ -21573,7 +21574,7 @@
       <c r="O15" s="2">
         <v>0</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="11" t="s">
         <v>122</v>
       </c>
     </row>
@@ -21623,7 +21624,7 @@
       <c r="O16" s="2">
         <v>0</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="11" t="s">
         <v>123</v>
       </c>
     </row>
@@ -21673,7 +21674,7 @@
       <c r="O17" s="2">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -21723,7 +21724,7 @@
       <c r="O18" s="2">
         <v>0</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="11" t="s">
         <v>125</v>
       </c>
     </row>
@@ -21773,7 +21774,7 @@
       <c r="O19" s="2">
         <v>0</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="11" t="s">
         <v>126</v>
       </c>
     </row>
@@ -21823,7 +21824,7 @@
       <c r="O20" s="2">
         <v>0</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="11" t="s">
         <v>127</v>
       </c>
     </row>
@@ -21873,7 +21874,7 @@
       <c r="O21" s="2">
         <v>0</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P21" s="11" t="s">
         <v>128</v>
       </c>
     </row>
@@ -21923,7 +21924,7 @@
       <c r="O22" s="2">
         <v>0</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="11" t="s">
         <v>129</v>
       </c>
     </row>
@@ -21973,7 +21974,7 @@
       <c r="O23" s="2">
         <v>0</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="11" t="s">
         <v>130</v>
       </c>
     </row>
@@ -22023,7 +22024,7 @@
       <c r="O24" s="2">
         <v>1</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="11" t="s">
         <v>131</v>
       </c>
     </row>
@@ -22073,7 +22074,7 @@
       <c r="O25" s="2">
         <v>1</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="11" t="s">
         <v>132</v>
       </c>
     </row>
@@ -22123,7 +22124,7 @@
       <c r="O26" s="2">
         <v>1</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="11" t="s">
         <v>133</v>
       </c>
     </row>
@@ -22173,7 +22174,7 @@
       <c r="O27" s="2">
         <v>1</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P27" s="11" t="s">
         <v>134</v>
       </c>
     </row>
@@ -22223,7 +22224,7 @@
       <c r="O28" s="2">
         <v>1</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P28" s="11" t="s">
         <v>135</v>
       </c>
     </row>
@@ -22273,7 +22274,7 @@
       <c r="O29" s="2">
         <v>1</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P29" s="11" t="s">
         <v>136</v>
       </c>
     </row>
@@ -22323,7 +22324,7 @@
       <c r="O30" s="2">
         <v>1</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="11" t="s">
         <v>137</v>
       </c>
     </row>
@@ -22373,7 +22374,7 @@
       <c r="O31" s="2">
         <v>1</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P31" s="11" t="s">
         <v>138</v>
       </c>
     </row>
@@ -22423,7 +22424,7 @@
       <c r="O32" s="2">
         <v>1</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P32" s="11" t="s">
         <v>139</v>
       </c>
     </row>
@@ -22473,7 +22474,7 @@
       <c r="O33" s="2">
         <v>1</v>
       </c>
-      <c r="P33" t="s">
+      <c r="P33" s="11" t="s">
         <v>140</v>
       </c>
     </row>
@@ -22523,7 +22524,7 @@
       <c r="O34" s="2">
         <v>1</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P34" s="11" t="s">
         <v>141</v>
       </c>
     </row>
@@ -22573,7 +22574,7 @@
       <c r="O35" s="2">
         <v>1</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="11" t="s">
         <v>142</v>
       </c>
     </row>
@@ -22623,7 +22624,7 @@
       <c r="O36" s="2">
         <v>1</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="11" t="s">
         <v>143</v>
       </c>
     </row>
@@ -22673,7 +22674,7 @@
       <c r="O37" s="2">
         <v>1</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="11" t="s">
         <v>144</v>
       </c>
     </row>
@@ -22723,7 +22724,7 @@
       <c r="O38" s="2">
         <v>1</v>
       </c>
-      <c r="P38" t="s">
+      <c r="P38" s="11" t="s">
         <v>145</v>
       </c>
     </row>
@@ -22773,7 +22774,7 @@
       <c r="O39" s="2">
         <v>1</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P39" s="11" t="s">
         <v>146</v>
       </c>
     </row>
@@ -22823,7 +22824,7 @@
       <c r="O40" s="2">
         <v>1</v>
       </c>
-      <c r="P40" t="s">
+      <c r="P40" s="11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -22873,7 +22874,7 @@
       <c r="O41" s="2">
         <v>1</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" s="11" t="s">
         <v>148</v>
       </c>
     </row>
@@ -22923,7 +22924,7 @@
       <c r="O42" s="2">
         <v>1</v>
       </c>
-      <c r="P42" t="s">
+      <c r="P42" s="11" t="s">
         <v>149</v>
       </c>
     </row>
@@ -22973,7 +22974,7 @@
       <c r="O43" s="2">
         <v>1</v>
       </c>
-      <c r="P43" t="s">
+      <c r="P43" s="11" t="s">
         <v>150</v>
       </c>
     </row>
@@ -23023,7 +23024,7 @@
       <c r="O44" s="2">
         <v>1</v>
       </c>
-      <c r="P44" t="s">
+      <c r="P44" s="11" t="s">
         <v>151</v>
       </c>
     </row>
@@ -23073,7 +23074,7 @@
       <c r="O45" s="2">
         <v>1</v>
       </c>
-      <c r="P45" t="s">
+      <c r="P45" s="11" t="s">
         <v>152</v>
       </c>
     </row>
@@ -23123,7 +23124,7 @@
       <c r="O46" s="2">
         <v>1</v>
       </c>
-      <c r="P46" t="s">
+      <c r="P46" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -23173,7 +23174,7 @@
       <c r="O47" s="2">
         <v>0</v>
       </c>
-      <c r="P47" t="s">
+      <c r="P47" s="11" t="s">
         <v>154</v>
       </c>
     </row>
@@ -23223,7 +23224,7 @@
       <c r="O48" s="2">
         <v>0</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P48" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -23273,7 +23274,7 @@
       <c r="O49" s="2">
         <v>0</v>
       </c>
-      <c r="P49" t="s">
+      <c r="P49" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -23323,7 +23324,7 @@
       <c r="O50" s="2">
         <v>0</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P50" s="11" t="s">
         <v>157</v>
       </c>
     </row>
@@ -23373,7 +23374,7 @@
       <c r="O51" s="2">
         <v>0</v>
       </c>
-      <c r="P51" t="s">
+      <c r="P51" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -23423,7 +23424,7 @@
       <c r="O52" s="2">
         <v>0</v>
       </c>
-      <c r="P52" t="s">
+      <c r="P52" s="11" t="s">
         <v>159</v>
       </c>
     </row>
@@ -23473,7 +23474,7 @@
       <c r="O53" s="2">
         <v>0</v>
       </c>
-      <c r="P53" t="s">
+      <c r="P53" s="11" t="s">
         <v>160</v>
       </c>
     </row>
@@ -23523,7 +23524,7 @@
       <c r="O54" s="2">
         <v>0</v>
       </c>
-      <c r="P54" t="s">
+      <c r="P54" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -23573,7 +23574,7 @@
       <c r="O55" s="2">
         <v>0</v>
       </c>
-      <c r="P55" t="s">
+      <c r="P55" s="11" t="s">
         <v>162</v>
       </c>
     </row>
@@ -23623,7 +23624,7 @@
       <c r="O56" s="2">
         <v>0</v>
       </c>
-      <c r="P56" t="s">
+      <c r="P56" s="11" t="s">
         <v>163</v>
       </c>
     </row>
@@ -23673,7 +23674,7 @@
       <c r="O57" s="2">
         <v>0</v>
       </c>
-      <c r="P57" t="s">
+      <c r="P57" s="11" t="s">
         <v>164</v>
       </c>
     </row>
@@ -23723,7 +23724,7 @@
       <c r="O58" s="2">
         <v>0</v>
       </c>
-      <c r="P58" t="s">
+      <c r="P58" s="11" t="s">
         <v>165</v>
       </c>
     </row>
@@ -23773,7 +23774,7 @@
       <c r="O59" s="2">
         <v>0</v>
       </c>
-      <c r="P59" t="s">
+      <c r="P59" s="11" t="s">
         <v>166</v>
       </c>
     </row>
@@ -23823,7 +23824,7 @@
       <c r="O60" s="2">
         <v>0</v>
       </c>
-      <c r="P60" t="s">
+      <c r="P60" s="11" t="s">
         <v>167</v>
       </c>
     </row>
@@ -23873,7 +23874,7 @@
       <c r="O61" s="2">
         <v>0</v>
       </c>
-      <c r="P61" t="s">
+      <c r="P61" s="11" t="s">
         <v>168</v>
       </c>
     </row>
@@ -23923,7 +23924,7 @@
       <c r="O62" s="2">
         <v>0</v>
       </c>
-      <c r="P62" t="s">
+      <c r="P62" s="11" t="s">
         <v>169</v>
       </c>
     </row>
@@ -23973,7 +23974,7 @@
       <c r="O63" s="2">
         <v>0</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P63" s="11" t="s">
         <v>170</v>
       </c>
     </row>
@@ -24023,7 +24024,7 @@
       <c r="O64" s="2">
         <v>0</v>
       </c>
-      <c r="P64" t="s">
+      <c r="P64" s="11" t="s">
         <v>171</v>
       </c>
     </row>
@@ -24073,7 +24074,7 @@
       <c r="O65" s="2">
         <v>0</v>
       </c>
-      <c r="P65" t="s">
+      <c r="P65" s="11" t="s">
         <v>172</v>
       </c>
     </row>
@@ -24123,7 +24124,7 @@
       <c r="O66" s="2">
         <v>0</v>
       </c>
-      <c r="P66" t="s">
+      <c r="P66" s="11" t="s">
         <v>173</v>
       </c>
     </row>
@@ -24173,7 +24174,7 @@
       <c r="O67" s="2">
         <v>1</v>
       </c>
-      <c r="P67" t="s">
+      <c r="P67" s="11" t="s">
         <v>174</v>
       </c>
     </row>
@@ -24223,7 +24224,7 @@
       <c r="O68" s="2">
         <v>1</v>
       </c>
-      <c r="P68" t="s">
+      <c r="P68" s="11" t="s">
         <v>175</v>
       </c>
     </row>
@@ -24273,7 +24274,7 @@
       <c r="O69" s="2">
         <v>1</v>
       </c>
-      <c r="P69" t="s">
+      <c r="P69" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -24323,7 +24324,7 @@
       <c r="O70" s="2">
         <v>1</v>
       </c>
-      <c r="P70" t="s">
+      <c r="P70" s="11" t="s">
         <v>177</v>
       </c>
     </row>
@@ -24373,7 +24374,7 @@
       <c r="O71" s="2">
         <v>1</v>
       </c>
-      <c r="P71" t="s">
+      <c r="P71" s="11" t="s">
         <v>178</v>
       </c>
     </row>
@@ -24423,7 +24424,7 @@
       <c r="O72" s="2">
         <v>1</v>
       </c>
-      <c r="P72" t="s">
+      <c r="P72" s="11" t="s">
         <v>179</v>
       </c>
     </row>
@@ -24473,7 +24474,7 @@
       <c r="O73" s="2">
         <v>1</v>
       </c>
-      <c r="P73" t="s">
+      <c r="P73" s="11" t="s">
         <v>180</v>
       </c>
     </row>
@@ -24523,7 +24524,7 @@
       <c r="O74" s="2">
         <v>1</v>
       </c>
-      <c r="P74" t="s">
+      <c r="P74" s="11" t="s">
         <v>181</v>
       </c>
     </row>
@@ -24573,7 +24574,7 @@
       <c r="O75" s="2">
         <v>1</v>
       </c>
-      <c r="P75" t="s">
+      <c r="P75" s="11" t="s">
         <v>182</v>
       </c>
     </row>
@@ -24623,7 +24624,7 @@
       <c r="O76" s="2">
         <v>1</v>
       </c>
-      <c r="P76" t="s">
+      <c r="P76" s="11" t="s">
         <v>183</v>
       </c>
     </row>
@@ -24673,7 +24674,7 @@
       <c r="O77" s="2">
         <v>0</v>
       </c>
-      <c r="P77" t="s">
+      <c r="P77" s="11" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated beacons in CSVs to before and after each station
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -1509,9 +1509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:P154"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N144" sqref="N144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,7 +1671,7 @@
         <v>56</v>
       </c>
       <c r="N3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="9">
         <v>0</v>
@@ -1721,7 +1721,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="9">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="9">
         <v>0</v>
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10" s="9">
         <v>0</v>
@@ -2071,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11" s="9">
         <v>0</v>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O12" s="9">
         <v>0</v>
@@ -2371,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O17" s="9">
         <v>0</v>
@@ -2421,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O18" s="9">
         <v>0</v>
@@ -2471,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O19" s="9">
         <v>0</v>
@@ -2671,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O23" s="9">
         <v>0</v>
@@ -2721,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O24" s="9">
         <v>0</v>
@@ -2771,7 +2771,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O25" s="9">
         <v>0</v>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O32" s="9">
         <v>0</v>
@@ -3171,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O33" s="9">
         <v>0</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="N34" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O34" s="9">
         <v>0</v>
@@ -3521,7 +3521,7 @@
         <v>0</v>
       </c>
       <c r="N40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O40" s="9">
         <v>1</v>
@@ -3571,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="N41" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O41" s="9">
         <v>1</v>
@@ -3621,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O42" s="9">
         <v>1</v>
@@ -3971,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="N49" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O49" s="9">
         <v>1</v>
@@ -4021,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="N50" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O50" s="9">
         <v>1</v>
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="N51" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O51" s="9">
         <v>1</v>
@@ -4421,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="N58" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O58" s="9">
         <v>1</v>
@@ -4471,7 +4471,7 @@
         <v>49</v>
       </c>
       <c r="N59" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O59" s="9">
         <v>1</v>
@@ -4521,7 +4521,7 @@
         <v>43</v>
       </c>
       <c r="N60" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O60" s="9">
         <v>0</v>
@@ -4821,7 +4821,7 @@
         <v>0</v>
       </c>
       <c r="N66" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O66" s="9">
         <v>0</v>
@@ -4871,7 +4871,7 @@
         <v>0</v>
       </c>
       <c r="N67" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="O67" s="9">
         <v>0</v>
@@ -4921,7 +4921,7 @@
         <v>0</v>
       </c>
       <c r="N68" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O68" s="9">
         <v>0</v>
@@ -5221,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="N74" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O74" s="9">
         <v>0</v>
@@ -5271,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="N75" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O75" s="9">
         <v>0</v>
@@ -5321,7 +5321,7 @@
         <v>0</v>
       </c>
       <c r="N76" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O76" s="9">
         <v>0</v>
@@ -5421,7 +5421,7 @@
         <v>45</v>
       </c>
       <c r="N78" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O78" s="9">
         <v>0</v>
@@ -5471,7 +5471,7 @@
         <v>51</v>
       </c>
       <c r="N79" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="O79" s="9">
         <v>0</v>
@@ -5521,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="N80" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O80" s="9">
         <v>0</v>
@@ -5971,7 +5971,7 @@
         <v>0</v>
       </c>
       <c r="N89" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O89" s="9">
         <v>0</v>
@@ -6021,7 +6021,7 @@
         <v>0</v>
       </c>
       <c r="N90" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O90" s="9">
         <v>0</v>
@@ -6071,7 +6071,7 @@
         <v>0</v>
       </c>
       <c r="N91" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O91" s="9">
         <v>0</v>
@@ -6371,7 +6371,7 @@
         <v>0</v>
       </c>
       <c r="N97" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O97" s="9">
         <v>0</v>
@@ -6421,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="N98" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O98" s="9">
         <v>0</v>
@@ -6471,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="N99" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O99" s="9">
         <v>0</v>
@@ -7271,7 +7271,7 @@
         <v>0</v>
       </c>
       <c r="N115" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O115" s="9">
         <v>0</v>
@@ -7321,7 +7321,7 @@
         <v>0</v>
       </c>
       <c r="N116" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O116" s="9">
         <v>0</v>
@@ -7371,7 +7371,7 @@
         <v>0</v>
       </c>
       <c r="N117" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O117" s="9">
         <v>0</v>
@@ -7721,7 +7721,7 @@
         <v>0</v>
       </c>
       <c r="N124" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O124" s="9">
         <v>1</v>
@@ -7771,7 +7771,7 @@
         <v>0</v>
       </c>
       <c r="N125" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O125" s="9">
         <v>1</v>
@@ -7821,7 +7821,7 @@
         <v>0</v>
       </c>
       <c r="N126" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O126" s="9">
         <v>1</v>
@@ -8171,7 +8171,7 @@
         <v>0</v>
       </c>
       <c r="N133" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O133" s="9">
         <v>1</v>
@@ -8221,7 +8221,7 @@
         <v>0</v>
       </c>
       <c r="N134" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="O134" s="9">
         <v>1</v>
@@ -8271,7 +8271,7 @@
         <v>0</v>
       </c>
       <c r="N135" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O135" s="9">
         <v>1</v>
@@ -8621,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="N142" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O142" s="9">
         <v>1</v>
@@ -8671,7 +8671,7 @@
         <v>0</v>
       </c>
       <c r="N143" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="O143" s="9">
         <v>1</v>
@@ -8721,7 +8721,7 @@
         <v>0</v>
       </c>
       <c r="N144" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O144" s="9">
         <v>1</v>
@@ -9240,9 +9240,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:P79"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9398,7 +9398,7 @@
         <v>88</v>
       </c>
       <c r="N3" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -9648,7 +9648,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -9701,7 +9701,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="P9" s="12" t="s">
         <v>299</v>
@@ -9748,7 +9748,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O10" s="2">
         <v>0</v>
@@ -10098,7 +10098,7 @@
         <v>86</v>
       </c>
       <c r="N17" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O17" s="2">
         <v>0</v>
@@ -10151,7 +10151,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="P18" s="12" t="s">
         <v>108</v>
@@ -10198,7 +10198,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O19" s="2">
         <v>0</v>
@@ -10348,7 +10348,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O22" s="2">
         <v>0</v>
@@ -10401,7 +10401,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P23" s="12" t="s">
         <v>308</v>
@@ -10448,7 +10448,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O24" s="2">
         <v>0</v>
@@ -10548,7 +10548,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O26" s="2">
         <v>1</v>
@@ -10601,7 +10601,7 @@
         <v>0</v>
       </c>
       <c r="O27" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="P27" s="12" t="s">
         <v>114</v>
@@ -10648,7 +10648,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O28" s="2">
         <v>1</v>
@@ -11048,7 +11048,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O36" s="2">
         <v>1</v>
@@ -11101,7 +11101,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="P37" s="12" t="s">
         <v>124</v>
@@ -11148,7 +11148,7 @@
         <v>0</v>
       </c>
       <c r="N38" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O38" s="2">
         <v>1</v>
@@ -11548,7 +11548,7 @@
         <v>0</v>
       </c>
       <c r="N46" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O46" s="2">
         <v>1</v>
@@ -11601,7 +11601,7 @@
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="P47" s="12" t="s">
         <v>134</v>
@@ -11648,7 +11648,7 @@
         <v>0</v>
       </c>
       <c r="N48" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O48" s="2">
         <v>1</v>
@@ -11698,7 +11698,7 @@
         <v>0</v>
       </c>
       <c r="N49" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="O49" s="2">
         <v>0</v>
@@ -11751,7 +11751,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="P50" s="12" t="s">
         <v>313</v>
@@ -11798,7 +11798,7 @@
         <v>0</v>
       </c>
       <c r="N51" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="O51" s="2">
         <v>0</v>
@@ -12298,7 +12298,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O61" s="2">
         <v>0</v>
@@ -12351,7 +12351,7 @@
         <v>0</v>
       </c>
       <c r="O62" s="2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P62" s="12" t="s">
         <v>325</v>
@@ -12398,7 +12398,7 @@
         <v>0</v>
       </c>
       <c r="N63" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O63" s="2">
         <v>0</v>
@@ -22035,8 +22035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated GreenLineFinal CSV's (in all modules) for YARD_IN direction to be 1
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="6615" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -1509,9 +1509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N144" sqref="N144"/>
+      <selection pane="bottomLeft" activeCell="I154" sqref="I154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9156,7 +9156,7 @@
         <v>55</v>
       </c>
       <c r="I153" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J153" s="2">
         <v>0</v>
@@ -9240,8 +9240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
@@ -14416,8 +14416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P152"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="K160" sqref="K160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21952,7 +21952,7 @@
         <v>55</v>
       </c>
       <c r="I151" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J151" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
updated CSV with lights and parsing into dynamic track view
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="2"/>
+    <workbookView xWindow="7650" yWindow="0" windowWidth="16170" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -1509,9 +1509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I154" sqref="I154"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:P154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1659,7 @@
         <v>-1</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2">
         <v>0</v>
@@ -2259,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
@@ -2511,7 +2511,7 @@
       <c r="J20" s="2">
         <v>0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>0</v>
       </c>
       <c r="L20" s="2">
@@ -2561,7 +2561,7 @@
       <c r="J21" s="2">
         <v>0</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>1</v>
       </c>
       <c r="L21" s="2">
@@ -2611,7 +2611,7 @@
       <c r="J22" s="2">
         <v>0</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>0</v>
       </c>
       <c r="L22" s="2">
@@ -2661,7 +2661,7 @@
       <c r="J23" s="2">
         <v>0</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>0</v>
       </c>
       <c r="L23" s="2">
@@ -2711,7 +2711,7 @@
       <c r="J24" s="2">
         <v>0</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>0</v>
       </c>
       <c r="L24" s="2" t="s">
@@ -2761,7 +2761,7 @@
       <c r="J25" s="2">
         <v>0</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>0</v>
       </c>
       <c r="L25" s="2">
@@ -2811,7 +2811,7 @@
       <c r="J26" s="2">
         <v>0</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="1">
         <v>0</v>
       </c>
       <c r="L26" s="2">
@@ -2861,7 +2861,7 @@
       <c r="J27" s="2">
         <v>0</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1">
         <v>0</v>
       </c>
       <c r="L27" s="2">
@@ -2911,7 +2911,7 @@
       <c r="J28" s="2">
         <v>0</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1">
         <v>0</v>
       </c>
       <c r="L28" s="2">
@@ -2961,7 +2961,7 @@
       <c r="J29" s="2">
         <v>0</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>0</v>
       </c>
       <c r="L29" s="2">
@@ -3009,9 +3009,9 @@
         <v>0</v>
       </c>
       <c r="J30" s="2">
-        <v>0</v>
-      </c>
-      <c r="K30" s="2">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1">
         <v>0</v>
       </c>
       <c r="L30" s="2">
@@ -3061,7 +3061,7 @@
       <c r="J31" s="2">
         <v>0</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1">
         <v>0</v>
       </c>
       <c r="L31" s="2">
@@ -3111,7 +3111,7 @@
       <c r="J32" s="2">
         <v>0</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>0</v>
       </c>
       <c r="L32" s="2">
@@ -3161,7 +3161,7 @@
       <c r="J33" s="2">
         <v>0</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="1">
         <v>0</v>
       </c>
       <c r="L33" s="2" t="s">
@@ -3211,7 +3211,7 @@
       <c r="J34" s="2">
         <v>0</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>0</v>
       </c>
       <c r="L34" s="2">
@@ -3261,7 +3261,7 @@
       <c r="J35" s="2">
         <v>0</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="1">
         <v>0</v>
       </c>
       <c r="L35" s="2">
@@ -3311,7 +3311,7 @@
       <c r="J36" s="2">
         <v>0</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="1">
         <v>0</v>
       </c>
       <c r="L36" s="2">
@@ -3361,7 +3361,7 @@
       <c r="J37" s="2">
         <v>0</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="1">
         <v>0</v>
       </c>
       <c r="L37" s="2">
@@ -3411,7 +3411,7 @@
       <c r="J38" s="2">
         <v>0</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="1">
         <v>0</v>
       </c>
       <c r="L38" s="2">
@@ -3461,7 +3461,7 @@
       <c r="J39" s="2">
         <v>0</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="1">
         <v>0</v>
       </c>
       <c r="L39" s="2">
@@ -3511,7 +3511,7 @@
       <c r="J40" s="2">
         <v>0</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="1">
         <v>0</v>
       </c>
       <c r="L40" s="2">
@@ -3561,7 +3561,7 @@
       <c r="J41" s="2">
         <v>0</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="1">
         <v>0</v>
       </c>
       <c r="L41" s="2" t="s">
@@ -3611,7 +3611,7 @@
       <c r="J42" s="2">
         <v>0</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="1">
         <v>0</v>
       </c>
       <c r="L42" s="2">
@@ -3661,7 +3661,7 @@
       <c r="J43" s="2">
         <v>0</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="1">
         <v>0</v>
       </c>
       <c r="L43" s="2">
@@ -3711,7 +3711,7 @@
       <c r="J44" s="2">
         <v>0</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1">
         <v>0</v>
       </c>
       <c r="L44" s="2">
@@ -3761,7 +3761,7 @@
       <c r="J45" s="2">
         <v>0</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>0</v>
       </c>
       <c r="L45" s="2">
@@ -3811,7 +3811,7 @@
       <c r="J46" s="2">
         <v>0</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="1">
         <v>0</v>
       </c>
       <c r="L46" s="2">
@@ -3861,7 +3861,7 @@
       <c r="J47" s="2">
         <v>0</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="1">
         <v>0</v>
       </c>
       <c r="L47" s="2">
@@ -3911,7 +3911,7 @@
       <c r="J48" s="2">
         <v>0</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="1">
         <v>0</v>
       </c>
       <c r="L48" s="2">
@@ -3961,7 +3961,7 @@
       <c r="J49" s="2">
         <v>0</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="1">
         <v>0</v>
       </c>
       <c r="L49" s="2">
@@ -4011,7 +4011,7 @@
       <c r="J50" s="2">
         <v>0</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="1">
         <v>0</v>
       </c>
       <c r="L50" s="2" t="s">
@@ -4061,7 +4061,7 @@
       <c r="J51" s="2">
         <v>0</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="1">
         <v>0</v>
       </c>
       <c r="L51" s="2">
@@ -4111,7 +4111,7 @@
       <c r="J52" s="2">
         <v>0</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="1">
         <v>0</v>
       </c>
       <c r="L52" s="2">
@@ -4161,7 +4161,7 @@
       <c r="J53" s="2">
         <v>0</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="1">
         <v>0</v>
       </c>
       <c r="L53" s="2">
@@ -4211,7 +4211,7 @@
       <c r="J54" s="2">
         <v>0</v>
       </c>
-      <c r="K54" s="2">
+      <c r="K54" s="1">
         <v>0</v>
       </c>
       <c r="L54" s="2">
@@ -4261,7 +4261,7 @@
       <c r="J55" s="2">
         <v>0</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="1">
         <v>0</v>
       </c>
       <c r="L55" s="2">
@@ -4311,7 +4311,7 @@
       <c r="J56" s="2">
         <v>0</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K56" s="1">
         <v>0</v>
       </c>
       <c r="L56" s="2">
@@ -4361,7 +4361,7 @@
       <c r="J57" s="2">
         <v>0</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="1">
         <v>0</v>
       </c>
       <c r="L57" s="2">
@@ -4411,7 +4411,7 @@
       <c r="J58" s="2">
         <v>0</v>
       </c>
-      <c r="K58" s="2">
+      <c r="K58" s="1">
         <v>0</v>
       </c>
       <c r="L58" s="2">
@@ -4461,7 +4461,7 @@
       <c r="J59" s="2">
         <v>0</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="1">
         <v>0</v>
       </c>
       <c r="L59" s="2" t="s">
@@ -4511,7 +4511,7 @@
       <c r="J60" s="2">
         <v>0</v>
       </c>
-      <c r="K60" s="2">
+      <c r="K60" s="1">
         <v>0</v>
       </c>
       <c r="L60" s="2">
@@ -4561,7 +4561,7 @@
       <c r="J61" s="2">
         <v>0</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="1">
         <v>0</v>
       </c>
       <c r="L61" s="2">
@@ -4611,7 +4611,7 @@
       <c r="J62" s="2">
         <v>0</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="1">
         <v>0</v>
       </c>
       <c r="L62" s="2">
@@ -4661,7 +4661,7 @@
       <c r="J63" s="2">
         <v>0</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="1">
         <v>0</v>
       </c>
       <c r="L63" s="2">
@@ -4709,9 +4709,9 @@
         <v>1</v>
       </c>
       <c r="J64" s="2">
-        <v>0</v>
-      </c>
-      <c r="K64" s="2">
+        <v>1</v>
+      </c>
+      <c r="K64" s="1">
         <v>0</v>
       </c>
       <c r="L64" s="2">
@@ -4761,7 +4761,7 @@
       <c r="J65" s="2">
         <v>0</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="1">
         <v>0</v>
       </c>
       <c r="L65" s="2">
@@ -4811,7 +4811,7 @@
       <c r="J66" s="2">
         <v>0</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="1">
         <v>0</v>
       </c>
       <c r="L66" s="2">
@@ -4861,7 +4861,7 @@
       <c r="J67" s="2">
         <v>0</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="1">
         <v>0</v>
       </c>
       <c r="L67" s="2" t="s">
@@ -4911,7 +4911,7 @@
       <c r="J68" s="2">
         <v>0</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="1">
         <v>0</v>
       </c>
       <c r="L68" s="2">
@@ -4961,7 +4961,7 @@
       <c r="J69" s="2">
         <v>0</v>
       </c>
-      <c r="K69" s="2">
+      <c r="K69" s="1">
         <v>0</v>
       </c>
       <c r="L69" s="2">
@@ -5011,7 +5011,7 @@
       <c r="J70" s="2">
         <v>0</v>
       </c>
-      <c r="K70" s="2">
+      <c r="K70" s="1">
         <v>0</v>
       </c>
       <c r="L70" s="2">
@@ -5061,7 +5061,7 @@
       <c r="J71" s="2">
         <v>0</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="1">
         <v>0</v>
       </c>
       <c r="L71" s="2">
@@ -5111,7 +5111,7 @@
       <c r="J72" s="2">
         <v>0</v>
       </c>
-      <c r="K72" s="2">
+      <c r="K72" s="1">
         <v>0</v>
       </c>
       <c r="L72" s="2">
@@ -5161,7 +5161,7 @@
       <c r="J73" s="2">
         <v>0</v>
       </c>
-      <c r="K73" s="2">
+      <c r="K73" s="1">
         <v>0</v>
       </c>
       <c r="L73" s="2">
@@ -5211,7 +5211,7 @@
       <c r="J74" s="2">
         <v>0</v>
       </c>
-      <c r="K74" s="2">
+      <c r="K74" s="1">
         <v>0</v>
       </c>
       <c r="L74" s="2">
@@ -5261,7 +5261,7 @@
       <c r="J75" s="2">
         <v>0</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="1">
         <v>0</v>
       </c>
       <c r="L75" s="2" t="s">
@@ -5311,7 +5311,7 @@
       <c r="J76" s="2">
         <v>0</v>
       </c>
-      <c r="K76" s="2">
+      <c r="K76" s="1">
         <v>0</v>
       </c>
       <c r="L76" s="2">
@@ -5361,7 +5361,7 @@
       <c r="J77" s="2">
         <v>0</v>
       </c>
-      <c r="K77" s="2">
+      <c r="K77" s="1">
         <v>0</v>
       </c>
       <c r="L77" s="2">
@@ -5409,9 +5409,9 @@
         <v>1</v>
       </c>
       <c r="J78" s="2">
-        <v>0</v>
-      </c>
-      <c r="K78" s="2">
+        <v>1</v>
+      </c>
+      <c r="K78" s="1">
         <v>0</v>
       </c>
       <c r="L78" s="2">
@@ -5459,9 +5459,9 @@
         <v>0</v>
       </c>
       <c r="J79" s="2">
-        <v>0</v>
-      </c>
-      <c r="K79" s="2">
+        <v>1</v>
+      </c>
+      <c r="K79" s="1">
         <v>0</v>
       </c>
       <c r="L79" s="2" t="s">
@@ -5511,7 +5511,7 @@
       <c r="J80" s="2">
         <v>0</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K80" s="1">
         <v>0</v>
       </c>
       <c r="L80" s="2">
@@ -5561,7 +5561,7 @@
       <c r="J81" s="2">
         <v>0</v>
       </c>
-      <c r="K81" s="2">
+      <c r="K81" s="1">
         <v>0</v>
       </c>
       <c r="L81" s="2">
@@ -5611,7 +5611,7 @@
       <c r="J82" s="2">
         <v>0</v>
       </c>
-      <c r="K82" s="2">
+      <c r="K82" s="1">
         <v>0</v>
       </c>
       <c r="L82" s="2">
@@ -5661,7 +5661,7 @@
       <c r="J83" s="2">
         <v>0</v>
       </c>
-      <c r="K83" s="2">
+      <c r="K83" s="1">
         <v>0</v>
       </c>
       <c r="L83" s="2">
@@ -5711,7 +5711,7 @@
       <c r="J84" s="2">
         <v>0</v>
       </c>
-      <c r="K84" s="2">
+      <c r="K84" s="1">
         <v>0</v>
       </c>
       <c r="L84" s="2">
@@ -5761,7 +5761,7 @@
       <c r="J85" s="2">
         <v>0</v>
       </c>
-      <c r="K85" s="2">
+      <c r="K85" s="1">
         <v>0</v>
       </c>
       <c r="L85" s="2">
@@ -5811,7 +5811,7 @@
       <c r="J86" s="2">
         <v>0</v>
       </c>
-      <c r="K86" s="2">
+      <c r="K86" s="1">
         <v>0</v>
       </c>
       <c r="L86" s="2">
@@ -5859,9 +5859,9 @@
         <v>0</v>
       </c>
       <c r="J87" s="2">
-        <v>0</v>
-      </c>
-      <c r="K87" s="2">
+        <v>1</v>
+      </c>
+      <c r="K87" s="1">
         <v>0</v>
       </c>
       <c r="L87" s="2">
@@ -5911,7 +5911,7 @@
       <c r="J88" s="2">
         <v>0</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K88" s="1">
         <v>0</v>
       </c>
       <c r="L88" s="2">
@@ -5961,7 +5961,7 @@
       <c r="J89" s="2">
         <v>0</v>
       </c>
-      <c r="K89" s="2">
+      <c r="K89" s="1">
         <v>0</v>
       </c>
       <c r="L89" s="2">
@@ -6011,7 +6011,7 @@
       <c r="J90" s="2">
         <v>0</v>
       </c>
-      <c r="K90" s="2">
+      <c r="K90" s="1">
         <v>0</v>
       </c>
       <c r="L90" s="2" t="s">
@@ -6061,7 +6061,7 @@
       <c r="J91" s="2">
         <v>0</v>
       </c>
-      <c r="K91" s="2">
+      <c r="K91" s="1">
         <v>0</v>
       </c>
       <c r="L91" s="2">
@@ -6111,7 +6111,7 @@
       <c r="J92" s="2">
         <v>0</v>
       </c>
-      <c r="K92" s="2">
+      <c r="K92" s="1">
         <v>0</v>
       </c>
       <c r="L92" s="2">
@@ -6161,7 +6161,7 @@
       <c r="J93" s="2">
         <v>0</v>
       </c>
-      <c r="K93" s="2">
+      <c r="K93" s="1">
         <v>0</v>
       </c>
       <c r="L93" s="2">
@@ -6211,7 +6211,7 @@
       <c r="J94" s="2">
         <v>0</v>
       </c>
-      <c r="K94" s="2">
+      <c r="K94" s="1">
         <v>0</v>
       </c>
       <c r="L94" s="2">
@@ -6261,7 +6261,7 @@
       <c r="J95" s="2">
         <v>0</v>
       </c>
-      <c r="K95" s="2">
+      <c r="K95" s="1">
         <v>0</v>
       </c>
       <c r="L95" s="2">
@@ -6311,7 +6311,7 @@
       <c r="J96" s="2">
         <v>0</v>
       </c>
-      <c r="K96" s="2">
+      <c r="K96" s="1">
         <v>0</v>
       </c>
       <c r="L96" s="2">
@@ -6361,7 +6361,7 @@
       <c r="J97" s="2">
         <v>0</v>
       </c>
-      <c r="K97" s="2">
+      <c r="K97" s="1">
         <v>0</v>
       </c>
       <c r="L97" s="2">
@@ -6411,7 +6411,7 @@
       <c r="J98" s="2">
         <v>0</v>
       </c>
-      <c r="K98" s="2">
+      <c r="K98" s="1">
         <v>0</v>
       </c>
       <c r="L98" s="2" t="s">
@@ -6461,7 +6461,7 @@
       <c r="J99" s="2">
         <v>0</v>
       </c>
-      <c r="K99" s="2">
+      <c r="K99" s="1">
         <v>0</v>
       </c>
       <c r="L99" s="2">
@@ -6511,7 +6511,7 @@
       <c r="J100" s="2">
         <v>0</v>
       </c>
-      <c r="K100" s="2">
+      <c r="K100" s="1">
         <v>0</v>
       </c>
       <c r="L100" s="2">
@@ -6561,7 +6561,7 @@
       <c r="J101" s="2">
         <v>0</v>
       </c>
-      <c r="K101" s="2">
+      <c r="K101" s="1">
         <v>0</v>
       </c>
       <c r="L101" s="2">
@@ -6609,9 +6609,9 @@
         <v>1</v>
       </c>
       <c r="J102" s="2">
-        <v>0</v>
-      </c>
-      <c r="K102" s="2">
+        <v>1</v>
+      </c>
+      <c r="K102" s="1">
         <v>0</v>
       </c>
       <c r="L102" s="2">
@@ -6661,7 +6661,7 @@
       <c r="J103" s="2">
         <v>0</v>
       </c>
-      <c r="K103" s="2">
+      <c r="K103" s="1">
         <v>0</v>
       </c>
       <c r="L103" s="2">
@@ -6711,7 +6711,7 @@
       <c r="J104" s="2">
         <v>0</v>
       </c>
-      <c r="K104" s="2">
+      <c r="K104" s="1">
         <v>0</v>
       </c>
       <c r="L104" s="2">
@@ -6761,7 +6761,7 @@
       <c r="J105" s="2">
         <v>0</v>
       </c>
-      <c r="K105" s="2">
+      <c r="K105" s="1">
         <v>0</v>
       </c>
       <c r="L105" s="2">
@@ -6811,7 +6811,7 @@
       <c r="J106" s="2">
         <v>0</v>
       </c>
-      <c r="K106" s="2">
+      <c r="K106" s="1">
         <v>0</v>
       </c>
       <c r="L106" s="2">
@@ -6861,7 +6861,7 @@
       <c r="J107" s="2">
         <v>0</v>
       </c>
-      <c r="K107" s="2">
+      <c r="K107" s="1">
         <v>0</v>
       </c>
       <c r="L107" s="2">
@@ -6911,7 +6911,7 @@
       <c r="J108" s="2">
         <v>0</v>
       </c>
-      <c r="K108" s="2">
+      <c r="K108" s="1">
         <v>0</v>
       </c>
       <c r="L108" s="2">
@@ -6961,7 +6961,7 @@
       <c r="J109" s="2">
         <v>0</v>
       </c>
-      <c r="K109" s="2">
+      <c r="K109" s="1">
         <v>0</v>
       </c>
       <c r="L109" s="2">
@@ -7011,7 +7011,7 @@
       <c r="J110" s="2">
         <v>0</v>
       </c>
-      <c r="K110" s="2">
+      <c r="K110" s="1">
         <v>0</v>
       </c>
       <c r="L110" s="2">
@@ -7061,7 +7061,7 @@
       <c r="J111" s="2">
         <v>0</v>
       </c>
-      <c r="K111" s="2">
+      <c r="K111" s="1">
         <v>0</v>
       </c>
       <c r="L111" s="2">
@@ -7111,7 +7111,7 @@
       <c r="J112" s="2">
         <v>0</v>
       </c>
-      <c r="K112" s="2">
+      <c r="K112" s="1">
         <v>0</v>
       </c>
       <c r="L112" s="2">
@@ -7161,7 +7161,7 @@
       <c r="J113" s="2">
         <v>0</v>
       </c>
-      <c r="K113" s="2">
+      <c r="K113" s="1">
         <v>0</v>
       </c>
       <c r="L113" s="2">
@@ -7211,7 +7211,7 @@
       <c r="J114" s="2">
         <v>0</v>
       </c>
-      <c r="K114" s="2">
+      <c r="K114" s="1">
         <v>0</v>
       </c>
       <c r="L114" s="2">
@@ -7261,7 +7261,7 @@
       <c r="J115" s="2">
         <v>0</v>
       </c>
-      <c r="K115" s="2">
+      <c r="K115" s="1">
         <v>0</v>
       </c>
       <c r="L115" s="2">
@@ -7311,7 +7311,7 @@
       <c r="J116" s="2">
         <v>0</v>
       </c>
-      <c r="K116" s="2">
+      <c r="K116" s="1">
         <v>0</v>
       </c>
       <c r="L116" s="2" t="s">
@@ -7361,7 +7361,7 @@
       <c r="J117" s="2">
         <v>0</v>
       </c>
-      <c r="K117" s="2">
+      <c r="K117" s="1">
         <v>0</v>
       </c>
       <c r="L117" s="2">
@@ -7411,7 +7411,7 @@
       <c r="J118" s="2">
         <v>0</v>
       </c>
-      <c r="K118" s="2">
+      <c r="K118" s="1">
         <v>0</v>
       </c>
       <c r="L118" s="2">
@@ -7461,7 +7461,7 @@
       <c r="J119" s="2">
         <v>0</v>
       </c>
-      <c r="K119" s="2">
+      <c r="K119" s="1">
         <v>0</v>
       </c>
       <c r="L119" s="2">
@@ -7511,7 +7511,7 @@
       <c r="J120" s="2">
         <v>0</v>
       </c>
-      <c r="K120" s="2">
+      <c r="K120" s="1">
         <v>0</v>
       </c>
       <c r="L120" s="2">
@@ -7561,7 +7561,7 @@
       <c r="J121" s="2">
         <v>0</v>
       </c>
-      <c r="K121" s="2">
+      <c r="K121" s="1">
         <v>0</v>
       </c>
       <c r="L121" s="2">
@@ -7611,7 +7611,7 @@
       <c r="J122" s="2">
         <v>0</v>
       </c>
-      <c r="K122" s="2">
+      <c r="K122" s="1">
         <v>0</v>
       </c>
       <c r="L122" s="2">
@@ -7661,7 +7661,7 @@
       <c r="J123" s="2">
         <v>0</v>
       </c>
-      <c r="K123" s="2">
+      <c r="K123" s="1">
         <v>0</v>
       </c>
       <c r="L123" s="2">
@@ -7711,7 +7711,7 @@
       <c r="J124" s="2">
         <v>0</v>
       </c>
-      <c r="K124" s="2">
+      <c r="K124" s="1">
         <v>0</v>
       </c>
       <c r="L124" s="2">
@@ -7761,7 +7761,7 @@
       <c r="J125" s="2">
         <v>0</v>
       </c>
-      <c r="K125" s="2">
+      <c r="K125" s="1">
         <v>0</v>
       </c>
       <c r="L125" s="2" t="s">
@@ -7811,7 +7811,7 @@
       <c r="J126" s="2">
         <v>0</v>
       </c>
-      <c r="K126" s="2">
+      <c r="K126" s="1">
         <v>0</v>
       </c>
       <c r="L126" s="2">
@@ -7861,7 +7861,7 @@
       <c r="J127" s="2">
         <v>0</v>
       </c>
-      <c r="K127" s="2">
+      <c r="K127" s="1">
         <v>0</v>
       </c>
       <c r="L127" s="2">
@@ -7911,7 +7911,7 @@
       <c r="J128" s="2">
         <v>0</v>
       </c>
-      <c r="K128" s="2">
+      <c r="K128" s="1">
         <v>0</v>
       </c>
       <c r="L128" s="2">
@@ -7961,7 +7961,7 @@
       <c r="J129" s="2">
         <v>0</v>
       </c>
-      <c r="K129" s="2">
+      <c r="K129" s="1">
         <v>0</v>
       </c>
       <c r="L129" s="2">
@@ -8011,7 +8011,7 @@
       <c r="J130" s="2">
         <v>0</v>
       </c>
-      <c r="K130" s="2">
+      <c r="K130" s="1">
         <v>0</v>
       </c>
       <c r="L130" s="2">
@@ -8061,7 +8061,7 @@
       <c r="J131" s="2">
         <v>0</v>
       </c>
-      <c r="K131" s="2">
+      <c r="K131" s="1">
         <v>0</v>
       </c>
       <c r="L131" s="2">
@@ -8111,7 +8111,7 @@
       <c r="J132" s="2">
         <v>0</v>
       </c>
-      <c r="K132" s="2">
+      <c r="K132" s="1">
         <v>0</v>
       </c>
       <c r="L132" s="2">
@@ -8161,7 +8161,7 @@
       <c r="J133" s="2">
         <v>0</v>
       </c>
-      <c r="K133" s="2">
+      <c r="K133" s="1">
         <v>0</v>
       </c>
       <c r="L133" s="2">
@@ -8211,7 +8211,7 @@
       <c r="J134" s="2">
         <v>0</v>
       </c>
-      <c r="K134" s="2">
+      <c r="K134" s="1">
         <v>0</v>
       </c>
       <c r="L134" s="2" t="s">
@@ -8261,7 +8261,7 @@
       <c r="J135" s="2">
         <v>0</v>
       </c>
-      <c r="K135" s="2">
+      <c r="K135" s="1">
         <v>0</v>
       </c>
       <c r="L135" s="2">
@@ -8311,7 +8311,7 @@
       <c r="J136" s="2">
         <v>0</v>
       </c>
-      <c r="K136" s="2">
+      <c r="K136" s="1">
         <v>0</v>
       </c>
       <c r="L136" s="2">
@@ -8361,7 +8361,7 @@
       <c r="J137" s="2">
         <v>0</v>
       </c>
-      <c r="K137" s="2">
+      <c r="K137" s="1">
         <v>0</v>
       </c>
       <c r="L137" s="2">
@@ -8411,7 +8411,7 @@
       <c r="J138" s="2">
         <v>0</v>
       </c>
-      <c r="K138" s="2">
+      <c r="K138" s="1">
         <v>0</v>
       </c>
       <c r="L138" s="2">
@@ -8461,7 +8461,7 @@
       <c r="J139" s="2">
         <v>0</v>
       </c>
-      <c r="K139" s="2">
+      <c r="K139" s="1">
         <v>0</v>
       </c>
       <c r="L139" s="2">
@@ -8511,7 +8511,7 @@
       <c r="J140" s="2">
         <v>0</v>
       </c>
-      <c r="K140" s="2">
+      <c r="K140" s="1">
         <v>0</v>
       </c>
       <c r="L140" s="2">
@@ -8561,7 +8561,7 @@
       <c r="J141" s="2">
         <v>0</v>
       </c>
-      <c r="K141" s="2">
+      <c r="K141" s="1">
         <v>0</v>
       </c>
       <c r="L141" s="2">
@@ -8611,7 +8611,7 @@
       <c r="J142" s="2">
         <v>0</v>
       </c>
-      <c r="K142" s="2">
+      <c r="K142" s="1">
         <v>0</v>
       </c>
       <c r="L142" s="2">
@@ -8661,7 +8661,7 @@
       <c r="J143" s="2">
         <v>0</v>
       </c>
-      <c r="K143" s="2">
+      <c r="K143" s="1">
         <v>0</v>
       </c>
       <c r="L143" s="2" t="s">
@@ -8711,7 +8711,7 @@
       <c r="J144" s="2">
         <v>0</v>
       </c>
-      <c r="K144" s="2">
+      <c r="K144" s="1">
         <v>0</v>
       </c>
       <c r="L144" s="2">
@@ -8761,7 +8761,7 @@
       <c r="J145" s="2">
         <v>0</v>
       </c>
-      <c r="K145" s="2">
+      <c r="K145" s="1">
         <v>0</v>
       </c>
       <c r="L145" s="2">
@@ -8811,7 +8811,7 @@
       <c r="J146" s="2">
         <v>0</v>
       </c>
-      <c r="K146" s="2">
+      <c r="K146" s="1">
         <v>0</v>
       </c>
       <c r="L146" s="2">
@@ -8861,7 +8861,7 @@
       <c r="J147" s="2">
         <v>0</v>
       </c>
-      <c r="K147" s="2">
+      <c r="K147" s="1">
         <v>0</v>
       </c>
       <c r="L147" s="2">
@@ -8911,7 +8911,7 @@
       <c r="J148" s="2">
         <v>0</v>
       </c>
-      <c r="K148" s="2">
+      <c r="K148" s="1">
         <v>0</v>
       </c>
       <c r="L148" s="2">
@@ -8961,7 +8961,7 @@
       <c r="J149" s="2">
         <v>0</v>
       </c>
-      <c r="K149" s="2">
+      <c r="K149" s="1">
         <v>0</v>
       </c>
       <c r="L149" s="2">
@@ -9011,7 +9011,7 @@
       <c r="J150" s="2">
         <v>0</v>
       </c>
-      <c r="K150" s="2">
+      <c r="K150" s="1">
         <v>0</v>
       </c>
       <c r="L150" s="2">
@@ -9061,7 +9061,7 @@
       <c r="J151" s="2">
         <v>0</v>
       </c>
-      <c r="K151" s="2">
+      <c r="K151" s="1">
         <v>0</v>
       </c>
       <c r="L151" s="2">
@@ -9109,9 +9109,9 @@
         <v>1</v>
       </c>
       <c r="J152" s="2">
-        <v>0</v>
-      </c>
-      <c r="K152" s="2">
+        <v>1</v>
+      </c>
+      <c r="K152" s="1">
         <v>0</v>
       </c>
       <c r="L152" s="2">
@@ -9161,7 +9161,7 @@
       <c r="J153" s="2">
         <v>0</v>
       </c>
-      <c r="K153" s="2">
+      <c r="K153" s="1">
         <v>0</v>
       </c>
       <c r="L153" s="2">
@@ -9209,9 +9209,9 @@
         <v>1</v>
       </c>
       <c r="J154" s="2">
-        <v>0</v>
-      </c>
-      <c r="K154" s="2">
+        <v>1</v>
+      </c>
+      <c r="K154" s="1">
         <v>0</v>
       </c>
       <c r="L154" s="2">
@@ -14416,8 +14416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="K160" sqref="K160"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14455,7 +14455,7 @@
         <v>-1</v>
       </c>
       <c r="J1" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K1" s="2">
         <v>0</v>
@@ -14467,7 +14467,7 @@
         <v>56</v>
       </c>
       <c r="N1" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O1" s="9">
         <v>0</v>
@@ -14517,7 +14517,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="9">
         <v>0</v>
@@ -14567,7 +14567,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="9">
         <v>0</v>
@@ -14817,7 +14817,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O8" s="9">
         <v>0</v>
@@ -14867,7 +14867,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O9" s="9">
         <v>0</v>
@@ -14917,7 +14917,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10" s="9">
         <v>0</v>
@@ -15055,7 +15055,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
@@ -15167,7 +15167,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O15" s="9">
         <v>0</v>
@@ -15217,7 +15217,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O16" s="9">
         <v>0</v>
@@ -15267,7 +15267,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O17" s="9">
         <v>0</v>
@@ -15307,7 +15307,7 @@
       <c r="J18" s="2">
         <v>0</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <v>0</v>
       </c>
       <c r="L18" s="2">
@@ -15357,7 +15357,7 @@
       <c r="J19" s="2">
         <v>0</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>1</v>
       </c>
       <c r="L19" s="2">
@@ -15407,7 +15407,7 @@
       <c r="J20" s="2">
         <v>0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>0</v>
       </c>
       <c r="L20" s="2">
@@ -15457,7 +15457,7 @@
       <c r="J21" s="2">
         <v>0</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>0</v>
       </c>
       <c r="L21" s="2">
@@ -15467,7 +15467,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O21" s="9">
         <v>0</v>
@@ -15507,7 +15507,7 @@
       <c r="J22" s="2">
         <v>0</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>0</v>
       </c>
       <c r="L22" s="2" t="s">
@@ -15517,7 +15517,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O22" s="9">
         <v>0</v>
@@ -15557,7 +15557,7 @@
       <c r="J23" s="2">
         <v>0</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>0</v>
       </c>
       <c r="L23" s="2">
@@ -15567,7 +15567,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O23" s="9">
         <v>0</v>
@@ -15607,7 +15607,7 @@
       <c r="J24" s="2">
         <v>0</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>0</v>
       </c>
       <c r="L24" s="2">
@@ -15657,7 +15657,7 @@
       <c r="J25" s="2">
         <v>0</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>0</v>
       </c>
       <c r="L25" s="2">
@@ -15707,7 +15707,7 @@
       <c r="J26" s="2">
         <v>0</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="1">
         <v>0</v>
       </c>
       <c r="L26" s="2">
@@ -15757,7 +15757,7 @@
       <c r="J27" s="2">
         <v>0</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1">
         <v>0</v>
       </c>
       <c r="L27" s="2">
@@ -15805,9 +15805,9 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>0</v>
-      </c>
-      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
         <v>0</v>
       </c>
       <c r="L28" s="2">
@@ -15857,7 +15857,7 @@
       <c r="J29" s="2">
         <v>0</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>0</v>
       </c>
       <c r="L29" s="2">
@@ -15907,7 +15907,7 @@
       <c r="J30" s="2">
         <v>0</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="1">
         <v>0</v>
       </c>
       <c r="L30" s="2">
@@ -15917,7 +15917,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O30" s="9">
         <v>0</v>
@@ -15957,7 +15957,7 @@
       <c r="J31" s="2">
         <v>0</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1">
         <v>0</v>
       </c>
       <c r="L31" s="2" t="s">
@@ -15967,7 +15967,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O31" s="9">
         <v>0</v>
@@ -16007,7 +16007,7 @@
       <c r="J32" s="2">
         <v>0</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>0</v>
       </c>
       <c r="L32" s="2">
@@ -16017,7 +16017,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O32" s="9">
         <v>0</v>
@@ -16057,7 +16057,7 @@
       <c r="J33" s="2">
         <v>0</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="1">
         <v>0</v>
       </c>
       <c r="L33" s="2">
@@ -16107,7 +16107,7 @@
       <c r="J34" s="2">
         <v>0</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>0</v>
       </c>
       <c r="L34" s="2">
@@ -16157,7 +16157,7 @@
       <c r="J35" s="2">
         <v>0</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="1">
         <v>0</v>
       </c>
       <c r="L35" s="2">
@@ -16207,7 +16207,7 @@
       <c r="J36" s="2">
         <v>0</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="1">
         <v>0</v>
       </c>
       <c r="L36" s="2">
@@ -16257,7 +16257,7 @@
       <c r="J37" s="2">
         <v>0</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="1">
         <v>0</v>
       </c>
       <c r="L37" s="2">
@@ -16307,7 +16307,7 @@
       <c r="J38" s="2">
         <v>0</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="1">
         <v>0</v>
       </c>
       <c r="L38" s="2">
@@ -16317,7 +16317,7 @@
         <v>0</v>
       </c>
       <c r="N38" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O38" s="9">
         <v>1</v>
@@ -16357,7 +16357,7 @@
       <c r="J39" s="2">
         <v>0</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="1">
         <v>0</v>
       </c>
       <c r="L39" s="2" t="s">
@@ -16367,7 +16367,7 @@
         <v>0</v>
       </c>
       <c r="N39" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O39" s="9">
         <v>1</v>
@@ -16407,7 +16407,7 @@
       <c r="J40" s="2">
         <v>0</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="1">
         <v>0</v>
       </c>
       <c r="L40" s="2">
@@ -16417,7 +16417,7 @@
         <v>0</v>
       </c>
       <c r="N40" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O40" s="9">
         <v>1</v>
@@ -16457,7 +16457,7 @@
       <c r="J41" s="2">
         <v>0</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="1">
         <v>0</v>
       </c>
       <c r="L41" s="2">
@@ -16507,7 +16507,7 @@
       <c r="J42" s="2">
         <v>0</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="1">
         <v>0</v>
       </c>
       <c r="L42" s="2">
@@ -16557,7 +16557,7 @@
       <c r="J43" s="2">
         <v>0</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="1">
         <v>0</v>
       </c>
       <c r="L43" s="2">
@@ -16607,7 +16607,7 @@
       <c r="J44" s="2">
         <v>0</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1">
         <v>0</v>
       </c>
       <c r="L44" s="2">
@@ -16657,7 +16657,7 @@
       <c r="J45" s="2">
         <v>0</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>0</v>
       </c>
       <c r="L45" s="2">
@@ -16707,7 +16707,7 @@
       <c r="J46" s="2">
         <v>0</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="1">
         <v>0</v>
       </c>
       <c r="L46" s="2">
@@ -16757,7 +16757,7 @@
       <c r="J47" s="2">
         <v>0</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="1">
         <v>0</v>
       </c>
       <c r="L47" s="2">
@@ -16767,7 +16767,7 @@
         <v>0</v>
       </c>
       <c r="N47" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O47" s="9">
         <v>1</v>
@@ -16807,7 +16807,7 @@
       <c r="J48" s="2">
         <v>0</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="1">
         <v>0</v>
       </c>
       <c r="L48" s="2" t="s">
@@ -16817,7 +16817,7 @@
         <v>0</v>
       </c>
       <c r="N48" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O48" s="9">
         <v>1</v>
@@ -16857,7 +16857,7 @@
       <c r="J49" s="2">
         <v>0</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="1">
         <v>0</v>
       </c>
       <c r="L49" s="2">
@@ -16867,7 +16867,7 @@
         <v>0</v>
       </c>
       <c r="N49" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O49" s="9">
         <v>1</v>
@@ -16907,7 +16907,7 @@
       <c r="J50" s="2">
         <v>0</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="1">
         <v>0</v>
       </c>
       <c r="L50" s="2">
@@ -16957,7 +16957,7 @@
       <c r="J51" s="2">
         <v>0</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="1">
         <v>0</v>
       </c>
       <c r="L51" s="2">
@@ -17007,7 +17007,7 @@
       <c r="J52" s="2">
         <v>0</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="1">
         <v>0</v>
       </c>
       <c r="L52" s="2">
@@ -17057,7 +17057,7 @@
       <c r="J53" s="2">
         <v>0</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="1">
         <v>0</v>
       </c>
       <c r="L53" s="2">
@@ -17107,7 +17107,7 @@
       <c r="J54" s="2">
         <v>0</v>
       </c>
-      <c r="K54" s="2">
+      <c r="K54" s="1">
         <v>0</v>
       </c>
       <c r="L54" s="2">
@@ -17157,7 +17157,7 @@
       <c r="J55" s="2">
         <v>0</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="1">
         <v>0</v>
       </c>
       <c r="L55" s="2">
@@ -17207,7 +17207,7 @@
       <c r="J56" s="2">
         <v>0</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K56" s="1">
         <v>0</v>
       </c>
       <c r="L56" s="2">
@@ -17217,7 +17217,7 @@
         <v>0</v>
       </c>
       <c r="N56" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O56" s="9">
         <v>1</v>
@@ -17257,7 +17257,7 @@
       <c r="J57" s="2">
         <v>0</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="1">
         <v>0</v>
       </c>
       <c r="L57" s="2" t="s">
@@ -17267,7 +17267,7 @@
         <v>49</v>
       </c>
       <c r="N57" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O57" s="9">
         <v>1</v>
@@ -17307,7 +17307,7 @@
       <c r="J58" s="2">
         <v>0</v>
       </c>
-      <c r="K58" s="2">
+      <c r="K58" s="1">
         <v>0</v>
       </c>
       <c r="L58" s="2">
@@ -17317,7 +17317,7 @@
         <v>43</v>
       </c>
       <c r="N58" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O58" s="9">
         <v>0</v>
@@ -17357,7 +17357,7 @@
       <c r="J59" s="2">
         <v>0</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="1">
         <v>0</v>
       </c>
       <c r="L59" s="2">
@@ -17407,7 +17407,7 @@
       <c r="J60" s="2">
         <v>0</v>
       </c>
-      <c r="K60" s="2">
+      <c r="K60" s="1">
         <v>0</v>
       </c>
       <c r="L60" s="2">
@@ -17457,7 +17457,7 @@
       <c r="J61" s="2">
         <v>0</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="1">
         <v>0</v>
       </c>
       <c r="L61" s="2">
@@ -17505,9 +17505,9 @@
         <v>1</v>
       </c>
       <c r="J62" s="2">
-        <v>0</v>
-      </c>
-      <c r="K62" s="2">
+        <v>1</v>
+      </c>
+      <c r="K62" s="1">
         <v>0</v>
       </c>
       <c r="L62" s="2">
@@ -17557,7 +17557,7 @@
       <c r="J63" s="2">
         <v>0</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="1">
         <v>0</v>
       </c>
       <c r="L63" s="2">
@@ -17607,7 +17607,7 @@
       <c r="J64" s="2">
         <v>0</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="1">
         <v>0</v>
       </c>
       <c r="L64" s="2">
@@ -17617,7 +17617,7 @@
         <v>0</v>
       </c>
       <c r="N64" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O64" s="9">
         <v>0</v>
@@ -17657,7 +17657,7 @@
       <c r="J65" s="2">
         <v>0</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="1">
         <v>0</v>
       </c>
       <c r="L65" s="2" t="s">
@@ -17667,7 +17667,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="O65" s="9">
         <v>0</v>
@@ -17707,7 +17707,7 @@
       <c r="J66" s="2">
         <v>0</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="1">
         <v>0</v>
       </c>
       <c r="L66" s="2">
@@ -17717,7 +17717,7 @@
         <v>0</v>
       </c>
       <c r="N66" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O66" s="9">
         <v>0</v>
@@ -17757,7 +17757,7 @@
       <c r="J67" s="2">
         <v>0</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="1">
         <v>0</v>
       </c>
       <c r="L67" s="2">
@@ -17807,7 +17807,7 @@
       <c r="J68" s="2">
         <v>0</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="1">
         <v>0</v>
       </c>
       <c r="L68" s="2">
@@ -17857,7 +17857,7 @@
       <c r="J69" s="2">
         <v>0</v>
       </c>
-      <c r="K69" s="2">
+      <c r="K69" s="1">
         <v>0</v>
       </c>
       <c r="L69" s="2">
@@ -17907,7 +17907,7 @@
       <c r="J70" s="2">
         <v>0</v>
       </c>
-      <c r="K70" s="2">
+      <c r="K70" s="1">
         <v>0</v>
       </c>
       <c r="L70" s="2">
@@ -17957,7 +17957,7 @@
       <c r="J71" s="2">
         <v>0</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="1">
         <v>0</v>
       </c>
       <c r="L71" s="2">
@@ -18007,7 +18007,7 @@
       <c r="J72" s="2">
         <v>0</v>
       </c>
-      <c r="K72" s="2">
+      <c r="K72" s="1">
         <v>0</v>
       </c>
       <c r="L72" s="2">
@@ -18017,7 +18017,7 @@
         <v>0</v>
       </c>
       <c r="N72" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O72" s="9">
         <v>0</v>
@@ -18057,7 +18057,7 @@
       <c r="J73" s="2">
         <v>0</v>
       </c>
-      <c r="K73" s="2">
+      <c r="K73" s="1">
         <v>0</v>
       </c>
       <c r="L73" s="2" t="s">
@@ -18067,7 +18067,7 @@
         <v>0</v>
       </c>
       <c r="N73" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O73" s="9">
         <v>0</v>
@@ -18107,7 +18107,7 @@
       <c r="J74" s="2">
         <v>0</v>
       </c>
-      <c r="K74" s="2">
+      <c r="K74" s="1">
         <v>0</v>
       </c>
       <c r="L74" s="2">
@@ -18117,7 +18117,7 @@
         <v>0</v>
       </c>
       <c r="N74" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O74" s="9">
         <v>0</v>
@@ -18157,7 +18157,7 @@
       <c r="J75" s="2">
         <v>0</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="1">
         <v>0</v>
       </c>
       <c r="L75" s="2">
@@ -18205,9 +18205,9 @@
         <v>1</v>
       </c>
       <c r="J76" s="2">
-        <v>0</v>
-      </c>
-      <c r="K76" s="2">
+        <v>1</v>
+      </c>
+      <c r="K76" s="1">
         <v>0</v>
       </c>
       <c r="L76" s="2">
@@ -18217,7 +18217,7 @@
         <v>45</v>
       </c>
       <c r="N76" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O76" s="9">
         <v>0</v>
@@ -18255,9 +18255,9 @@
         <v>0</v>
       </c>
       <c r="J77" s="2">
-        <v>0</v>
-      </c>
-      <c r="K77" s="2">
+        <v>1</v>
+      </c>
+      <c r="K77" s="1">
         <v>0</v>
       </c>
       <c r="L77" s="2" t="s">
@@ -18267,7 +18267,7 @@
         <v>51</v>
       </c>
       <c r="N77" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="O77" s="9">
         <v>0</v>
@@ -18307,7 +18307,7 @@
       <c r="J78" s="2">
         <v>0</v>
       </c>
-      <c r="K78" s="2">
+      <c r="K78" s="1">
         <v>0</v>
       </c>
       <c r="L78" s="2">
@@ -18317,7 +18317,7 @@
         <v>0</v>
       </c>
       <c r="N78" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O78" s="9">
         <v>0</v>
@@ -18357,7 +18357,7 @@
       <c r="J79" s="2">
         <v>0</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K79" s="1">
         <v>0</v>
       </c>
       <c r="L79" s="2">
@@ -18407,7 +18407,7 @@
       <c r="J80" s="2">
         <v>0</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K80" s="1">
         <v>0</v>
       </c>
       <c r="L80" s="2">
@@ -18457,7 +18457,7 @@
       <c r="J81" s="2">
         <v>0</v>
       </c>
-      <c r="K81" s="2">
+      <c r="K81" s="1">
         <v>0</v>
       </c>
       <c r="L81" s="2">
@@ -18507,7 +18507,7 @@
       <c r="J82" s="2">
         <v>0</v>
       </c>
-      <c r="K82" s="2">
+      <c r="K82" s="1">
         <v>0</v>
       </c>
       <c r="L82" s="2">
@@ -18557,7 +18557,7 @@
       <c r="J83" s="2">
         <v>0</v>
       </c>
-      <c r="K83" s="2">
+      <c r="K83" s="1">
         <v>0</v>
       </c>
       <c r="L83" s="2">
@@ -18607,7 +18607,7 @@
       <c r="J84" s="2">
         <v>0</v>
       </c>
-      <c r="K84" s="2">
+      <c r="K84" s="1">
         <v>0</v>
       </c>
       <c r="L84" s="2">
@@ -18655,9 +18655,9 @@
         <v>0</v>
       </c>
       <c r="J85" s="2">
-        <v>0</v>
-      </c>
-      <c r="K85" s="2">
+        <v>1</v>
+      </c>
+      <c r="K85" s="1">
         <v>0</v>
       </c>
       <c r="L85" s="2">
@@ -18707,7 +18707,7 @@
       <c r="J86" s="2">
         <v>0</v>
       </c>
-      <c r="K86" s="2">
+      <c r="K86" s="1">
         <v>0</v>
       </c>
       <c r="L86" s="2">
@@ -18757,7 +18757,7 @@
       <c r="J87" s="2">
         <v>0</v>
       </c>
-      <c r="K87" s="2">
+      <c r="K87" s="1">
         <v>0</v>
       </c>
       <c r="L87" s="2">
@@ -18767,7 +18767,7 @@
         <v>0</v>
       </c>
       <c r="N87" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O87" s="9">
         <v>0</v>
@@ -18807,7 +18807,7 @@
       <c r="J88" s="2">
         <v>0</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K88" s="1">
         <v>0</v>
       </c>
       <c r="L88" s="2" t="s">
@@ -18817,7 +18817,7 @@
         <v>0</v>
       </c>
       <c r="N88" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="O88" s="9">
         <v>0</v>
@@ -18857,7 +18857,7 @@
       <c r="J89" s="2">
         <v>0</v>
       </c>
-      <c r="K89" s="2">
+      <c r="K89" s="1">
         <v>0</v>
       </c>
       <c r="L89" s="2">
@@ -18867,7 +18867,7 @@
         <v>0</v>
       </c>
       <c r="N89" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O89" s="9">
         <v>0</v>
@@ -18907,7 +18907,7 @@
       <c r="J90" s="2">
         <v>0</v>
       </c>
-      <c r="K90" s="2">
+      <c r="K90" s="1">
         <v>0</v>
       </c>
       <c r="L90" s="2">
@@ -18957,7 +18957,7 @@
       <c r="J91" s="2">
         <v>0</v>
       </c>
-      <c r="K91" s="2">
+      <c r="K91" s="1">
         <v>0</v>
       </c>
       <c r="L91" s="2">
@@ -19007,7 +19007,7 @@
       <c r="J92" s="2">
         <v>0</v>
       </c>
-      <c r="K92" s="2">
+      <c r="K92" s="1">
         <v>0</v>
       </c>
       <c r="L92" s="2">
@@ -19057,7 +19057,7 @@
       <c r="J93" s="2">
         <v>0</v>
       </c>
-      <c r="K93" s="2">
+      <c r="K93" s="1">
         <v>0</v>
       </c>
       <c r="L93" s="2">
@@ -19107,7 +19107,7 @@
       <c r="J94" s="2">
         <v>0</v>
       </c>
-      <c r="K94" s="2">
+      <c r="K94" s="1">
         <v>0</v>
       </c>
       <c r="L94" s="2">
@@ -19157,7 +19157,7 @@
       <c r="J95" s="2">
         <v>0</v>
       </c>
-      <c r="K95" s="2">
+      <c r="K95" s="1">
         <v>0</v>
       </c>
       <c r="L95" s="2">
@@ -19167,7 +19167,7 @@
         <v>0</v>
       </c>
       <c r="N95" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O95" s="9">
         <v>0</v>
@@ -19207,7 +19207,7 @@
       <c r="J96" s="2">
         <v>0</v>
       </c>
-      <c r="K96" s="2">
+      <c r="K96" s="1">
         <v>0</v>
       </c>
       <c r="L96" s="2" t="s">
@@ -19217,7 +19217,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O96" s="9">
         <v>0</v>
@@ -19257,7 +19257,7 @@
       <c r="J97" s="2">
         <v>0</v>
       </c>
-      <c r="K97" s="2">
+      <c r="K97" s="1">
         <v>0</v>
       </c>
       <c r="L97" s="2">
@@ -19267,7 +19267,7 @@
         <v>0</v>
       </c>
       <c r="N97" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O97" s="9">
         <v>0</v>
@@ -19307,7 +19307,7 @@
       <c r="J98" s="2">
         <v>0</v>
       </c>
-      <c r="K98" s="2">
+      <c r="K98" s="1">
         <v>0</v>
       </c>
       <c r="L98" s="2">
@@ -19357,7 +19357,7 @@
       <c r="J99" s="2">
         <v>0</v>
       </c>
-      <c r="K99" s="2">
+      <c r="K99" s="1">
         <v>0</v>
       </c>
       <c r="L99" s="2">
@@ -19405,9 +19405,9 @@
         <v>1</v>
       </c>
       <c r="J100" s="2">
-        <v>0</v>
-      </c>
-      <c r="K100" s="2">
+        <v>1</v>
+      </c>
+      <c r="K100" s="1">
         <v>0</v>
       </c>
       <c r="L100" s="2">
@@ -19457,7 +19457,7 @@
       <c r="J101" s="2">
         <v>0</v>
       </c>
-      <c r="K101" s="2">
+      <c r="K101" s="1">
         <v>0</v>
       </c>
       <c r="L101" s="2">
@@ -19507,7 +19507,7 @@
       <c r="J102" s="2">
         <v>0</v>
       </c>
-      <c r="K102" s="2">
+      <c r="K102" s="1">
         <v>0</v>
       </c>
       <c r="L102" s="2">
@@ -19557,7 +19557,7 @@
       <c r="J103" s="2">
         <v>0</v>
       </c>
-      <c r="K103" s="2">
+      <c r="K103" s="1">
         <v>0</v>
       </c>
       <c r="L103" s="2">
@@ -19607,7 +19607,7 @@
       <c r="J104" s="2">
         <v>0</v>
       </c>
-      <c r="K104" s="2">
+      <c r="K104" s="1">
         <v>0</v>
       </c>
       <c r="L104" s="2">
@@ -19657,7 +19657,7 @@
       <c r="J105" s="2">
         <v>0</v>
       </c>
-      <c r="K105" s="2">
+      <c r="K105" s="1">
         <v>0</v>
       </c>
       <c r="L105" s="2">
@@ -19707,7 +19707,7 @@
       <c r="J106" s="2">
         <v>0</v>
       </c>
-      <c r="K106" s="2">
+      <c r="K106" s="1">
         <v>0</v>
       </c>
       <c r="L106" s="2">
@@ -19757,7 +19757,7 @@
       <c r="J107" s="2">
         <v>0</v>
       </c>
-      <c r="K107" s="2">
+      <c r="K107" s="1">
         <v>0</v>
       </c>
       <c r="L107" s="2">
@@ -19807,7 +19807,7 @@
       <c r="J108" s="2">
         <v>0</v>
       </c>
-      <c r="K108" s="2">
+      <c r="K108" s="1">
         <v>0</v>
       </c>
       <c r="L108" s="2">
@@ -19857,7 +19857,7 @@
       <c r="J109" s="2">
         <v>0</v>
       </c>
-      <c r="K109" s="2">
+      <c r="K109" s="1">
         <v>0</v>
       </c>
       <c r="L109" s="2">
@@ -19907,7 +19907,7 @@
       <c r="J110" s="2">
         <v>0</v>
       </c>
-      <c r="K110" s="2">
+      <c r="K110" s="1">
         <v>0</v>
       </c>
       <c r="L110" s="2">
@@ -19957,7 +19957,7 @@
       <c r="J111" s="2">
         <v>0</v>
       </c>
-      <c r="K111" s="2">
+      <c r="K111" s="1">
         <v>0</v>
       </c>
       <c r="L111" s="2">
@@ -20007,7 +20007,7 @@
       <c r="J112" s="2">
         <v>0</v>
       </c>
-      <c r="K112" s="2">
+      <c r="K112" s="1">
         <v>0</v>
       </c>
       <c r="L112" s="2">
@@ -20057,7 +20057,7 @@
       <c r="J113" s="2">
         <v>0</v>
       </c>
-      <c r="K113" s="2">
+      <c r="K113" s="1">
         <v>0</v>
       </c>
       <c r="L113" s="2">
@@ -20067,7 +20067,7 @@
         <v>0</v>
       </c>
       <c r="N113" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O113" s="9">
         <v>0</v>
@@ -20107,7 +20107,7 @@
       <c r="J114" s="2">
         <v>0</v>
       </c>
-      <c r="K114" s="2">
+      <c r="K114" s="1">
         <v>0</v>
       </c>
       <c r="L114" s="2" t="s">
@@ -20117,7 +20117,7 @@
         <v>0</v>
       </c>
       <c r="N114" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O114" s="9">
         <v>0</v>
@@ -20157,7 +20157,7 @@
       <c r="J115" s="2">
         <v>0</v>
       </c>
-      <c r="K115" s="2">
+      <c r="K115" s="1">
         <v>0</v>
       </c>
       <c r="L115" s="2">
@@ -20167,7 +20167,7 @@
         <v>0</v>
       </c>
       <c r="N115" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O115" s="9">
         <v>0</v>
@@ -20207,7 +20207,7 @@
       <c r="J116" s="2">
         <v>0</v>
       </c>
-      <c r="K116" s="2">
+      <c r="K116" s="1">
         <v>0</v>
       </c>
       <c r="L116" s="2">
@@ -20257,7 +20257,7 @@
       <c r="J117" s="2">
         <v>0</v>
       </c>
-      <c r="K117" s="2">
+      <c r="K117" s="1">
         <v>0</v>
       </c>
       <c r="L117" s="2">
@@ -20307,7 +20307,7 @@
       <c r="J118" s="2">
         <v>0</v>
       </c>
-      <c r="K118" s="2">
+      <c r="K118" s="1">
         <v>0</v>
       </c>
       <c r="L118" s="2">
@@ -20357,7 +20357,7 @@
       <c r="J119" s="2">
         <v>0</v>
       </c>
-      <c r="K119" s="2">
+      <c r="K119" s="1">
         <v>0</v>
       </c>
       <c r="L119" s="2">
@@ -20407,7 +20407,7 @@
       <c r="J120" s="2">
         <v>0</v>
       </c>
-      <c r="K120" s="2">
+      <c r="K120" s="1">
         <v>0</v>
       </c>
       <c r="L120" s="2">
@@ -20457,7 +20457,7 @@
       <c r="J121" s="2">
         <v>0</v>
       </c>
-      <c r="K121" s="2">
+      <c r="K121" s="1">
         <v>0</v>
       </c>
       <c r="L121" s="2">
@@ -20507,7 +20507,7 @@
       <c r="J122" s="2">
         <v>0</v>
       </c>
-      <c r="K122" s="2">
+      <c r="K122" s="1">
         <v>0</v>
       </c>
       <c r="L122" s="2">
@@ -20517,7 +20517,7 @@
         <v>0</v>
       </c>
       <c r="N122" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O122" s="9">
         <v>1</v>
@@ -20557,7 +20557,7 @@
       <c r="J123" s="2">
         <v>0</v>
       </c>
-      <c r="K123" s="2">
+      <c r="K123" s="1">
         <v>0</v>
       </c>
       <c r="L123" s="2" t="s">
@@ -20567,7 +20567,7 @@
         <v>0</v>
       </c>
       <c r="N123" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O123" s="9">
         <v>1</v>
@@ -20607,7 +20607,7 @@
       <c r="J124" s="2">
         <v>0</v>
       </c>
-      <c r="K124" s="2">
+      <c r="K124" s="1">
         <v>0</v>
       </c>
       <c r="L124" s="2">
@@ -20617,7 +20617,7 @@
         <v>0</v>
       </c>
       <c r="N124" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O124" s="9">
         <v>1</v>
@@ -20657,7 +20657,7 @@
       <c r="J125" s="2">
         <v>0</v>
       </c>
-      <c r="K125" s="2">
+      <c r="K125" s="1">
         <v>0</v>
       </c>
       <c r="L125" s="2">
@@ -20707,7 +20707,7 @@
       <c r="J126" s="2">
         <v>0</v>
       </c>
-      <c r="K126" s="2">
+      <c r="K126" s="1">
         <v>0</v>
       </c>
       <c r="L126" s="2">
@@ -20757,7 +20757,7 @@
       <c r="J127" s="2">
         <v>0</v>
       </c>
-      <c r="K127" s="2">
+      <c r="K127" s="1">
         <v>0</v>
       </c>
       <c r="L127" s="2">
@@ -20807,7 +20807,7 @@
       <c r="J128" s="2">
         <v>0</v>
       </c>
-      <c r="K128" s="2">
+      <c r="K128" s="1">
         <v>0</v>
       </c>
       <c r="L128" s="2">
@@ -20857,7 +20857,7 @@
       <c r="J129" s="2">
         <v>0</v>
       </c>
-      <c r="K129" s="2">
+      <c r="K129" s="1">
         <v>0</v>
       </c>
       <c r="L129" s="2">
@@ -20907,7 +20907,7 @@
       <c r="J130" s="2">
         <v>0</v>
       </c>
-      <c r="K130" s="2">
+      <c r="K130" s="1">
         <v>0</v>
       </c>
       <c r="L130" s="2">
@@ -20957,7 +20957,7 @@
       <c r="J131" s="2">
         <v>0</v>
       </c>
-      <c r="K131" s="2">
+      <c r="K131" s="1">
         <v>0</v>
       </c>
       <c r="L131" s="2">
@@ -20967,7 +20967,7 @@
         <v>0</v>
       </c>
       <c r="N131" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O131" s="9">
         <v>1</v>
@@ -21007,7 +21007,7 @@
       <c r="J132" s="2">
         <v>0</v>
       </c>
-      <c r="K132" s="2">
+      <c r="K132" s="1">
         <v>0</v>
       </c>
       <c r="L132" s="2" t="s">
@@ -21017,7 +21017,7 @@
         <v>0</v>
       </c>
       <c r="N132" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="O132" s="9">
         <v>1</v>
@@ -21057,7 +21057,7 @@
       <c r="J133" s="2">
         <v>0</v>
       </c>
-      <c r="K133" s="2">
+      <c r="K133" s="1">
         <v>0</v>
       </c>
       <c r="L133" s="2">
@@ -21067,7 +21067,7 @@
         <v>0</v>
       </c>
       <c r="N133" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O133" s="9">
         <v>1</v>
@@ -21107,7 +21107,7 @@
       <c r="J134" s="2">
         <v>0</v>
       </c>
-      <c r="K134" s="2">
+      <c r="K134" s="1">
         <v>0</v>
       </c>
       <c r="L134" s="2">
@@ -21157,7 +21157,7 @@
       <c r="J135" s="2">
         <v>0</v>
       </c>
-      <c r="K135" s="2">
+      <c r="K135" s="1">
         <v>0</v>
       </c>
       <c r="L135" s="2">
@@ -21207,7 +21207,7 @@
       <c r="J136" s="2">
         <v>0</v>
       </c>
-      <c r="K136" s="2">
+      <c r="K136" s="1">
         <v>0</v>
       </c>
       <c r="L136" s="2">
@@ -21257,7 +21257,7 @@
       <c r="J137" s="2">
         <v>0</v>
       </c>
-      <c r="K137" s="2">
+      <c r="K137" s="1">
         <v>0</v>
       </c>
       <c r="L137" s="2">
@@ -21307,7 +21307,7 @@
       <c r="J138" s="2">
         <v>0</v>
       </c>
-      <c r="K138" s="2">
+      <c r="K138" s="1">
         <v>0</v>
       </c>
       <c r="L138" s="2">
@@ -21357,7 +21357,7 @@
       <c r="J139" s="2">
         <v>0</v>
       </c>
-      <c r="K139" s="2">
+      <c r="K139" s="1">
         <v>0</v>
       </c>
       <c r="L139" s="2">
@@ -21407,7 +21407,7 @@
       <c r="J140" s="2">
         <v>0</v>
       </c>
-      <c r="K140" s="2">
+      <c r="K140" s="1">
         <v>0</v>
       </c>
       <c r="L140" s="2">
@@ -21417,7 +21417,7 @@
         <v>0</v>
       </c>
       <c r="N140" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O140" s="9">
         <v>1</v>
@@ -21457,7 +21457,7 @@
       <c r="J141" s="2">
         <v>0</v>
       </c>
-      <c r="K141" s="2">
+      <c r="K141" s="1">
         <v>0</v>
       </c>
       <c r="L141" s="2" t="s">
@@ -21467,7 +21467,7 @@
         <v>0</v>
       </c>
       <c r="N141" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="O141" s="9">
         <v>1</v>
@@ -21507,7 +21507,7 @@
       <c r="J142" s="2">
         <v>0</v>
       </c>
-      <c r="K142" s="2">
+      <c r="K142" s="1">
         <v>0</v>
       </c>
       <c r="L142" s="2">
@@ -21517,7 +21517,7 @@
         <v>0</v>
       </c>
       <c r="N142" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O142" s="9">
         <v>1</v>
@@ -21557,7 +21557,7 @@
       <c r="J143" s="2">
         <v>0</v>
       </c>
-      <c r="K143" s="2">
+      <c r="K143" s="1">
         <v>0</v>
       </c>
       <c r="L143" s="2">
@@ -21607,7 +21607,7 @@
       <c r="J144" s="2">
         <v>0</v>
       </c>
-      <c r="K144" s="2">
+      <c r="K144" s="1">
         <v>0</v>
       </c>
       <c r="L144" s="2">
@@ -21657,7 +21657,7 @@
       <c r="J145" s="2">
         <v>0</v>
       </c>
-      <c r="K145" s="2">
+      <c r="K145" s="1">
         <v>0</v>
       </c>
       <c r="L145" s="2">
@@ -21707,7 +21707,7 @@
       <c r="J146" s="2">
         <v>0</v>
       </c>
-      <c r="K146" s="2">
+      <c r="K146" s="1">
         <v>0</v>
       </c>
       <c r="L146" s="2">
@@ -21757,7 +21757,7 @@
       <c r="J147" s="2">
         <v>0</v>
       </c>
-      <c r="K147" s="2">
+      <c r="K147" s="1">
         <v>0</v>
       </c>
       <c r="L147" s="2">
@@ -21807,7 +21807,7 @@
       <c r="J148" s="2">
         <v>0</v>
       </c>
-      <c r="K148" s="2">
+      <c r="K148" s="1">
         <v>0</v>
       </c>
       <c r="L148" s="2">
@@ -21857,7 +21857,7 @@
       <c r="J149" s="2">
         <v>0</v>
       </c>
-      <c r="K149" s="2">
+      <c r="K149" s="1">
         <v>0</v>
       </c>
       <c r="L149" s="2">
@@ -21905,9 +21905,9 @@
         <v>1</v>
       </c>
       <c r="J150" s="2">
-        <v>0</v>
-      </c>
-      <c r="K150" s="2">
+        <v>1</v>
+      </c>
+      <c r="K150" s="1">
         <v>0</v>
       </c>
       <c r="L150" s="2">
@@ -21957,7 +21957,7 @@
       <c r="J151" s="2">
         <v>0</v>
       </c>
-      <c r="K151" s="2">
+      <c r="K151" s="1">
         <v>0</v>
       </c>
       <c r="L151" s="2">
@@ -22005,9 +22005,9 @@
         <v>1</v>
       </c>
       <c r="J152" s="2">
-        <v>0</v>
-      </c>
-      <c r="K152" s="2">
+        <v>1</v>
+      </c>
+      <c r="K152" s="1">
         <v>0</v>
       </c>
       <c r="L152" s="2">

</xml_diff>

<commit_message>
added red line lights and directionality on dynamic screen mouseover
</commit_message>
<xml_diff>
--- a/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
+++ b/TrainSystem/src/Modules/TrackModel/Track Layout/RedGreenLinesTrackLayout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="0" windowWidth="16170" windowHeight="7965"/>
+    <workbookView xWindow="8685" yWindow="0" windowWidth="16170" windowHeight="7965" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="1" r:id="rId1"/>
@@ -1509,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:P154"/>
     </sheetView>
@@ -9240,9 +9240,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N83" sqref="N83"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:P79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9386,7 +9386,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2">
         <v>0</v>
@@ -9786,7 +9786,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
@@ -9836,7 +9836,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
@@ -10086,7 +10086,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2">
         <v>0</v>
@@ -10136,7 +10136,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="2">
         <v>0</v>
@@ -10686,7 +10686,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2">
         <v>0</v>
@@ -10736,7 +10736,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="2">
         <v>0</v>
@@ -10886,7 +10886,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
@@ -10936,7 +10936,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="2">
         <v>0</v>
@@ -11236,7 +11236,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="2">
         <v>0</v>
@@ -11286,7 +11286,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="2">
         <v>0</v>
@@ -11436,7 +11436,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="2">
         <v>0</v>
@@ -11486,7 +11486,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="2">
         <v>0</v>
@@ -11936,7 +11936,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" s="2">
         <v>0</v>
@@ -11986,7 +11986,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" s="2">
         <v>0</v>
@@ -12636,7 +12636,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68" s="2">
         <v>0</v>
@@ -12686,7 +12686,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K69" s="2">
         <v>0</v>
@@ -12886,7 +12886,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K73" s="2">
         <v>0</v>
@@ -12936,7 +12936,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K74" s="2">
         <v>0</v>
@@ -13136,7 +13136,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" s="2">
         <v>0</v>
@@ -13186,7 +13186,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K79" s="2">
         <v>0</v>
@@ -22035,8 +22035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22074,7 +22074,7 @@
         <v>0</v>
       </c>
       <c r="J1" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K1" s="2">
         <v>0</v>
@@ -22086,7 +22086,7 @@
         <v>88</v>
       </c>
       <c r="N1" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O1" s="2">
         <v>0</v>
@@ -22336,7 +22336,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
@@ -22389,7 +22389,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="P7" s="12" t="s">
         <v>299</v>
@@ -22436,7 +22436,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -22474,7 +22474,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -22524,7 +22524,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
@@ -22774,7 +22774,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
@@ -22786,7 +22786,7 @@
         <v>86</v>
       </c>
       <c r="N15" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O15" s="2">
         <v>0</v>
@@ -22824,7 +22824,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="2">
         <v>0</v>
@@ -22839,7 +22839,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="P16" s="12" t="s">
         <v>108</v>
@@ -22886,7 +22886,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O17" s="2">
         <v>0</v>
@@ -23036,7 +23036,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O20" s="2">
         <v>0</v>
@@ -23089,7 +23089,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P21" s="12" t="s">
         <v>308</v>
@@ -23136,7 +23136,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O22" s="2">
         <v>0</v>
@@ -23236,7 +23236,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O24" s="2">
         <v>1</v>
@@ -23289,7 +23289,7 @@
         <v>0</v>
       </c>
       <c r="O25" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="P25" s="12" t="s">
         <v>114</v>
@@ -23336,7 +23336,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O26" s="2">
         <v>1</v>
@@ -23374,7 +23374,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
         <v>0</v>
@@ -23424,7 +23424,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
@@ -23574,7 +23574,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="2">
         <v>0</v>
@@ -23624,7 +23624,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
@@ -23736,7 +23736,7 @@
         <v>0</v>
       </c>
       <c r="N34" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O34" s="2">
         <v>1</v>
@@ -23789,7 +23789,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="P35" s="12" t="s">
         <v>124</v>
@@ -23836,7 +23836,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O36" s="2">
         <v>1</v>
@@ -23924,7 +23924,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="2">
         <v>0</v>
@@ -23974,7 +23974,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="2">
         <v>0</v>
@@ -24124,7 +24124,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="2">
         <v>0</v>
@@ -24174,7 +24174,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
@@ -24236,7 +24236,7 @@
         <v>0</v>
       </c>
       <c r="N44" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O44" s="2">
         <v>1</v>
@@ -24289,7 +24289,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="2">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="P45" s="12" t="s">
         <v>134</v>
@@ -24336,7 +24336,7 @@
         <v>0</v>
       </c>
       <c r="N46" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="O46" s="2">
         <v>1</v>
@@ -24386,7 +24386,7 @@
         <v>0</v>
       </c>
       <c r="N47" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="O47" s="2">
         <v>0</v>
@@ -24439,7 +24439,7 @@
         <v>0</v>
       </c>
       <c r="O48" s="2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="P48" s="12" t="s">
         <v>313</v>
@@ -24486,7 +24486,7 @@
         <v>0</v>
       </c>
       <c r="N49" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="O49" s="2">
         <v>0</v>
@@ -24624,7 +24624,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="2">
         <v>0</v>
@@ -24674,7 +24674,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="2">
         <v>0</v>
@@ -24986,7 +24986,7 @@
         <v>0</v>
       </c>
       <c r="N59" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O59" s="2">
         <v>0</v>
@@ -25039,7 +25039,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P60" s="12" t="s">
         <v>325</v>
@@ -25086,7 +25086,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="O61" s="2">
         <v>0</v>
@@ -25324,7 +25324,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" s="2">
         <v>0</v>
@@ -25374,7 +25374,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K67" s="2">
         <v>0</v>
@@ -25574,7 +25574,7 @@
         <v>0</v>
       </c>
       <c r="J71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K71" s="2">
         <v>0</v>
@@ -25624,7 +25624,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72" s="2">
         <v>0</v>
@@ -25824,7 +25824,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K76" s="2">
         <v>0</v>
@@ -25874,7 +25874,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K77" s="2">
         <v>0</v>

</xml_diff>